<commit_message>
no longer printing to terminal
</commit_message>
<xml_diff>
--- a/filtered_excel_df.xlsx
+++ b/filtered_excel_df.xlsx
@@ -704,10 +704,10 @@
         <v>1</v>
       </c>
       <c r="AF2" t="n">
-        <v>108.23</v>
+        <v>216.78</v>
       </c>
       <c r="AG2" t="n">
-        <v>408.23</v>
+        <v>816.78</v>
       </c>
       <c r="AH2" t="n">
         <v>1</v>
@@ -811,10 +811,10 @@
         <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>-171.97</v>
+        <v>-344.36</v>
       </c>
       <c r="AG3" t="n">
-        <v>236.26</v>
+        <v>472.42</v>
       </c>
       <c r="AH3" t="n">
         <v>0</v>
@@ -918,10 +918,10 @@
         <v>1</v>
       </c>
       <c r="AF4" t="n">
-        <v>108.24</v>
+        <v>216.78</v>
       </c>
       <c r="AG4" t="n">
-        <v>344.5</v>
+        <v>689.1999999999999</v>
       </c>
       <c r="AH4" t="n">
         <v>1</v>
@@ -1025,10 +1025,10 @@
         <v>1</v>
       </c>
       <c r="AF5" t="n">
-        <v>108.24</v>
+        <v>216.78</v>
       </c>
       <c r="AG5" t="n">
-        <v>452.74</v>
+        <v>905.9799999999999</v>
       </c>
       <c r="AH5" t="n">
         <v>2</v>
@@ -1132,10 +1132,10 @@
         <v>0</v>
       </c>
       <c r="AF6" t="n">
-        <v>-75.25</v>
+        <v>-150.68</v>
       </c>
       <c r="AG6" t="n">
-        <v>377.49</v>
+        <v>755.3</v>
       </c>
       <c r="AH6" t="n">
         <v>0</v>
@@ -1241,10 +1241,10 @@
         <v>1</v>
       </c>
       <c r="AF7" t="n">
-        <v>108.24</v>
+        <v>216.78</v>
       </c>
       <c r="AG7" t="n">
-        <v>485.73</v>
+        <v>972.0799999999999</v>
       </c>
       <c r="AH7" t="n">
         <v>1</v>
@@ -1348,10 +1348,10 @@
         <v>1</v>
       </c>
       <c r="AF8" t="n">
-        <v>108.24</v>
+        <v>216.78</v>
       </c>
       <c r="AG8" t="n">
-        <v>593.97</v>
+        <v>1188.86</v>
       </c>
       <c r="AH8" t="n">
         <v>2</v>
@@ -1455,10 +1455,10 @@
         <v>0</v>
       </c>
       <c r="AF9" t="n">
-        <v>-97.98999999999999</v>
+        <v>-196.21</v>
       </c>
       <c r="AG9" t="n">
-        <v>495.98</v>
+        <v>992.6499999999999</v>
       </c>
       <c r="AH9" t="n">
         <v>0</v>
@@ -1562,10 +1562,10 @@
         <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>-44.03</v>
+        <v>-88.17</v>
       </c>
       <c r="AG10" t="n">
-        <v>451.95</v>
+        <v>904.4799999999999</v>
       </c>
       <c r="AH10" t="n">
         <v>0</v>
@@ -1671,10 +1671,10 @@
         <v>1</v>
       </c>
       <c r="AF11" t="n">
-        <v>108.25</v>
+        <v>216.77</v>
       </c>
       <c r="AG11" t="n">
-        <v>560.2</v>
+        <v>1121.25</v>
       </c>
       <c r="AH11" t="n">
         <v>1</v>
@@ -1780,10 +1780,10 @@
         <v>1</v>
       </c>
       <c r="AF12" t="n">
-        <v>108.24</v>
+        <v>216.76</v>
       </c>
       <c r="AG12" t="n">
-        <v>668.4400000000001</v>
+        <v>1338.01</v>
       </c>
       <c r="AH12" t="n">
         <v>2</v>
@@ -1887,10 +1887,10 @@
         <v>1</v>
       </c>
       <c r="AF13" t="n">
-        <v>108.25</v>
+        <v>216.76</v>
       </c>
       <c r="AG13" t="n">
-        <v>776.6900000000001</v>
+        <v>1554.77</v>
       </c>
       <c r="AH13" t="n">
         <v>3</v>
@@ -1996,10 +1996,10 @@
         <v>1</v>
       </c>
       <c r="AF14" t="n">
-        <v>108.26</v>
+        <v>216.76</v>
       </c>
       <c r="AG14" t="n">
-        <v>884.95</v>
+        <v>1771.53</v>
       </c>
       <c r="AH14" t="n">
         <v>4</v>
@@ -2103,10 +2103,10 @@
         <v>1</v>
       </c>
       <c r="AF15" t="n">
-        <v>108.26</v>
+        <v>216.75</v>
       </c>
       <c r="AG15" t="n">
-        <v>993.21</v>
+        <v>1988.28</v>
       </c>
       <c r="AH15" t="n">
         <v>5</v>
@@ -2212,10 +2212,10 @@
         <v>1</v>
       </c>
       <c r="AF16" t="n">
-        <v>54.13</v>
+        <v>108.38</v>
       </c>
       <c r="AG16" t="n">
-        <v>1047.34</v>
+        <v>2096.66</v>
       </c>
       <c r="AH16" t="n">
         <v>6</v>
@@ -2319,10 +2319,10 @@
         <v>1</v>
       </c>
       <c r="AF17" t="n">
-        <v>108.26</v>
+        <v>216.76</v>
       </c>
       <c r="AG17" t="n">
-        <v>1155.6</v>
+        <v>2313.42</v>
       </c>
       <c r="AH17" t="n">
         <v>7</v>
@@ -2428,10 +2428,10 @@
         <v>1</v>
       </c>
       <c r="AF18" t="n">
-        <v>54.13</v>
+        <v>108.38</v>
       </c>
       <c r="AG18" t="n">
-        <v>1209.73</v>
+        <v>2421.8</v>
       </c>
       <c r="AH18" t="n">
         <v>8</v>
@@ -2535,10 +2535,10 @@
         <v>0</v>
       </c>
       <c r="AF19" t="n">
-        <v>-107.57</v>
+        <v>-215.36</v>
       </c>
       <c r="AG19" t="n">
-        <v>1102.16</v>
+        <v>2206.44</v>
       </c>
       <c r="AH19" t="n">
         <v>0</v>
@@ -2642,10 +2642,10 @@
         <v>0</v>
       </c>
       <c r="AF20" t="n">
-        <v>-54.69</v>
+        <v>-109.49</v>
       </c>
       <c r="AG20" t="n">
-        <v>1047.47</v>
+        <v>2096.95</v>
       </c>
       <c r="AH20" t="n">
         <v>0</v>
@@ -2749,10 +2749,10 @@
         <v>0</v>
       </c>
       <c r="AF21" t="n">
-        <v>-51.08</v>
+        <v>-102.26</v>
       </c>
       <c r="AG21" t="n">
-        <v>996.3900000000002</v>
+        <v>1994.69</v>
       </c>
       <c r="AH21" t="n">
         <v>0</v>
@@ -2856,10 +2856,10 @@
         <v>1</v>
       </c>
       <c r="AF22" t="n">
-        <v>-68.22</v>
+        <v>-136.59</v>
       </c>
       <c r="AG22" t="n">
-        <v>928.1700000000002</v>
+        <v>1858.1</v>
       </c>
       <c r="AH22" t="n">
         <v>1</v>
@@ -2963,10 +2963,10 @@
         <v>0</v>
       </c>
       <c r="AF23" t="n">
-        <v>-67.5</v>
+        <v>-135.14</v>
       </c>
       <c r="AG23" t="n">
-        <v>860.6700000000002</v>
+        <v>1722.96</v>
       </c>
       <c r="AH23" t="n">
         <v>0</v>
@@ -3070,10 +3070,10 @@
         <v>0</v>
       </c>
       <c r="AF24" t="n">
-        <v>-132.84</v>
+        <v>-265.95</v>
       </c>
       <c r="AG24" t="n">
-        <v>727.8300000000002</v>
+        <v>1457.01</v>
       </c>
       <c r="AH24" t="n">
         <v>0</v>
@@ -3177,10 +3177,10 @@
         <v>1</v>
       </c>
       <c r="AF25" t="n">
-        <v>108.25</v>
+        <v>216.76</v>
       </c>
       <c r="AG25" t="n">
-        <v>836.0800000000002</v>
+        <v>1673.77</v>
       </c>
       <c r="AH25" t="n">
         <v>1</v>
@@ -3284,10 +3284,10 @@
         <v>1</v>
       </c>
       <c r="AF26" t="n">
-        <v>108.25</v>
+        <v>216.77</v>
       </c>
       <c r="AG26" t="n">
-        <v>944.3300000000002</v>
+        <v>1890.54</v>
       </c>
       <c r="AH26" t="n">
         <v>2</v>
@@ -3391,10 +3391,10 @@
         <v>0</v>
       </c>
       <c r="AF27" t="n">
-        <v>-132.29</v>
+        <v>-264.87</v>
       </c>
       <c r="AG27" t="n">
-        <v>812.0400000000002</v>
+        <v>1625.670000000001</v>
       </c>
       <c r="AH27" t="n">
         <v>0</v>
@@ -3498,10 +3498,10 @@
         <v>0</v>
       </c>
       <c r="AF28" t="n">
-        <v>-115.69</v>
+        <v>-231.62</v>
       </c>
       <c r="AG28" t="n">
-        <v>696.3500000000001</v>
+        <v>1394.050000000001</v>
       </c>
       <c r="AH28" t="n">
         <v>0</v>
@@ -3607,10 +3607,10 @@
         <v>1</v>
       </c>
       <c r="AF29" t="n">
-        <v>108.26</v>
+        <v>216.76</v>
       </c>
       <c r="AG29" t="n">
-        <v>804.6100000000001</v>
+        <v>1610.810000000001</v>
       </c>
       <c r="AH29" t="n">
         <v>1</v>
@@ -3714,10 +3714,10 @@
         <v>1</v>
       </c>
       <c r="AF30" t="n">
-        <v>108.26</v>
+        <v>216.76</v>
       </c>
       <c r="AG30" t="n">
-        <v>912.8700000000001</v>
+        <v>1827.570000000001</v>
       </c>
       <c r="AH30" t="n">
         <v>2</v>
@@ -3823,10 +3823,10 @@
         <v>1</v>
       </c>
       <c r="AF31" t="n">
-        <v>108.26</v>
+        <v>216.76</v>
       </c>
       <c r="AG31" t="n">
-        <v>1021.13</v>
+        <v>2044.330000000001</v>
       </c>
       <c r="AH31" t="n">
         <v>3</v>
@@ -3932,10 +3932,10 @@
         <v>1</v>
       </c>
       <c r="AF32" t="n">
-        <v>54.13</v>
+        <v>108.38</v>
       </c>
       <c r="AG32" t="n">
-        <v>1075.26</v>
+        <v>2152.71</v>
       </c>
       <c r="AH32" t="n">
         <v>4</v>
@@ -4039,10 +4039,10 @@
         <v>0</v>
       </c>
       <c r="AF33" t="n">
-        <v>-42.6</v>
+        <v>-85.28</v>
       </c>
       <c r="AG33" t="n">
-        <v>1032.66</v>
+        <v>2067.43</v>
       </c>
       <c r="AH33" t="n">
         <v>0</v>
@@ -4148,10 +4148,10 @@
         <v>1</v>
       </c>
       <c r="AF34" t="n">
-        <v>108.26</v>
+        <v>216.76</v>
       </c>
       <c r="AG34" t="n">
-        <v>1140.92</v>
+        <v>2284.190000000001</v>
       </c>
       <c r="AH34" t="n">
         <v>1</v>
@@ -4257,10 +4257,10 @@
         <v>1</v>
       </c>
       <c r="AF35" t="n">
-        <v>108.26</v>
+        <v>216.76</v>
       </c>
       <c r="AG35" t="n">
-        <v>1249.18</v>
+        <v>2500.950000000001</v>
       </c>
       <c r="AH35" t="n">
         <v>2</v>
@@ -4364,10 +4364,10 @@
         <v>0</v>
       </c>
       <c r="AF36" t="n">
-        <v>-64.62</v>
+        <v>-129.36</v>
       </c>
       <c r="AG36" t="n">
-        <v>1184.56</v>
+        <v>2371.590000000001</v>
       </c>
       <c r="AH36" t="n">
         <v>0</v>
@@ -4473,10 +4473,10 @@
         <v>1</v>
       </c>
       <c r="AF37" t="n">
-        <v>54.12</v>
+        <v>108.38</v>
       </c>
       <c r="AG37" t="n">
-        <v>1238.68</v>
+        <v>2479.970000000001</v>
       </c>
       <c r="AH37" t="n">
         <v>1</v>
@@ -4580,10 +4580,10 @@
         <v>1</v>
       </c>
       <c r="AF38" t="n">
-        <v>108.25</v>
+        <v>216.76</v>
       </c>
       <c r="AG38" t="n">
-        <v>1346.93</v>
+        <v>2696.73</v>
       </c>
       <c r="AH38" t="n">
         <v>2</v>
@@ -4689,10 +4689,10 @@
         <v>1</v>
       </c>
       <c r="AF39" t="n">
-        <v>108.25</v>
+        <v>216.76</v>
       </c>
       <c r="AG39" t="n">
-        <v>1455.18</v>
+        <v>2913.490000000001</v>
       </c>
       <c r="AH39" t="n">
         <v>3</v>
@@ -4796,10 +4796,10 @@
         <v>1</v>
       </c>
       <c r="AF40" t="n">
-        <v>108.25</v>
+        <v>216.76</v>
       </c>
       <c r="AG40" t="n">
-        <v>1563.43</v>
+        <v>3130.250000000001</v>
       </c>
       <c r="AH40" t="n">
         <v>4</v>
@@ -4903,10 +4903,10 @@
         <v>1</v>
       </c>
       <c r="AF41" t="n">
-        <v>108.25</v>
+        <v>216.76</v>
       </c>
       <c r="AG41" t="n">
-        <v>1671.68</v>
+        <v>3347.010000000001</v>
       </c>
       <c r="AH41" t="n">
         <v>5</v>
@@ -5012,10 +5012,10 @@
         <v>1</v>
       </c>
       <c r="AF42" t="n">
-        <v>54.13</v>
+        <v>108.38</v>
       </c>
       <c r="AG42" t="n">
-        <v>1725.81</v>
+        <v>3455.390000000001</v>
       </c>
       <c r="AH42" t="n">
         <v>6</v>
@@ -5121,10 +5121,10 @@
         <v>1</v>
       </c>
       <c r="AF43" t="n">
-        <v>108.26</v>
+        <v>216.76</v>
       </c>
       <c r="AG43" t="n">
-        <v>1834.07</v>
+        <v>3672.150000000001</v>
       </c>
       <c r="AH43" t="n">
         <v>7</v>
@@ -5230,10 +5230,10 @@
         <v>1</v>
       </c>
       <c r="AF44" t="n">
-        <v>54.13</v>
+        <v>108.38</v>
       </c>
       <c r="AG44" t="n">
-        <v>1888.200000000001</v>
+        <v>3780.530000000002</v>
       </c>
       <c r="AH44" t="n">
         <v>8</v>
@@ -5337,10 +5337,10 @@
         <v>0</v>
       </c>
       <c r="AF45" t="n">
-        <v>-64.79000000000001</v>
+        <v>-129.72</v>
       </c>
       <c r="AG45" t="n">
-        <v>1823.410000000001</v>
+        <v>3650.810000000002</v>
       </c>
       <c r="AH45" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
updated trailing stop loss
</commit_message>
<xml_diff>
--- a/filtered_excel_df.xlsx
+++ b/filtered_excel_df.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI34"/>
+  <dimension ref="A1:AI35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -677,10 +677,10 @@
         <v>2291.29</v>
       </c>
       <c r="W2" t="n">
-        <v>2297.12</v>
+        <v>2296.12</v>
       </c>
       <c r="X2" t="n">
-        <v>2298.12</v>
+        <v>2296.82</v>
       </c>
       <c r="Y2" t="b">
         <v>0</v>
@@ -704,10 +704,10 @@
         <v>1</v>
       </c>
       <c r="AF2" t="n">
-        <v>125.81</v>
+        <v>125.34</v>
       </c>
       <c r="AG2" t="n">
-        <v>425.81</v>
+        <v>425.34</v>
       </c>
       <c r="AH2" t="n">
         <v>1</v>
@@ -784,10 +784,10 @@
         <v>2311.07</v>
       </c>
       <c r="W3" t="n">
-        <v>2303.9</v>
+        <v>2304.9</v>
       </c>
       <c r="X3" t="n">
-        <v>2302.9</v>
+        <v>2304.2</v>
       </c>
       <c r="Y3" t="b">
         <v>0</v>
@@ -811,10 +811,10 @@
         <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>-74.97</v>
+        <v>-74.69</v>
       </c>
       <c r="AG3" t="n">
-        <v>350.84</v>
+        <v>350.65</v>
       </c>
       <c r="AH3" t="n">
         <v>0</v>
@@ -888,28 +888,28 @@
         <v>2315.58</v>
       </c>
       <c r="V4" t="n">
-        <v>2319.58</v>
+        <v>2320.58</v>
       </c>
       <c r="W4" t="n">
-        <v>2319.58</v>
+        <v>2320.58</v>
       </c>
       <c r="X4" t="n">
-        <v>2318.58</v>
+        <v>2319.88</v>
       </c>
       <c r="Y4" t="b">
         <v>1</v>
       </c>
       <c r="Z4" s="2" t="n">
-        <v>45418.5</v>
+        <v>45418.48958333334</v>
       </c>
       <c r="AA4" s="2" t="n">
-        <v>45418.5</v>
+        <v>45418.48958333334</v>
       </c>
       <c r="AB4" s="2" t="n">
         <v>45418.51630787037</v>
       </c>
       <c r="AC4" s="2" t="n">
-        <v>45418.53233796296</v>
+        <v>45418.53309027778</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
@@ -920,10 +920,10 @@
         <v>1</v>
       </c>
       <c r="AF4" t="n">
-        <v>125.81</v>
+        <v>125.34</v>
       </c>
       <c r="AG4" t="n">
-        <v>476.65</v>
+        <v>475.99</v>
       </c>
       <c r="AH4" t="n">
         <v>1</v>
@@ -997,40 +997,42 @@
         <v>2320.83</v>
       </c>
       <c r="V5" t="n">
-        <v>2332.07</v>
+        <v>2325.83</v>
       </c>
       <c r="W5" t="n">
-        <v>2324.83</v>
+        <v>2325.83</v>
       </c>
       <c r="X5" t="n">
-        <v>2323.83</v>
+        <v>2325.13</v>
       </c>
       <c r="Y5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <v>45418.72916666666</v>
+      </c>
       <c r="AA5" s="2" t="n">
-        <v>45418.73958333334</v>
+        <v>45418.72916666666</v>
       </c>
       <c r="AB5" s="2" t="n">
         <v>45418.73547453704</v>
       </c>
       <c r="AC5" s="2" t="n">
-        <v>45421.71508101852</v>
+        <v>45418.72989583333</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AE5" t="b">
         <v>1</v>
       </c>
       <c r="AF5" t="n">
-        <v>125.81</v>
+        <v>35.81</v>
       </c>
       <c r="AG5" t="n">
-        <v>602.46</v>
+        <v>511.8</v>
       </c>
       <c r="AH5" t="n">
         <v>2</v>
@@ -1107,10 +1109,10 @@
         <v>2317.6</v>
       </c>
       <c r="W6" t="n">
-        <v>2326.03</v>
+        <v>2325.03</v>
       </c>
       <c r="X6" t="n">
-        <v>2327.03</v>
+        <v>2325.73</v>
       </c>
       <c r="Y6" t="b">
         <v>0</v>
@@ -1134,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="AF6" t="n">
-        <v>-97.62</v>
+        <v>-97.23999999999999</v>
       </c>
       <c r="AG6" t="n">
-        <v>504.84</v>
+        <v>414.56</v>
       </c>
       <c r="AH6" t="n">
         <v>0</v>
@@ -1214,17 +1216,17 @@
         <v>2312.12</v>
       </c>
       <c r="W7" t="n">
-        <v>2319.48</v>
+        <v>2318.48</v>
       </c>
       <c r="X7" t="n">
-        <v>2320.48</v>
+        <v>2319.18</v>
       </c>
       <c r="Y7" t="b">
         <v>0</v>
       </c>
       <c r="Z7" t="inlineStr"/>
       <c r="AA7" s="2" t="n">
-        <v>45421.65625</v>
+        <v>45420.33333333334</v>
       </c>
       <c r="AB7" s="2" t="n">
         <v>45421.64862268518</v>
@@ -1241,10 +1243,10 @@
         <v>0</v>
       </c>
       <c r="AF7" t="n">
-        <v>-78.38</v>
+        <v>-78.08</v>
       </c>
       <c r="AG7" t="n">
-        <v>426.46</v>
+        <v>336.48</v>
       </c>
       <c r="AH7" t="n">
         <v>0</v>
@@ -1321,17 +1323,17 @@
         <v>2311.71</v>
       </c>
       <c r="W8" t="n">
-        <v>2317.15</v>
+        <v>2316.15</v>
       </c>
       <c r="X8" t="n">
-        <v>2318.15</v>
+        <v>2316.85</v>
       </c>
       <c r="Y8" t="b">
         <v>0</v>
       </c>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" s="2" t="n">
-        <v>45420.30208333334</v>
+        <v>45420.25</v>
       </c>
       <c r="AB8" s="2" t="n">
         <v>45420.35515046296</v>
@@ -1348,10 +1350,10 @@
         <v>0</v>
       </c>
       <c r="AF8" t="n">
-        <v>-43.87</v>
+        <v>-43.7</v>
       </c>
       <c r="AG8" t="n">
-        <v>382.59</v>
+        <v>292.78</v>
       </c>
       <c r="AH8" t="n">
         <v>0</v>
@@ -1425,13 +1427,13 @@
         <v>2315.84</v>
       </c>
       <c r="V9" t="n">
-        <v>2311.84</v>
+        <v>2310.84</v>
       </c>
       <c r="W9" t="n">
-        <v>2311.84</v>
+        <v>2310.84</v>
       </c>
       <c r="X9" t="n">
-        <v>2312.84</v>
+        <v>2311.54</v>
       </c>
       <c r="Y9" t="b">
         <v>1</v>
@@ -1446,7 +1448,7 @@
         <v>45420.24600694444</v>
       </c>
       <c r="AC9" s="2" t="n">
-        <v>45420.43472222222</v>
+        <v>45420.44150462963</v>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
@@ -1457,10 +1459,10 @@
         <v>1</v>
       </c>
       <c r="AF9" t="n">
-        <v>125.81</v>
+        <v>125.31</v>
       </c>
       <c r="AG9" t="n">
-        <v>508.4</v>
+        <v>418.09</v>
       </c>
       <c r="AH9" t="n">
         <v>1</v>
@@ -1534,13 +1536,13 @@
         <v>2313.53</v>
       </c>
       <c r="V10" t="n">
-        <v>2309.53</v>
+        <v>2308.53</v>
       </c>
       <c r="W10" t="n">
-        <v>2309.53</v>
+        <v>2308.53</v>
       </c>
       <c r="X10" t="n">
-        <v>2310.53</v>
+        <v>2309.23</v>
       </c>
       <c r="Y10" t="b">
         <v>1</v>
@@ -1566,10 +1568,10 @@
         <v>1</v>
       </c>
       <c r="AF10" t="n">
-        <v>125.81</v>
+        <v>125.31</v>
       </c>
       <c r="AG10" t="n">
-        <v>634.21</v>
+        <v>543.4000000000001</v>
       </c>
       <c r="AH10" t="n">
         <v>2</v>
@@ -1643,42 +1645,42 @@
         <v>2316.29</v>
       </c>
       <c r="V11" t="n">
-        <v>2312.29</v>
+        <v>2311.29</v>
       </c>
       <c r="W11" t="n">
-        <v>2312.29</v>
+        <v>2311.29</v>
       </c>
       <c r="X11" t="n">
-        <v>2313.29</v>
+        <v>2311.99</v>
       </c>
       <c r="Y11" t="b">
         <v>1</v>
       </c>
       <c r="Z11" s="2" t="n">
-        <v>45421.61458333334</v>
+        <v>45421.48958333334</v>
       </c>
       <c r="AA11" s="2" t="n">
-        <v>45421.61458333334</v>
+        <v>45421.48958333334</v>
       </c>
       <c r="AB11" s="2" t="n">
         <v>45421.61857638889</v>
       </c>
       <c r="AC11" s="2" t="n">
-        <v>45421.6750925926</v>
+        <v>45421.49377314815</v>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AE11" t="b">
         <v>1</v>
       </c>
       <c r="AF11" t="n">
-        <v>125.81</v>
+        <v>35.8</v>
       </c>
       <c r="AG11" t="n">
-        <v>760.02</v>
+        <v>579.2</v>
       </c>
       <c r="AH11" t="n">
         <v>3</v>
@@ -1755,10 +1757,10 @@
         <v>2331.24</v>
       </c>
       <c r="W12" t="n">
-        <v>2323.61</v>
+        <v>2324.61</v>
       </c>
       <c r="X12" t="n">
-        <v>2322.61</v>
+        <v>2323.91</v>
       </c>
       <c r="Y12" t="b">
         <v>0</v>
@@ -1782,10 +1784,10 @@
         <v>1</v>
       </c>
       <c r="AF12" t="n">
-        <v>125.81</v>
+        <v>125.32</v>
       </c>
       <c r="AG12" t="n">
-        <v>885.8299999999999</v>
+        <v>704.52</v>
       </c>
       <c r="AH12" t="n">
         <v>4</v>
@@ -1859,28 +1861,28 @@
         <v>2342.88</v>
       </c>
       <c r="V13" t="n">
-        <v>2338.88</v>
+        <v>2337.88</v>
       </c>
       <c r="W13" t="n">
-        <v>2338.88</v>
+        <v>2337.88</v>
       </c>
       <c r="X13" t="n">
-        <v>2339.88</v>
+        <v>2338.58</v>
       </c>
       <c r="Y13" t="b">
         <v>1</v>
       </c>
       <c r="Z13" s="2" t="n">
-        <v>45426.17708333334</v>
+        <v>45426.13541666666</v>
       </c>
       <c r="AA13" s="2" t="n">
-        <v>45426.17708333334</v>
+        <v>45426.13541666666</v>
       </c>
       <c r="AB13" s="2" t="n">
         <v>45426.20903935185</v>
       </c>
       <c r="AC13" s="2" t="n">
-        <v>45426.18340277778</v>
+        <v>45426.14709490741</v>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
@@ -1891,10 +1893,10 @@
         <v>1</v>
       </c>
       <c r="AF13" t="n">
-        <v>53.92</v>
+        <v>35.8</v>
       </c>
       <c r="AG13" t="n">
-        <v>939.7499999999999</v>
+        <v>740.3199999999999</v>
       </c>
       <c r="AH13" t="n">
         <v>5</v>
@@ -1968,40 +1970,42 @@
         <v>2339.58</v>
       </c>
       <c r="V14" t="n">
-        <v>2350.16</v>
+        <v>2344.58</v>
       </c>
       <c r="W14" t="n">
-        <v>2343.58</v>
+        <v>2344.58</v>
       </c>
       <c r="X14" t="n">
-        <v>2342.58</v>
+        <v>2343.88</v>
       </c>
       <c r="Y14" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="Z14" s="2" t="n">
+        <v>45426.60416666666</v>
+      </c>
       <c r="AA14" s="2" t="n">
-        <v>45435.76041666666</v>
+        <v>45426.60416666666</v>
       </c>
       <c r="AB14" s="2" t="n">
         <v>45426.64584490741</v>
       </c>
       <c r="AC14" s="2" t="n">
-        <v>45426.66172453704</v>
+        <v>45426.62665509259</v>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AE14" t="b">
         <v>1</v>
       </c>
       <c r="AF14" t="n">
-        <v>125.81</v>
+        <v>35.8</v>
       </c>
       <c r="AG14" t="n">
-        <v>1065.56</v>
+        <v>776.1199999999999</v>
       </c>
       <c r="AH14" t="n">
         <v>6</v>
@@ -2078,10 +2082,10 @@
         <v>2436.13</v>
       </c>
       <c r="W15" t="n">
-        <v>2430.1</v>
+        <v>2431.1</v>
       </c>
       <c r="X15" t="n">
-        <v>2429.1</v>
+        <v>2430.4</v>
       </c>
       <c r="Y15" t="b">
         <v>0</v>
@@ -2105,10 +2109,10 @@
         <v>0</v>
       </c>
       <c r="AF15" t="n">
-        <v>-54.47</v>
+        <v>-54.25</v>
       </c>
       <c r="AG15" t="n">
-        <v>1011.09</v>
+        <v>721.8699999999999</v>
       </c>
       <c r="AH15" t="n">
         <v>0</v>
@@ -2185,17 +2189,17 @@
         <v>2415.81</v>
       </c>
       <c r="W16" t="n">
-        <v>2421.64</v>
+        <v>2420.64</v>
       </c>
       <c r="X16" t="n">
-        <v>2422.64</v>
+        <v>2421.34</v>
       </c>
       <c r="Y16" t="b">
         <v>0</v>
       </c>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" s="2" t="n">
-        <v>45433.625</v>
+        <v>45433.44791666666</v>
       </c>
       <c r="AB16" s="2" t="n">
         <v>45433.63902777778</v>
@@ -2212,10 +2216,10 @@
         <v>0</v>
       </c>
       <c r="AF16" t="n">
-        <v>-50.88</v>
+        <v>-50.68</v>
       </c>
       <c r="AG16" t="n">
-        <v>960.2099999999999</v>
+        <v>671.1899999999999</v>
       </c>
       <c r="AH16" t="n">
         <v>0</v>
@@ -2289,40 +2293,42 @@
         <v>2412.15</v>
       </c>
       <c r="V17" t="n">
-        <v>2424.1</v>
+        <v>2417.15</v>
       </c>
       <c r="W17" t="n">
-        <v>2416.15</v>
+        <v>2417.15</v>
       </c>
       <c r="X17" t="n">
-        <v>2415.15</v>
+        <v>2416.45</v>
       </c>
       <c r="Y17" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z17" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="Z17" s="2" t="n">
+        <v>45433.47916666666</v>
+      </c>
       <c r="AA17" s="2" t="n">
-        <v>45433.53125</v>
+        <v>45433.47916666666</v>
       </c>
       <c r="AB17" s="2" t="n">
         <v>45433.52934027778</v>
       </c>
       <c r="AC17" s="2" t="n">
-        <v>45433.62893518519</v>
+        <v>45433.48001157407</v>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AE17" t="b">
         <v>1</v>
       </c>
       <c r="AF17" t="n">
-        <v>125.81</v>
+        <v>35.8</v>
       </c>
       <c r="AG17" t="n">
-        <v>1086.02</v>
+        <v>706.9899999999999</v>
       </c>
       <c r="AH17" t="n">
         <v>1</v>
@@ -2399,17 +2405,17 @@
         <v>2417.32</v>
       </c>
       <c r="W18" t="n">
-        <v>2424.04</v>
+        <v>2423.04</v>
       </c>
       <c r="X18" t="n">
-        <v>2425.04</v>
+        <v>2423.74</v>
       </c>
       <c r="Y18" t="b">
         <v>0</v>
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" s="2" t="n">
-        <v>45434.21875</v>
+        <v>45433.9375</v>
       </c>
       <c r="AB18" s="2" t="n">
         <v>132320.9911673006</v>
@@ -2426,10 +2432,10 @@
         <v>0</v>
       </c>
       <c r="AF18" t="n">
-        <v>-66.88</v>
+        <v>-66.61</v>
       </c>
       <c r="AG18" t="n">
-        <v>1019.14</v>
+        <v>640.3799999999999</v>
       </c>
       <c r="AH18" t="n">
         <v>0</v>
@@ -2506,10 +2512,10 @@
         <v>2427.79</v>
       </c>
       <c r="W19" t="n">
-        <v>2421.01</v>
+        <v>2422.01</v>
       </c>
       <c r="X19" t="n">
-        <v>2420.01</v>
+        <v>2421.31</v>
       </c>
       <c r="Y19" t="b">
         <v>0</v>
@@ -2533,10 +2539,10 @@
         <v>1</v>
       </c>
       <c r="AF19" t="n">
-        <v>-67.95999999999999</v>
+        <v>-67.68000000000001</v>
       </c>
       <c r="AG19" t="n">
-        <v>951.1799999999999</v>
+        <v>572.6999999999998</v>
       </c>
       <c r="AH19" t="n">
         <v>1</v>
@@ -2613,10 +2619,10 @@
         <v>2415.23</v>
       </c>
       <c r="W20" t="n">
-        <v>2421.97</v>
+        <v>2420.97</v>
       </c>
       <c r="X20" t="n">
-        <v>2422.97</v>
+        <v>2421.67</v>
       </c>
       <c r="Y20" t="b">
         <v>0</v>
@@ -2640,10 +2646,10 @@
         <v>0</v>
       </c>
       <c r="AF20" t="n">
-        <v>-67.23999999999999</v>
+        <v>-66.97</v>
       </c>
       <c r="AG20" t="n">
-        <v>883.9399999999999</v>
+        <v>505.7299999999998</v>
       </c>
       <c r="AH20" t="n">
         <v>0</v>
@@ -2720,10 +2726,10 @@
         <v>2336.05</v>
       </c>
       <c r="W21" t="n">
-        <v>2342.94</v>
+        <v>2341.94</v>
       </c>
       <c r="X21" t="n">
-        <v>2343.94</v>
+        <v>2342.64</v>
       </c>
       <c r="Y21" t="b">
         <v>0</v>
@@ -2747,10 +2753,10 @@
         <v>0</v>
       </c>
       <c r="AF21" t="n">
-        <v>-69.93000000000001</v>
+        <v>-69.66</v>
       </c>
       <c r="AG21" t="n">
-        <v>814.01</v>
+        <v>436.0699999999998</v>
       </c>
       <c r="AH21" t="n">
         <v>0</v>
@@ -2824,26 +2830,28 @@
         <v>2350.4</v>
       </c>
       <c r="V22" t="n">
-        <v>2339.73</v>
+        <v>2345.4</v>
       </c>
       <c r="W22" t="n">
-        <v>2346.4</v>
+        <v>2345.4</v>
       </c>
       <c r="X22" t="n">
-        <v>2347.4</v>
+        <v>2346.1</v>
       </c>
       <c r="Y22" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z22" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="Z22" s="2" t="n">
+        <v>45440.625</v>
+      </c>
       <c r="AA22" s="2" t="n">
-        <v>45440.63541666666</v>
+        <v>45440.625</v>
       </c>
       <c r="AB22" s="2" t="n">
         <v>45440.63300925926</v>
       </c>
       <c r="AC22" s="2" t="n">
-        <v>45441.6203125</v>
+        <v>45441.49803240741</v>
       </c>
       <c r="AD22" t="inlineStr">
         <is>
@@ -2854,10 +2862,10 @@
         <v>1</v>
       </c>
       <c r="AF22" t="n">
-        <v>125.81</v>
+        <v>125.31</v>
       </c>
       <c r="AG22" t="n">
-        <v>939.8199999999999</v>
+        <v>561.3799999999999</v>
       </c>
       <c r="AH22" t="n">
         <v>1</v>
@@ -2931,42 +2939,42 @@
         <v>2351.41</v>
       </c>
       <c r="V23" t="n">
-        <v>2355.41</v>
+        <v>2356.41</v>
       </c>
       <c r="W23" t="n">
-        <v>2355.41</v>
+        <v>2356.41</v>
       </c>
       <c r="X23" t="n">
-        <v>2354.41</v>
+        <v>2355.71</v>
       </c>
       <c r="Y23" t="b">
         <v>1</v>
       </c>
       <c r="Z23" s="2" t="n">
-        <v>45441.38541666666</v>
+        <v>45441.25</v>
       </c>
       <c r="AA23" s="2" t="n">
-        <v>45441.38541666666</v>
+        <v>45441.25</v>
       </c>
       <c r="AB23" s="2" t="n">
         <v>45441.40065972223</v>
       </c>
       <c r="AC23" s="2" t="n">
-        <v>45441.41162037037</v>
+        <v>45441.25077546296</v>
       </c>
       <c r="AD23" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AE23" t="b">
         <v>1</v>
       </c>
       <c r="AF23" t="n">
-        <v>125.81</v>
+        <v>35.8</v>
       </c>
       <c r="AG23" t="n">
-        <v>1065.63</v>
+        <v>597.1799999999998</v>
       </c>
       <c r="AH23" t="n">
         <v>2</v>
@@ -3040,13 +3048,13 @@
         <v>2346.59</v>
       </c>
       <c r="V24" t="n">
-        <v>2342.59</v>
+        <v>2341.59</v>
       </c>
       <c r="W24" t="n">
-        <v>2342.59</v>
+        <v>2341.59</v>
       </c>
       <c r="X24" t="n">
-        <v>2343.59</v>
+        <v>2342.29</v>
       </c>
       <c r="Y24" t="b">
         <v>1</v>
@@ -3061,7 +3069,7 @@
         <v>45443.4137962963</v>
       </c>
       <c r="AC24" s="2" t="n">
-        <v>45443.30530092592</v>
+        <v>45443.3134375</v>
       </c>
       <c r="AD24" t="inlineStr">
         <is>
@@ -3072,10 +3080,10 @@
         <v>1</v>
       </c>
       <c r="AF24" t="n">
-        <v>53.92</v>
+        <v>35.8</v>
       </c>
       <c r="AG24" t="n">
-        <v>1119.55</v>
+        <v>632.9799999999998</v>
       </c>
       <c r="AH24" t="n">
         <v>3</v>
@@ -3152,17 +3160,17 @@
         <v>2332.74</v>
       </c>
       <c r="W25" t="n">
-        <v>2338.1</v>
+        <v>2337.1</v>
       </c>
       <c r="X25" t="n">
-        <v>2339.1</v>
+        <v>2337.8</v>
       </c>
       <c r="Y25" t="b">
         <v>0</v>
       </c>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" s="2" t="n">
-        <v>45448.34375</v>
+        <v>45448.33333333334</v>
       </c>
       <c r="AB25" s="2" t="n">
         <v>45448.66273148148</v>
@@ -3179,10 +3187,10 @@
         <v>0</v>
       </c>
       <c r="AF25" t="n">
-        <v>-42.43</v>
+        <v>-42.26</v>
       </c>
       <c r="AG25" t="n">
-        <v>1077.12</v>
+        <v>590.7199999999998</v>
       </c>
       <c r="AH25" t="n">
         <v>0</v>
@@ -3256,28 +3264,28 @@
         <v>2334.57</v>
       </c>
       <c r="V26" t="n">
-        <v>2330.57</v>
+        <v>2329.57</v>
       </c>
       <c r="W26" t="n">
-        <v>2330.57</v>
+        <v>2329.57</v>
       </c>
       <c r="X26" t="n">
-        <v>2331.57</v>
+        <v>2330.27</v>
       </c>
       <c r="Y26" t="b">
         <v>1</v>
       </c>
       <c r="Z26" s="2" t="n">
-        <v>45448.22916666666</v>
+        <v>45448.20833333334</v>
       </c>
       <c r="AA26" s="2" t="n">
-        <v>45448.22916666666</v>
+        <v>45448.20833333334</v>
       </c>
       <c r="AB26" s="2" t="n">
         <v>45448.25472222222</v>
       </c>
       <c r="AC26" s="2" t="n">
-        <v>45448.38711805556</v>
+        <v>45448.38762731481</v>
       </c>
       <c r="AD26" t="inlineStr">
         <is>
@@ -3288,10 +3296,10 @@
         <v>1</v>
       </c>
       <c r="AF26" t="n">
-        <v>125.81</v>
+        <v>125.31</v>
       </c>
       <c r="AG26" t="n">
-        <v>1202.93</v>
+        <v>716.0299999999997</v>
       </c>
       <c r="AH26" t="n">
         <v>1</v>
@@ -3368,17 +3376,17 @@
         <v>2348.81</v>
       </c>
       <c r="W27" t="n">
-        <v>2355.39</v>
+        <v>2354.39</v>
       </c>
       <c r="X27" t="n">
-        <v>2356.39</v>
+        <v>2355.09</v>
       </c>
       <c r="Y27" t="b">
         <v>0</v>
       </c>
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" s="2" t="n">
-        <v>45463.73958333334</v>
+        <v>45463.72916666666</v>
       </c>
       <c r="AB27" s="2" t="n">
         <v>45463.73726851852</v>
@@ -3395,10 +3403,10 @@
         <v>0</v>
       </c>
       <c r="AF27" t="n">
-        <v>-64.36</v>
+        <v>-64.09999999999999</v>
       </c>
       <c r="AG27" t="n">
-        <v>1138.57</v>
+        <v>651.9299999999997</v>
       </c>
       <c r="AH27" t="n">
         <v>0</v>
@@ -3475,10 +3483,10 @@
         <v>2342.96</v>
       </c>
       <c r="W28" t="n">
-        <v>2337.34</v>
+        <v>2338.34</v>
       </c>
       <c r="X28" t="n">
-        <v>2336.34</v>
+        <v>2337.64</v>
       </c>
       <c r="Y28" t="b">
         <v>0</v>
@@ -3502,10 +3510,10 @@
         <v>1</v>
       </c>
       <c r="AF28" t="n">
-        <v>125.81</v>
+        <v>125.31</v>
       </c>
       <c r="AG28" t="n">
-        <v>1264.38</v>
+        <v>777.2399999999998</v>
       </c>
       <c r="AH28" t="n">
         <v>1</v>
@@ -3579,28 +3587,28 @@
         <v>2325.99</v>
       </c>
       <c r="V29" t="n">
-        <v>2321.99</v>
+        <v>2320.99</v>
       </c>
       <c r="W29" t="n">
-        <v>2321.99</v>
+        <v>2320.99</v>
       </c>
       <c r="X29" t="n">
-        <v>2322.99</v>
+        <v>2321.69</v>
       </c>
       <c r="Y29" t="b">
         <v>1</v>
       </c>
       <c r="Z29" s="2" t="n">
-        <v>45455.97916666666</v>
+        <v>45455.96875</v>
       </c>
       <c r="AA29" s="2" t="n">
-        <v>45455.97916666666</v>
+        <v>45455.96875</v>
       </c>
       <c r="AB29" s="2" t="n">
         <v>45456.65079861111</v>
       </c>
       <c r="AC29" s="2" t="n">
-        <v>45456.08188657407</v>
+        <v>45456.09047453704</v>
       </c>
       <c r="AD29" t="inlineStr">
         <is>
@@ -3611,10 +3619,10 @@
         <v>1</v>
       </c>
       <c r="AF29" t="n">
-        <v>53.92</v>
+        <v>35.8</v>
       </c>
       <c r="AG29" t="n">
-        <v>1318.3</v>
+        <v>813.0399999999997</v>
       </c>
       <c r="AH29" t="n">
         <v>2</v>
@@ -3691,10 +3699,10 @@
         <v>2301.89</v>
       </c>
       <c r="W30" t="n">
-        <v>2309.97</v>
+        <v>2308.97</v>
       </c>
       <c r="X30" t="n">
-        <v>2310.97</v>
+        <v>2309.67</v>
       </c>
       <c r="Y30" t="b">
         <v>0</v>
@@ -3718,10 +3726,10 @@
         <v>1</v>
       </c>
       <c r="AF30" t="n">
-        <v>125.81</v>
+        <v>125.31</v>
       </c>
       <c r="AG30" t="n">
-        <v>1444.11</v>
+        <v>938.3499999999997</v>
       </c>
       <c r="AH30" t="n">
         <v>3</v>
@@ -3795,28 +3803,28 @@
         <v>2310.37</v>
       </c>
       <c r="V31" t="n">
-        <v>2306.37</v>
+        <v>2305.37</v>
       </c>
       <c r="W31" t="n">
-        <v>2306.37</v>
+        <v>2305.37</v>
       </c>
       <c r="X31" t="n">
-        <v>2307.37</v>
+        <v>2306.07</v>
       </c>
       <c r="Y31" t="b">
         <v>1</v>
       </c>
       <c r="Z31" s="2" t="n">
-        <v>45457.26041666666</v>
+        <v>45457.17708333334</v>
       </c>
       <c r="AA31" s="2" t="n">
-        <v>45457.26041666666</v>
+        <v>45457.17708333334</v>
       </c>
       <c r="AB31" s="2" t="n">
         <v>45457.35988425926</v>
       </c>
       <c r="AC31" s="2" t="n">
-        <v>45457.26668981482</v>
+        <v>45457.18391203704</v>
       </c>
       <c r="AD31" t="inlineStr">
         <is>
@@ -3827,10 +3835,10 @@
         <v>1</v>
       </c>
       <c r="AF31" t="n">
-        <v>53.92</v>
+        <v>35.8</v>
       </c>
       <c r="AG31" t="n">
-        <v>1498.03</v>
+        <v>974.1499999999996</v>
       </c>
       <c r="AH31" t="n">
         <v>4</v>
@@ -3904,13 +3912,13 @@
         <v>2317.94</v>
       </c>
       <c r="V32" t="n">
-        <v>2321.94</v>
+        <v>2322.94</v>
       </c>
       <c r="W32" t="n">
-        <v>2321.94</v>
+        <v>2322.94</v>
       </c>
       <c r="X32" t="n">
-        <v>2320.94</v>
+        <v>2322.24</v>
       </c>
       <c r="Y32" t="b">
         <v>1</v>
@@ -3925,7 +3933,7 @@
         <v>45460.77172453704</v>
       </c>
       <c r="AC32" s="2" t="n">
-        <v>45461.12537037037</v>
+        <v>45461.12627314815</v>
       </c>
       <c r="AD32" t="inlineStr">
         <is>
@@ -3936,10 +3944,10 @@
         <v>1</v>
       </c>
       <c r="AF32" t="n">
-        <v>125.81</v>
+        <v>125.33</v>
       </c>
       <c r="AG32" t="n">
-        <v>1623.84</v>
+        <v>1099.48</v>
       </c>
       <c r="AH32" t="n">
         <v>5</v>
@@ -4013,13 +4021,13 @@
         <v>2319.48</v>
       </c>
       <c r="V33" t="n">
-        <v>2315.48</v>
+        <v>2314.48</v>
       </c>
       <c r="W33" t="n">
-        <v>2315.48</v>
+        <v>2314.48</v>
       </c>
       <c r="X33" t="n">
-        <v>2316.48</v>
+        <v>2315.18</v>
       </c>
       <c r="Y33" t="b">
         <v>1</v>
@@ -4034,7 +4042,7 @@
         <v>45460.92664351852</v>
       </c>
       <c r="AC33" s="2" t="n">
-        <v>45460.84846064815</v>
+        <v>45460.8528125</v>
       </c>
       <c r="AD33" t="inlineStr">
         <is>
@@ -4045,10 +4053,10 @@
         <v>1</v>
       </c>
       <c r="AF33" t="n">
-        <v>53.92</v>
+        <v>35.81</v>
       </c>
       <c r="AG33" t="n">
-        <v>1677.76</v>
+        <v>1135.29</v>
       </c>
       <c r="AH33" t="n">
         <v>6</v>
@@ -4122,46 +4130,157 @@
         <v>2329.24</v>
       </c>
       <c r="V34" t="n">
-        <v>2339.83</v>
+        <v>2334.24</v>
       </c>
       <c r="W34" t="n">
-        <v>2333.24</v>
+        <v>2334.24</v>
       </c>
       <c r="X34" t="n">
-        <v>2332.24</v>
+        <v>2333.54</v>
       </c>
       <c r="Y34" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z34" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="Z34" s="2" t="n">
+        <v>45463.26041666666</v>
+      </c>
       <c r="AA34" s="2" t="n">
-        <v>45463.51041666666</v>
+        <v>45463.26041666666</v>
       </c>
       <c r="AB34" s="2" t="n">
         <v>132320.9911673006</v>
       </c>
       <c r="AC34" s="2" t="n">
-        <v>45463.31947916667</v>
+        <v>45463.26679398148</v>
       </c>
       <c r="AD34" t="inlineStr">
         <is>
-          <t>fail</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AE34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF34" t="n">
-        <v>-64.54000000000001</v>
+        <v>35.81</v>
       </c>
       <c r="AG34" t="n">
-        <v>1613.22</v>
+        <v>1171.099999999999</v>
       </c>
       <c r="AH34" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AI34" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>3392</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>45464.20833333334</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2359.53</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2361.53</v>
+      </c>
+      <c r="E35" t="n">
+        <v>2358.97</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2361.47</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1566</v>
+      </c>
+      <c r="H35" t="n">
+        <v>27</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>2360.799459543979</v>
+      </c>
+      <c r="K35" t="n">
+        <v>2359.503650661006</v>
+      </c>
+      <c r="L35" t="n">
+        <v>2361.580576923076</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1.295808882972324</v>
+      </c>
+      <c r="N35" t="n">
+        <v>1.710920156750212</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1.497236342544712</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.06446153846127345</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>2365.101845985511</v>
+      </c>
+      <c r="R35" t="n">
+        <v>2359.55930786064</v>
+      </c>
+      <c r="S35" t="b">
+        <v>1</v>
+      </c>
+      <c r="T35" t="b">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>2368.47</v>
+      </c>
+      <c r="V35" t="n">
+        <v>2363.47</v>
+      </c>
+      <c r="W35" t="n">
+        <v>2363.47</v>
+      </c>
+      <c r="X35" t="n">
+        <v>2364.17</v>
+      </c>
+      <c r="Y35" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="2" t="n">
+        <v>45464.375</v>
+      </c>
+      <c r="AA35" s="2" t="n">
+        <v>45464.375</v>
+      </c>
+      <c r="AB35" s="2" t="n">
+        <v>132320.9911673006</v>
+      </c>
+      <c r="AC35" s="2" t="n">
+        <v>45464.37663194445</v>
+      </c>
+      <c r="AD35" t="inlineStr">
+        <is>
+          <t>even</t>
+        </is>
+      </c>
+      <c r="AE35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>35.81</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>1206.909999999999</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
strategy changes for more trades
</commit_message>
<xml_diff>
--- a/filtered_excel_df.xlsx
+++ b/filtered_excel_df.xlsx
@@ -706,10 +706,10 @@
         <v>1</v>
       </c>
       <c r="AF2" t="n">
-        <v>125.36</v>
+        <v>125.77</v>
       </c>
       <c r="AG2" t="n">
-        <v>425.36</v>
+        <v>425.77</v>
       </c>
       <c r="AH2" t="n">
         <v>1</v>
@@ -815,10 +815,10 @@
         <v>1</v>
       </c>
       <c r="AF3" t="n">
-        <v>35.83</v>
+        <v>35.93</v>
       </c>
       <c r="AG3" t="n">
-        <v>461.19</v>
+        <v>461.7</v>
       </c>
       <c r="AH3" t="n">
         <v>2</v>
@@ -924,10 +924,10 @@
         <v>1</v>
       </c>
       <c r="AF4" t="n">
-        <v>125.41</v>
+        <v>125.76</v>
       </c>
       <c r="AG4" t="n">
-        <v>586.6</v>
+        <v>587.46</v>
       </c>
       <c r="AH4" t="n">
         <v>3</v>
@@ -1031,10 +1031,10 @@
         <v>1</v>
       </c>
       <c r="AF5" t="n">
-        <v>125.41</v>
+        <v>125.77</v>
       </c>
       <c r="AG5" t="n">
-        <v>712.01</v>
+        <v>713.23</v>
       </c>
       <c r="AH5" t="n">
         <v>4</v>
@@ -1140,10 +1140,10 @@
         <v>1</v>
       </c>
       <c r="AF6" t="n">
-        <v>125.39</v>
+        <v>125.77</v>
       </c>
       <c r="AG6" t="n">
-        <v>837.4</v>
+        <v>839</v>
       </c>
       <c r="AH6" t="n">
         <v>5</v>
@@ -1247,10 +1247,10 @@
         <v>0</v>
       </c>
       <c r="AF7" t="n">
-        <v>-80.45</v>
+        <v>-80.7</v>
       </c>
       <c r="AG7" t="n">
-        <v>756.9499999999999</v>
+        <v>758.3</v>
       </c>
       <c r="AH7" t="n">
         <v>0</v>
@@ -1354,10 +1354,10 @@
         <v>0</v>
       </c>
       <c r="AF8" t="n">
-        <v>-84.93000000000001</v>
+        <v>-85.19</v>
       </c>
       <c r="AG8" t="n">
-        <v>672.02</v>
+        <v>673.1099999999999</v>
       </c>
       <c r="AH8" t="n">
         <v>0</v>
@@ -1461,10 +1461,10 @@
         <v>0</v>
       </c>
       <c r="AF9" t="n">
-        <v>-94.61</v>
+        <v>-94.90000000000001</v>
       </c>
       <c r="AG9" t="n">
-        <v>577.41</v>
+        <v>578.2099999999999</v>
       </c>
       <c r="AH9" t="n">
         <v>0</v>
@@ -1568,10 +1568,10 @@
         <v>0</v>
       </c>
       <c r="AF10" t="n">
-        <v>-79.03</v>
+        <v>-79.26000000000001</v>
       </c>
       <c r="AG10" t="n">
-        <v>498.38</v>
+        <v>498.9499999999999</v>
       </c>
       <c r="AH10" t="n">
         <v>0</v>
@@ -1675,10 +1675,10 @@
         <v>0</v>
       </c>
       <c r="AF11" t="n">
-        <v>-80.98999999999999</v>
+        <v>-81.23999999999999</v>
       </c>
       <c r="AG11" t="n">
-        <v>417.39</v>
+        <v>417.7099999999999</v>
       </c>
       <c r="AH11" t="n">
         <v>0</v>
@@ -1784,10 +1784,10 @@
         <v>1</v>
       </c>
       <c r="AF12" t="n">
-        <v>125.4</v>
+        <v>125.77</v>
       </c>
       <c r="AG12" t="n">
-        <v>542.79</v>
+        <v>543.4799999999999</v>
       </c>
       <c r="AH12" t="n">
         <v>1</v>
@@ -1893,10 +1893,10 @@
         <v>1</v>
       </c>
       <c r="AF13" t="n">
-        <v>35.83</v>
+        <v>35.93</v>
       </c>
       <c r="AG13" t="n">
-        <v>578.62</v>
+        <v>579.4099999999999</v>
       </c>
       <c r="AH13" t="n">
         <v>2</v>
@@ -2002,10 +2002,10 @@
         <v>1</v>
       </c>
       <c r="AF14" t="n">
-        <v>125.4</v>
+        <v>125.77</v>
       </c>
       <c r="AG14" t="n">
-        <v>704.02</v>
+        <v>705.1799999999998</v>
       </c>
       <c r="AH14" t="n">
         <v>3</v>
@@ -2109,10 +2109,10 @@
         <v>0</v>
       </c>
       <c r="AF15" t="n">
-        <v>-64.87</v>
+        <v>-65.06</v>
       </c>
       <c r="AG15" t="n">
-        <v>639.15</v>
+        <v>640.1199999999999</v>
       </c>
       <c r="AH15" t="n">
         <v>0</v>
@@ -2216,10 +2216,10 @@
         <v>1</v>
       </c>
       <c r="AF16" t="n">
-        <v>125.41</v>
+        <v>125.77</v>
       </c>
       <c r="AG16" t="n">
-        <v>764.5599999999999</v>
+        <v>765.8899999999999</v>
       </c>
       <c r="AH16" t="n">
         <v>1</v>
@@ -2323,10 +2323,10 @@
         <v>0</v>
       </c>
       <c r="AF17" t="n">
-        <v>-74.73999999999999</v>
+        <v>-74.94</v>
       </c>
       <c r="AG17" t="n">
-        <v>689.8199999999999</v>
+        <v>690.9499999999998</v>
       </c>
       <c r="AH17" t="n">
         <v>0</v>
@@ -2432,10 +2432,10 @@
         <v>1</v>
       </c>
       <c r="AF18" t="n">
-        <v>125.43</v>
+        <v>125.77</v>
       </c>
       <c r="AG18" t="n">
-        <v>815.25</v>
+        <v>816.7199999999998</v>
       </c>
       <c r="AH18" t="n">
         <v>1</v>
@@ -2541,10 +2541,10 @@
         <v>1</v>
       </c>
       <c r="AF19" t="n">
-        <v>35.84</v>
+        <v>35.94</v>
       </c>
       <c r="AG19" t="n">
-        <v>851.09</v>
+        <v>852.6599999999999</v>
       </c>
       <c r="AH19" t="n">
         <v>2</v>
@@ -2648,10 +2648,10 @@
         <v>0</v>
       </c>
       <c r="AF20" t="n">
-        <v>-97.31999999999999</v>
+        <v>-97.59999999999999</v>
       </c>
       <c r="AG20" t="n">
-        <v>753.77</v>
+        <v>755.0599999999998</v>
       </c>
       <c r="AH20" t="n">
         <v>0</v>
@@ -2755,10 +2755,10 @@
         <v>0</v>
       </c>
       <c r="AF21" t="n">
-        <v>-78.15000000000001</v>
+        <v>-78.38</v>
       </c>
       <c r="AG21" t="n">
-        <v>675.62</v>
+        <v>676.6799999999998</v>
       </c>
       <c r="AH21" t="n">
         <v>0</v>
@@ -2862,10 +2862,10 @@
         <v>0</v>
       </c>
       <c r="AF22" t="n">
-        <v>-43.73</v>
+        <v>-43.86</v>
       </c>
       <c r="AG22" t="n">
-        <v>631.89</v>
+        <v>632.8199999999998</v>
       </c>
       <c r="AH22" t="n">
         <v>0</v>
@@ -2971,10 +2971,10 @@
         <v>1</v>
       </c>
       <c r="AF23" t="n">
-        <v>125.46</v>
+        <v>125.81</v>
       </c>
       <c r="AG23" t="n">
-        <v>757.35</v>
+        <v>758.6299999999999</v>
       </c>
       <c r="AH23" t="n">
         <v>1</v>
@@ -3080,10 +3080,10 @@
         <v>1</v>
       </c>
       <c r="AF24" t="n">
-        <v>125.46</v>
+        <v>125.81</v>
       </c>
       <c r="AG24" t="n">
-        <v>882.8100000000001</v>
+        <v>884.4399999999998</v>
       </c>
       <c r="AH24" t="n">
         <v>2</v>
@@ -3189,10 +3189,10 @@
         <v>1</v>
       </c>
       <c r="AF25" t="n">
-        <v>35.84</v>
+        <v>35.95</v>
       </c>
       <c r="AG25" t="n">
-        <v>918.6500000000001</v>
+        <v>920.3899999999999</v>
       </c>
       <c r="AH25" t="n">
         <v>3</v>
@@ -3296,10 +3296,10 @@
         <v>1</v>
       </c>
       <c r="AF26" t="n">
-        <v>125.44</v>
+        <v>125.81</v>
       </c>
       <c r="AG26" t="n">
-        <v>1044.09</v>
+        <v>1046.2</v>
       </c>
       <c r="AH26" t="n">
         <v>4</v>
@@ -3405,10 +3405,10 @@
         <v>1</v>
       </c>
       <c r="AF27" t="n">
-        <v>35.83</v>
+        <v>35.95</v>
       </c>
       <c r="AG27" t="n">
-        <v>1079.92</v>
+        <v>1082.15</v>
       </c>
       <c r="AH27" t="n">
         <v>5</v>
@@ -3514,10 +3514,10 @@
         <v>1</v>
       </c>
       <c r="AF28" t="n">
-        <v>35.81</v>
+        <v>35.95</v>
       </c>
       <c r="AG28" t="n">
-        <v>1115.73</v>
+        <v>1118.1</v>
       </c>
       <c r="AH28" t="n">
         <v>6</v>
@@ -3621,10 +3621,10 @@
         <v>0</v>
       </c>
       <c r="AF29" t="n">
-        <v>-54.27</v>
+        <v>-54.48</v>
       </c>
       <c r="AG29" t="n">
-        <v>1061.46</v>
+        <v>1063.62</v>
       </c>
       <c r="AH29" t="n">
         <v>0</v>
@@ -3728,10 +3728,10 @@
         <v>0</v>
       </c>
       <c r="AF30" t="n">
-        <v>-50.69</v>
+        <v>-50.88</v>
       </c>
       <c r="AG30" t="n">
-        <v>1010.77</v>
+        <v>1012.74</v>
       </c>
       <c r="AH30" t="n">
         <v>0</v>
@@ -3837,10 +3837,10 @@
         <v>1</v>
       </c>
       <c r="AF31" t="n">
-        <v>35.81</v>
+        <v>35.95</v>
       </c>
       <c r="AG31" t="n">
-        <v>1046.58</v>
+        <v>1048.69</v>
       </c>
       <c r="AH31" t="n">
         <v>1</v>
@@ -3944,10 +3944,10 @@
         <v>0</v>
       </c>
       <c r="AF32" t="n">
-        <v>-66.63</v>
+        <v>-66.88</v>
       </c>
       <c r="AG32" t="n">
-        <v>979.9499999999999</v>
+        <v>981.8099999999998</v>
       </c>
       <c r="AH32" t="n">
         <v>0</v>
@@ -4051,10 +4051,10 @@
         <v>1</v>
       </c>
       <c r="AF33" t="n">
-        <v>-67.70999999999999</v>
+        <v>-67.95999999999999</v>
       </c>
       <c r="AG33" t="n">
-        <v>912.2399999999999</v>
+        <v>913.8499999999998</v>
       </c>
       <c r="AH33" t="n">
         <v>1</v>
@@ -4158,10 +4158,10 @@
         <v>0</v>
       </c>
       <c r="AF34" t="n">
-        <v>-66.98999999999999</v>
+        <v>-67.23999999999999</v>
       </c>
       <c r="AG34" t="n">
-        <v>845.2499999999999</v>
+        <v>846.6099999999998</v>
       </c>
       <c r="AH34" t="n">
         <v>0</v>
@@ -4265,10 +4265,10 @@
         <v>0</v>
       </c>
       <c r="AF35" t="n">
-        <v>-69.67</v>
+        <v>-69.94</v>
       </c>
       <c r="AG35" t="n">
-        <v>775.5799999999999</v>
+        <v>776.6699999999998</v>
       </c>
       <c r="AH35" t="n">
         <v>0</v>
@@ -4374,10 +4374,10 @@
         <v>1</v>
       </c>
       <c r="AF36" t="n">
-        <v>125.35</v>
+        <v>125.82</v>
       </c>
       <c r="AG36" t="n">
-        <v>900.9299999999999</v>
+        <v>902.4899999999998</v>
       </c>
       <c r="AH36" t="n">
         <v>1</v>
@@ -4483,10 +4483,10 @@
         <v>1</v>
       </c>
       <c r="AF37" t="n">
-        <v>35.81</v>
+        <v>35.95</v>
       </c>
       <c r="AG37" t="n">
-        <v>936.74</v>
+        <v>938.4399999999998</v>
       </c>
       <c r="AH37" t="n">
         <v>2</v>
@@ -4592,10 +4592,10 @@
         <v>1</v>
       </c>
       <c r="AF38" t="n">
-        <v>35.81</v>
+        <v>35.95</v>
       </c>
       <c r="AG38" t="n">
-        <v>972.55</v>
+        <v>974.3899999999999</v>
       </c>
       <c r="AH38" t="n">
         <v>3</v>
@@ -4699,10 +4699,10 @@
         <v>0</v>
       </c>
       <c r="AF39" t="n">
-        <v>-42.27</v>
+        <v>-42.43</v>
       </c>
       <c r="AG39" t="n">
-        <v>930.28</v>
+        <v>931.9599999999999</v>
       </c>
       <c r="AH39" t="n">
         <v>0</v>
@@ -4808,10 +4808,10 @@
         <v>1</v>
       </c>
       <c r="AF40" t="n">
-        <v>125.34</v>
+        <v>125.81</v>
       </c>
       <c r="AG40" t="n">
-        <v>1055.62</v>
+        <v>1057.77</v>
       </c>
       <c r="AH40" t="n">
         <v>1</v>
@@ -4915,10 +4915,10 @@
         <v>0</v>
       </c>
       <c r="AF41" t="n">
-        <v>-64.12</v>
+        <v>-64.36</v>
       </c>
       <c r="AG41" t="n">
-        <v>991.4999999999999</v>
+        <v>993.41</v>
       </c>
       <c r="AH41" t="n">
         <v>0</v>
@@ -5022,10 +5022,10 @@
         <v>1</v>
       </c>
       <c r="AF42" t="n">
-        <v>125.35</v>
+        <v>125.81</v>
       </c>
       <c r="AG42" t="n">
-        <v>1116.85</v>
+        <v>1119.22</v>
       </c>
       <c r="AH42" t="n">
         <v>1</v>
@@ -5131,10 +5131,10 @@
         <v>1</v>
       </c>
       <c r="AF43" t="n">
-        <v>35.82</v>
+        <v>35.95</v>
       </c>
       <c r="AG43" t="n">
-        <v>1152.67</v>
+        <v>1155.17</v>
       </c>
       <c r="AH43" t="n">
         <v>2</v>
@@ -5238,10 +5238,10 @@
         <v>1</v>
       </c>
       <c r="AF44" t="n">
-        <v>125.36</v>
+        <v>125.81</v>
       </c>
       <c r="AG44" t="n">
-        <v>1278.03</v>
+        <v>1280.98</v>
       </c>
       <c r="AH44" t="n">
         <v>3</v>
@@ -5347,10 +5347,10 @@
         <v>1</v>
       </c>
       <c r="AF45" t="n">
-        <v>35.82</v>
+        <v>35.95</v>
       </c>
       <c r="AG45" t="n">
-        <v>1313.85</v>
+        <v>1316.93</v>
       </c>
       <c r="AH45" t="n">
         <v>4</v>
@@ -5456,10 +5456,10 @@
         <v>1</v>
       </c>
       <c r="AF46" t="n">
-        <v>125.36</v>
+        <v>125.82</v>
       </c>
       <c r="AG46" t="n">
-        <v>1439.21</v>
+        <v>1442.75</v>
       </c>
       <c r="AH46" t="n">
         <v>5</v>
@@ -5565,10 +5565,10 @@
         <v>1</v>
       </c>
       <c r="AF47" t="n">
-        <v>35.82</v>
+        <v>35.95</v>
       </c>
       <c r="AG47" t="n">
-        <v>1475.03</v>
+        <v>1478.7</v>
       </c>
       <c r="AH47" t="n">
         <v>6</v>
@@ -5660,7 +5660,7 @@
         <v>45463.26041666666</v>
       </c>
       <c r="AB48" s="2" t="n">
-        <v>132320.9911673006</v>
+        <v>45464.72574074074</v>
       </c>
       <c r="AC48" s="2" t="n">
         <v>45463.26679398148</v>
@@ -5674,10 +5674,10 @@
         <v>1</v>
       </c>
       <c r="AF48" t="n">
-        <v>35.82</v>
+        <v>35.95</v>
       </c>
       <c r="AG48" t="n">
-        <v>1510.849999999999</v>
+        <v>1514.65</v>
       </c>
       <c r="AH48" t="n">
         <v>7</v>
@@ -5769,7 +5769,7 @@
         <v>45464.375</v>
       </c>
       <c r="AB49" s="2" t="n">
-        <v>132320.9911673006</v>
+        <v>45464.61050925926</v>
       </c>
       <c r="AC49" s="2" t="n">
         <v>45464.37663194445</v>
@@ -5783,10 +5783,10 @@
         <v>1</v>
       </c>
       <c r="AF49" t="n">
-        <v>35.82</v>
+        <v>35.95</v>
       </c>
       <c r="AG49" t="n">
-        <v>1546.669999999999</v>
+        <v>1550.6</v>
       </c>
       <c r="AH49" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
fixed success key error
</commit_message>
<xml_diff>
--- a/filtered_excel_df.xlsx
+++ b/filtered_excel_df.xlsx
@@ -995,10 +995,10 @@
         <v>0</v>
       </c>
       <c r="AV3" t="n">
-        <v>-73.69</v>
+        <v>-73.70999999999999</v>
       </c>
       <c r="AW3" t="n">
-        <v>376.31</v>
+        <v>376.29</v>
       </c>
       <c r="AX3" t="n">
         <v>0</v>
@@ -1145,7 +1145,7 @@
         <v>69.33979999999865</v>
       </c>
       <c r="AS4" t="n">
-        <v>63.91</v>
+        <v>63.93</v>
       </c>
       <c r="AT4" t="inlineStr">
         <is>
@@ -1159,7 +1159,7 @@
         <v>18.42</v>
       </c>
       <c r="AW4" t="n">
-        <v>394.73</v>
+        <v>394.71</v>
       </c>
       <c r="AX4" t="n">
         <v>1</v>
@@ -1306,7 +1306,7 @@
         <v>97.75940000000118</v>
       </c>
       <c r="AS5" t="n">
-        <v>90.06</v>
+        <v>90.08</v>
       </c>
       <c r="AT5" t="inlineStr">
         <is>
@@ -1320,7 +1320,7 @@
         <v>18.42</v>
       </c>
       <c r="AW5" t="n">
-        <v>413.15</v>
+        <v>413.1300000000001</v>
       </c>
       <c r="AX5" t="n">
         <v>2</v>
@@ -1465,7 +1465,7 @@
         <v>100</v>
       </c>
       <c r="AS6" t="n">
-        <v>92.64</v>
+        <v>92.66</v>
       </c>
       <c r="AT6" t="inlineStr">
         <is>
@@ -1476,10 +1476,10 @@
         <v>1</v>
       </c>
       <c r="AV6" t="n">
-        <v>92.09</v>
+        <v>92.11</v>
       </c>
       <c r="AW6" t="n">
-        <v>505.24</v>
+        <v>505.2400000000001</v>
       </c>
       <c r="AX6" t="n">
         <v>3</v>
@@ -1624,7 +1624,7 @@
         <v>100</v>
       </c>
       <c r="AS7" t="n">
-        <v>92.45</v>
+        <v>92.48</v>
       </c>
       <c r="AT7" t="inlineStr">
         <is>
@@ -1635,10 +1635,10 @@
         <v>1</v>
       </c>
       <c r="AV7" t="n">
-        <v>92.09</v>
+        <v>92.11</v>
       </c>
       <c r="AW7" t="n">
-        <v>597.33</v>
+        <v>597.35</v>
       </c>
       <c r="AX7" t="n">
         <v>4</v>
@@ -1783,7 +1783,7 @@
         <v>49.41399999999994</v>
       </c>
       <c r="AS8" t="n">
-        <v>45.49</v>
+        <v>45.5</v>
       </c>
       <c r="AT8" t="inlineStr">
         <is>
@@ -1794,10 +1794,10 @@
         <v>0</v>
       </c>
       <c r="AV8" t="n">
-        <v>-73.69</v>
+        <v>-73.70999999999999</v>
       </c>
       <c r="AW8" t="n">
-        <v>523.6400000000001</v>
+        <v>523.64</v>
       </c>
       <c r="AX8" t="n">
         <v>0</v>
@@ -1944,7 +1944,7 @@
         <v>100</v>
       </c>
       <c r="AS9" t="n">
-        <v>94.66</v>
+        <v>94.69</v>
       </c>
       <c r="AT9" t="inlineStr">
         <is>
@@ -1955,10 +1955,10 @@
         <v>1</v>
       </c>
       <c r="AV9" t="n">
-        <v>92.09</v>
+        <v>92.11</v>
       </c>
       <c r="AW9" t="n">
-        <v>615.7300000000001</v>
+        <v>615.75</v>
       </c>
       <c r="AX9" t="n">
         <v>1</v>
@@ -2105,7 +2105,7 @@
         <v>100</v>
       </c>
       <c r="AS10" t="n">
-        <v>94.48</v>
+        <v>94.51000000000001</v>
       </c>
       <c r="AT10" t="inlineStr">
         <is>
@@ -2116,10 +2116,10 @@
         <v>1</v>
       </c>
       <c r="AV10" t="n">
-        <v>92.09</v>
+        <v>92.11</v>
       </c>
       <c r="AW10" t="n">
-        <v>707.8200000000002</v>
+        <v>707.86</v>
       </c>
       <c r="AX10" t="n">
         <v>2</v>
@@ -2277,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="AV11" t="n">
-        <v>-73.69</v>
+        <v>-73.70999999999999</v>
       </c>
       <c r="AW11" t="n">
-        <v>634.1300000000001</v>
+        <v>634.15</v>
       </c>
       <c r="AX11" t="n">
         <v>0</v>
@@ -2427,7 +2427,7 @@
         <v>100</v>
       </c>
       <c r="AS12" t="n">
-        <v>93.37</v>
+        <v>93.40000000000001</v>
       </c>
       <c r="AT12" t="inlineStr">
         <is>
@@ -2438,10 +2438,10 @@
         <v>1</v>
       </c>
       <c r="AV12" t="n">
-        <v>92.09</v>
+        <v>92.11</v>
       </c>
       <c r="AW12" t="n">
-        <v>726.2200000000001</v>
+        <v>726.26</v>
       </c>
       <c r="AX12" t="n">
         <v>1</v>
@@ -2590,7 +2590,7 @@
         <v>46.41960000000108</v>
       </c>
       <c r="AS13" t="n">
-        <v>42.73</v>
+        <v>42.74</v>
       </c>
       <c r="AT13" t="inlineStr">
         <is>
@@ -2604,7 +2604,7 @@
         <v>18.42</v>
       </c>
       <c r="AW13" t="n">
-        <v>744.6400000000001</v>
+        <v>744.6799999999999</v>
       </c>
       <c r="AX13" t="n">
         <v>2</v>
@@ -2751,7 +2751,7 @@
         <v>95.18039999999893</v>
       </c>
       <c r="AS14" t="n">
-        <v>87.66</v>
+        <v>87.69</v>
       </c>
       <c r="AT14" t="inlineStr">
         <is>
@@ -2762,10 +2762,10 @@
         <v>0</v>
       </c>
       <c r="AV14" t="n">
-        <v>-73.69</v>
+        <v>-73.70999999999999</v>
       </c>
       <c r="AW14" t="n">
-        <v>670.95</v>
+        <v>670.9699999999999</v>
       </c>
       <c r="AX14" t="n">
         <v>0</v>
@@ -2914,7 +2914,7 @@
         <v>100</v>
       </c>
       <c r="AS15" t="n">
-        <v>93.01000000000001</v>
+        <v>93.03</v>
       </c>
       <c r="AT15" t="inlineStr">
         <is>
@@ -2925,10 +2925,10 @@
         <v>1</v>
       </c>
       <c r="AV15" t="n">
-        <v>92.09</v>
+        <v>92.11</v>
       </c>
       <c r="AW15" t="n">
-        <v>763.0400000000001</v>
+        <v>763.0799999999999</v>
       </c>
       <c r="AX15" t="n">
         <v>1</v>
@@ -3075,7 +3075,7 @@
         <v>100</v>
       </c>
       <c r="AS16" t="n">
-        <v>93.19</v>
+        <v>93.22</v>
       </c>
       <c r="AT16" t="inlineStr">
         <is>
@@ -3086,10 +3086,10 @@
         <v>1</v>
       </c>
       <c r="AV16" t="n">
-        <v>92.09</v>
+        <v>92.11</v>
       </c>
       <c r="AW16" t="n">
-        <v>855.1300000000001</v>
+        <v>855.1899999999999</v>
       </c>
       <c r="AX16" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
no longer need to push csv files
</commit_message>
<xml_diff>
--- a/filtered_excel_df.xlsx
+++ b/filtered_excel_df.xlsx
@@ -834,16 +834,16 @@
         <v>1.103976700108335</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0005625621254012441</v>
+        <v>0.0005625621254012641</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.000132892167184748</v>
+        <v>-0.000132892167184728</v>
       </c>
       <c r="N2" t="n">
-        <v>3.717965388881562e-05</v>
+        <v>3.717965388884158e-05</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.0002810527295769741</v>
+        <v>-0.0002810527295769481</v>
       </c>
       <c r="P2" t="n">
         <v>1.102380053355647</v>
@@ -987,16 +987,16 @@
         <v>45293.5234837963</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN2" t="b">
         <v>1</v>
       </c>
       <c r="BO2" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP2" t="n">
-        <v>714.66</v>
+        <v>743.97</v>
       </c>
       <c r="BQ2" t="inlineStr"/>
       <c r="BR2" t="n">
@@ -1047,16 +1047,16 @@
         <v>1.10345</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.0008297774663810043</v>
+        <v>-0.0008297774663809894</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.0008212831803437468</v>
+        <v>-0.0008212831803437318</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.0002527880739864354</v>
+        <v>-0.0002527880739864094</v>
       </c>
       <c r="O3" t="n">
-        <v>-0.0001902624927409818</v>
+        <v>-0.0001902624927409558</v>
       </c>
       <c r="P3" t="n">
         <v>1.102459642059706</v>
@@ -1078,10 +1078,10 @@
         <v>1.102219761904762</v>
       </c>
       <c r="W3" t="n">
-        <v>-0.0002491483076996399</v>
+        <v>-0.0002491483076996476</v>
       </c>
       <c r="X3" t="n">
-        <v>-7.154300701045606e-05</v>
+        <v>-7.15430070104637e-05</v>
       </c>
       <c r="Y3" t="n">
         <v>1.102443928571429</v>
@@ -1099,10 +1099,10 @@
         <v>1.103513897725263</v>
       </c>
       <c r="AD3" t="n">
-        <v>7.339999611457545e-05</v>
+        <v>7.339999611458304e-05</v>
       </c>
       <c r="AE3" t="n">
-        <v>-4.568452957131297e-05</v>
+        <v>-4.568452957130536e-05</v>
       </c>
       <c r="AF3" t="n">
         <v>1.101844314213619</v>
@@ -1198,16 +1198,16 @@
       </c>
       <c r="BL3" t="inlineStr"/>
       <c r="BM3" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN3" t="b">
         <v>1</v>
       </c>
       <c r="BO3" t="n">
-        <v>91.59999999999999</v>
+        <v>274.83</v>
       </c>
       <c r="BP3" t="n">
-        <v>806.26</v>
+        <v>1018.8</v>
       </c>
       <c r="BQ3" t="inlineStr"/>
       <c r="BR3" t="n">
@@ -1258,16 +1258,16 @@
         <v>1.10195</v>
       </c>
       <c r="L4" t="n">
-        <v>3.107862077660194e-06</v>
+        <v>3.107862077680279e-06</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.0002822704977555949</v>
+        <v>-0.0002822704977555748</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0003128177301227008</v>
+        <v>-0.0003128177301226859</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.0005472227570029678</v>
+        <v>-0.000547222757002953</v>
       </c>
       <c r="P4" t="n">
         <v>1.102781675974336</v>
@@ -1289,10 +1289,10 @@
         <v>1.102219761904762</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.0002491483076996399</v>
+        <v>-0.0002491483076996476</v>
       </c>
       <c r="X4" t="n">
-        <v>-7.154300701045606e-05</v>
+        <v>-7.15430070104637e-05</v>
       </c>
       <c r="Y4" t="n">
         <v>1.102443928571429</v>
@@ -1310,10 +1310,10 @@
         <v>1.103513897725263</v>
       </c>
       <c r="AD4" t="n">
-        <v>7.339999611457545e-05</v>
+        <v>7.339999611458304e-05</v>
       </c>
       <c r="AE4" t="n">
-        <v>-4.568452957131297e-05</v>
+        <v>-4.568452957130536e-05</v>
       </c>
       <c r="AF4" t="n">
         <v>1.101844314213619</v>
@@ -1411,16 +1411,16 @@
         <v>45293.52337962963</v>
       </c>
       <c r="BM4" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN4" t="b">
         <v>1</v>
       </c>
       <c r="BO4" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP4" t="n">
-        <v>820.92</v>
+        <v>1062.77</v>
       </c>
       <c r="BQ4" t="inlineStr"/>
       <c r="BR4" t="n">
@@ -1471,22 +1471,22 @@
         <v>1.10165</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0001663810363405276</v>
+        <v>0.0001663810363405462</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.0001818716511032766</v>
+        <v>-0.0001818716511032581</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.0008113058846554884</v>
+        <v>-0.0008113058846554624</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.0009951489981755083</v>
+        <v>-0.0009951489981754823</v>
       </c>
       <c r="P5" t="n">
         <v>1.10284332473382</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.10424924166338</v>
+        <v>1.104249241663379</v>
       </c>
       <c r="R5" s="2" t="n">
         <v>45293.5</v>
@@ -1523,10 +1523,10 @@
         <v>1.104048270943628</v>
       </c>
       <c r="AD5" t="n">
-        <v>-7.154300701045606e-05</v>
+        <v>-7.15430070104637e-05</v>
       </c>
       <c r="AE5" t="n">
-        <v>-0.0002491483076996399</v>
+        <v>-0.0002491483076996476</v>
       </c>
       <c r="AF5" t="n">
         <v>1.101088104737873</v>
@@ -1624,16 +1624,16 @@
         <v>45293.55274305555</v>
       </c>
       <c r="BM5" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN5" t="b">
         <v>1</v>
       </c>
       <c r="BO5" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP5" t="n">
-        <v>835.5799999999999</v>
+        <v>1106.74</v>
       </c>
       <c r="BQ5" t="inlineStr"/>
       <c r="BR5" t="n">
@@ -1684,16 +1684,16 @@
         <v>1.09182</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0003423917784751058</v>
+        <v>0.0003423917784751243</v>
       </c>
       <c r="M6" t="n">
-        <v>-1.858876562218149e-05</v>
+        <v>-1.858876562216295e-05</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0006405805642645864</v>
+        <v>-0.0006405805642645667</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.0002777880620179127</v>
+        <v>-0.000277788062017893</v>
       </c>
       <c r="P6" t="n">
         <v>1.091313654939383</v>
@@ -1717,10 +1717,10 @@
         <v>1.091096428571429</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.0004036387479401274</v>
+        <v>-0.0004036387479401299</v>
       </c>
       <c r="X6" t="n">
-        <v>0.0002014665683177163</v>
+        <v>0.0002014665683177137</v>
       </c>
       <c r="Y6" t="n">
         <v>1.091590952380953</v>
@@ -1738,10 +1738,10 @@
         <v>1.093823903948947</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.0002715814298317457</v>
+        <v>-0.000271581429831733</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.0002478393967054742</v>
+        <v>-0.0002478393967054616</v>
       </c>
       <c r="AF6" t="n">
         <v>1.090902357172989</v>
@@ -1841,16 +1841,16 @@
         <v>45294.88635416667</v>
       </c>
       <c r="BM6" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN6" t="b">
         <v>1</v>
       </c>
       <c r="BO6" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP6" t="n">
-        <v>850.2399999999999</v>
+        <v>1150.71</v>
       </c>
       <c r="BQ6" t="inlineStr"/>
       <c r="BR6" t="n">
@@ -1901,22 +1901,22 @@
         <v>1.095563348454684</v>
       </c>
       <c r="L7" t="n">
-        <v>4.566971295858888e-06</v>
+        <v>4.566971295881142e-06</v>
       </c>
       <c r="M7" t="n">
-        <v>-1.522000635435092e-05</v>
+        <v>-1.522000635432866e-05</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0001719554089344839</v>
+        <v>0.0001719554089345061</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0001202570469781759</v>
+        <v>0.0001202570469781982</v>
       </c>
       <c r="P7" t="n">
         <v>1.09462031980158</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.095040455958558</v>
+        <v>1.095040455958557</v>
       </c>
       <c r="R7" s="2" t="n">
         <v>45296.125</v>
@@ -2060,16 +2060,16 @@
         <v>45296.67912037037</v>
       </c>
       <c r="BM7" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN7" t="b">
         <v>1</v>
       </c>
       <c r="BO7" t="n">
-        <v>91.59999999999999</v>
+        <v>274.83</v>
       </c>
       <c r="BP7" t="n">
-        <v>941.8399999999999</v>
+        <v>1425.54</v>
       </c>
       <c r="BQ7" t="inlineStr"/>
       <c r="BR7" t="n">
@@ -2120,16 +2120,16 @@
         <v>1.095519049906471</v>
       </c>
       <c r="L8" t="n">
-        <v>-5.75584870616731e-05</v>
+        <v>-5.755848706164931e-05</v>
       </c>
       <c r="M8" t="n">
-        <v>-6.803170005686655e-05</v>
+        <v>-6.803170005684278e-05</v>
       </c>
       <c r="N8" t="n">
-        <v>1.912508817831289e-05</v>
+        <v>1.912508817833886e-05</v>
       </c>
       <c r="O8" t="n">
-        <v>1.869851155059669e-05</v>
+        <v>1.869851155062265e-05</v>
       </c>
       <c r="P8" t="n">
         <v>1.094941859953228</v>
@@ -2279,16 +2279,16 @@
         <v>45296.67912037037</v>
       </c>
       <c r="BM8" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN8" t="b">
         <v>1</v>
       </c>
       <c r="BO8" t="n">
-        <v>91.59999999999999</v>
+        <v>274.83</v>
       </c>
       <c r="BP8" t="n">
-        <v>1033.44</v>
+        <v>1700.37</v>
       </c>
       <c r="BQ8" t="inlineStr"/>
       <c r="BR8" t="n">
@@ -2339,16 +2339,16 @@
         <v>1.095457337865719</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0002365926659236495</v>
+        <v>-0.0002365926659236236</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0002366177027410276</v>
+        <v>-0.0002366177027410017</v>
       </c>
       <c r="N9" t="n">
-        <v>-7.802777684450638e-05</v>
+        <v>-7.802777684449156e-05</v>
       </c>
       <c r="O9" t="n">
-        <v>2.326338023844653e-05</v>
+        <v>2.326338023846137e-05</v>
       </c>
       <c r="P9" t="n">
         <v>1.094972315250603</v>
@@ -2498,16 +2498,16 @@
         <v>45296.67916666667</v>
       </c>
       <c r="BM9" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN9" t="b">
         <v>1</v>
       </c>
       <c r="BO9" t="n">
-        <v>91.59999999999999</v>
+        <v>274.83</v>
       </c>
       <c r="BP9" t="n">
-        <v>1125.04</v>
+        <v>1975.2</v>
       </c>
       <c r="BQ9" t="inlineStr"/>
       <c r="BR9" t="n">
@@ -2558,16 +2558,16 @@
         <v>1.095198678010586</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.0002433948348646795</v>
+        <v>-0.0002433948348646684</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.0002370817808695181</v>
+        <v>-0.000237081780869507</v>
       </c>
       <c r="N10" t="n">
-        <v>-6.803170005686655e-05</v>
+        <v>-6.803170005684278e-05</v>
       </c>
       <c r="O10" t="n">
-        <v>-5.75584870616731e-05</v>
+        <v>-5.755848706164931e-05</v>
       </c>
       <c r="P10" t="n">
         <v>1.095004290390314</v>
@@ -2717,16 +2717,16 @@
         <v>45296.27300925926</v>
       </c>
       <c r="BM10" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN10" t="b">
         <v>1</v>
       </c>
       <c r="BO10" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP10" t="n">
-        <v>1139.7</v>
+        <v>2019.17</v>
       </c>
       <c r="BQ10" t="inlineStr"/>
       <c r="BR10" t="n">
@@ -2777,16 +2777,16 @@
         <v>1.09495</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.0002345623796050615</v>
+        <v>-0.0002345623796050355</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.0002453497068003821</v>
+        <v>-0.0002453497068003561</v>
       </c>
       <c r="N11" t="n">
-        <v>-0.0001726120159934097</v>
+        <v>-0.0001726120159933949</v>
       </c>
       <c r="O11" t="n">
-        <v>-0.0001215075353745791</v>
+        <v>-0.0001215075353745643</v>
       </c>
       <c r="P11" t="n">
         <v>1.094997971200884</v>
@@ -2936,16 +2936,16 @@
         <v>45296.67077546296</v>
       </c>
       <c r="BM11" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN11" t="b">
         <v>1</v>
       </c>
       <c r="BO11" t="n">
-        <v>91.59999999999999</v>
+        <v>274.83</v>
       </c>
       <c r="BP11" t="n">
-        <v>1231.3</v>
+        <v>2294</v>
       </c>
       <c r="BQ11" t="inlineStr"/>
       <c r="BR11" t="n">
@@ -2996,16 +2996,16 @@
         <v>1.09468</v>
       </c>
       <c r="L12" t="n">
-        <v>-9.749792255601432e-05</v>
+        <v>-9.749792255599424e-05</v>
       </c>
       <c r="M12" t="n">
-        <v>-0.0002013150342937231</v>
+        <v>-0.000201315034293703</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.0002366177027410276</v>
+        <v>-0.0002366177027410017</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0002365926659236495</v>
+        <v>-0.0002365926659236236</v>
       </c>
       <c r="P12" t="n">
         <v>1.095056650204181</v>
@@ -3155,16 +3155,16 @@
         <v>45296.67059027778</v>
       </c>
       <c r="BM12" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN12" t="b">
         <v>1</v>
       </c>
       <c r="BO12" t="n">
-        <v>91.59</v>
+        <v>274.83</v>
       </c>
       <c r="BP12" t="n">
-        <v>1322.89</v>
+        <v>2568.83</v>
       </c>
       <c r="BQ12" t="inlineStr"/>
       <c r="BR12" t="n">
@@ -3215,22 +3215,22 @@
         <v>1.09442</v>
       </c>
       <c r="L13" t="n">
-        <v>-9.169988816471014e-05</v>
+        <v>-9.169988816469159e-05</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.0001525966927486224</v>
+        <v>-0.0001525966927486039</v>
       </c>
       <c r="N13" t="n">
-        <v>-0.0002370817808695181</v>
+        <v>-0.000237081780869507</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.0002433948348646795</v>
+        <v>-0.0002433948348646684</v>
       </c>
       <c r="P13" t="n">
         <v>1.094786055439249</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.09517534622503</v>
+        <v>1.095175346225029</v>
       </c>
       <c r="R13" s="2" t="n">
         <v>45296.20833333334</v>
@@ -3374,16 +3374,16 @@
         <v>45296.39158564815</v>
       </c>
       <c r="BM13" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN13" t="b">
         <v>1</v>
       </c>
       <c r="BO13" t="n">
-        <v>14.65</v>
+        <v>43.97</v>
       </c>
       <c r="BP13" t="n">
-        <v>1337.54</v>
+        <v>2612.8</v>
       </c>
       <c r="BQ13" t="inlineStr"/>
       <c r="BR13" t="n">
@@ -3434,16 +3434,16 @@
         <v>1.09394</v>
       </c>
       <c r="L14" t="n">
-        <v>1.800098932082572e-05</v>
+        <v>1.800098932084798e-05</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0001215845248809404</v>
+        <v>0.0001215845248809627</v>
       </c>
       <c r="N14" t="n">
-        <v>-7.769775495846668e-05</v>
+        <v>-7.769775495845556e-05</v>
       </c>
       <c r="O14" t="n">
-        <v>5.986598279755665e-05</v>
+        <v>5.986598279756778e-05</v>
       </c>
       <c r="P14" t="n">
         <v>1.09351586998174</v>
@@ -3467,10 +3467,10 @@
         <v>1.094217380952381</v>
       </c>
       <c r="W14" t="n">
-        <v>2.78498694367819e-05</v>
+        <v>2.784986943676417e-05</v>
       </c>
       <c r="X14" t="n">
-        <v>-0.0003415671670448203</v>
+        <v>-0.0003415671670448381</v>
       </c>
       <c r="Y14" t="n">
         <v>1.094871071428572</v>
@@ -3593,16 +3593,16 @@
         <v>45299.16766203703</v>
       </c>
       <c r="BM14" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN14" t="b">
         <v>1</v>
       </c>
       <c r="BO14" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP14" t="n">
-        <v>1352.2</v>
+        <v>2656.79</v>
       </c>
       <c r="BQ14" t="inlineStr"/>
       <c r="BR14" t="n">
@@ -3653,16 +3653,16 @@
         <v>1.093999981197643</v>
       </c>
       <c r="L15" t="n">
-        <v>5.483896472687021e-05</v>
+        <v>5.483896472688504e-05</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0001599464474829571</v>
+        <v>0.0001599464474829719</v>
       </c>
       <c r="N15" t="n">
-        <v>-7.035967669347469e-05</v>
+        <v>-7.035967669345463e-05</v>
       </c>
       <c r="O15" t="n">
-        <v>5.638206634660495e-05</v>
+        <v>5.638206634662503e-05</v>
       </c>
       <c r="P15" t="n">
         <v>1.093573870980823</v>
@@ -3686,10 +3686,10 @@
         <v>1.094217380952381</v>
       </c>
       <c r="W15" t="n">
-        <v>2.78498694367819e-05</v>
+        <v>2.784986943676417e-05</v>
       </c>
       <c r="X15" t="n">
-        <v>-0.0003415671670448203</v>
+        <v>-0.0003415671670448381</v>
       </c>
       <c r="Y15" t="n">
         <v>1.094871071428572</v>
@@ -3812,16 +3812,16 @@
         <v>45299.16766203703</v>
       </c>
       <c r="BM15" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN15" t="b">
         <v>1</v>
       </c>
       <c r="BO15" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP15" t="n">
-        <v>1366.86</v>
+        <v>2700.779999999999</v>
       </c>
       <c r="BQ15" t="inlineStr"/>
       <c r="BR15" t="n">
@@ -3872,16 +3872,16 @@
         <v>1.094331664122122</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0001645395217053621</v>
+        <v>0.0001645395217053732</v>
       </c>
       <c r="M16" t="n">
-        <v>1.675518023385628e-05</v>
+        <v>1.67551802338674e-05</v>
       </c>
       <c r="N16" t="n">
-        <v>8.25439579583799e-05</v>
+        <v>8.254395795839102e-05</v>
       </c>
       <c r="O16" t="n">
-        <v>5.152552583244453e-05</v>
+        <v>5.152552583245565e-05</v>
       </c>
       <c r="P16" t="n">
         <v>1.093645999264471</v>
@@ -3905,10 +3905,10 @@
         <v>1.094217380952381</v>
       </c>
       <c r="W16" t="n">
-        <v>2.78498694367819e-05</v>
+        <v>2.784986943676417e-05</v>
       </c>
       <c r="X16" t="n">
-        <v>-0.0003415671670448203</v>
+        <v>-0.0003415671670448381</v>
       </c>
       <c r="Y16" t="n">
         <v>1.094871071428572</v>
@@ -4031,16 +4031,16 @@
         <v>45299.16256944444</v>
       </c>
       <c r="BM16" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN16" t="b">
         <v>1</v>
       </c>
       <c r="BO16" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP16" t="n">
-        <v>1381.52</v>
+        <v>2744.769999999999</v>
       </c>
       <c r="BQ16" t="inlineStr"/>
       <c r="BR16" t="n">
@@ -4091,16 +4091,16 @@
         <v>1.094339066701666</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0001465291101249623</v>
+        <v>0.0001465291101249919</v>
       </c>
       <c r="M17" t="n">
-        <v>2.769693698910219e-05</v>
+        <v>2.769693698913186e-05</v>
       </c>
       <c r="N17" t="n">
-        <v>0.0001215845248809404</v>
+        <v>0.0001215845248809627</v>
       </c>
       <c r="O17" t="n">
-        <v>1.800098932082572e-05</v>
+        <v>1.800098932084798e-05</v>
       </c>
       <c r="P17" t="n">
         <v>1.093732707893472</v>
@@ -4124,10 +4124,10 @@
         <v>1.093953928571429</v>
       </c>
       <c r="W17" t="n">
-        <v>2.784895217010841e-05</v>
+        <v>2.784895217010334e-05</v>
       </c>
       <c r="X17" t="n">
-        <v>-0.0004537699999650305</v>
+        <v>-0.0004537699999650356</v>
       </c>
       <c r="Y17" t="n">
         <v>1.094217380952381</v>
@@ -4145,10 +4145,10 @@
         <v>1.096625250419115</v>
       </c>
       <c r="AD17" t="n">
-        <v>-0.0003415671670448203</v>
+        <v>-0.0003415671670448381</v>
       </c>
       <c r="AE17" t="n">
-        <v>2.78498694367819e-05</v>
+        <v>2.784986943676417e-05</v>
       </c>
       <c r="AF17" t="n">
         <v>1.094246209619318</v>
@@ -4250,16 +4250,16 @@
         <v>45299.86118055556</v>
       </c>
       <c r="BM17" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN17" t="b">
         <v>1</v>
       </c>
       <c r="BO17" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP17" t="n">
-        <v>1396.18</v>
+        <v>2788.759999999999</v>
       </c>
       <c r="BQ17" t="inlineStr"/>
       <c r="BR17" t="n">
@@ -4310,16 +4310,16 @@
         <v>1.094398154385114</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0002151962591490006</v>
+        <v>0.0002151962591490117</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0001835583583854034</v>
+        <v>0.0001835583583854146</v>
       </c>
       <c r="N18" t="n">
-        <v>0.0001154879926281756</v>
+        <v>0.0001154879926281964</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0002094712637320516</v>
+        <v>0.0002094712637320723</v>
       </c>
       <c r="P18" t="n">
         <v>1.093222555461569</v>
@@ -4469,16 +4469,16 @@
         <v>45299.86111111111</v>
       </c>
       <c r="BM18" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN18" t="b">
         <v>1</v>
       </c>
       <c r="BO18" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP18" t="n">
-        <v>1410.84</v>
+        <v>2832.749999999999</v>
       </c>
       <c r="BQ18" t="inlineStr"/>
       <c r="BR18" t="n">
@@ -4529,16 +4529,16 @@
         <v>1.094693597900951</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0001007867353749572</v>
+        <v>0.0001007867353749831</v>
       </c>
       <c r="M19" t="n">
-        <v>8.71978060889806e-05</v>
+        <v>8.719780608900656e-05</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0002421787871820618</v>
+        <v>0.0002421787871820781</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0002833812103911197</v>
+        <v>0.000283381210391136</v>
       </c>
       <c r="P19" t="n">
         <v>1.09337812157671</v>
@@ -4688,16 +4688,16 @@
         <v>45299.70575231482</v>
       </c>
       <c r="BM19" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN19" t="b">
         <v>1</v>
       </c>
       <c r="BO19" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP19" t="n">
-        <v>1425.5</v>
+        <v>2876.739999999998</v>
       </c>
       <c r="BQ19" t="inlineStr"/>
       <c r="BR19" t="n">
@@ -4748,16 +4748,16 @@
         <v>1.09362666272648</v>
       </c>
       <c r="L20" t="n">
-        <v>3.687107619642627e-05</v>
+        <v>3.687107619644264e-05</v>
       </c>
       <c r="M20" t="n">
-        <v>1.524138289269439e-05</v>
+        <v>1.524138289271076e-05</v>
       </c>
       <c r="N20" t="n">
-        <v>-3.685887644104231e-05</v>
+        <v>-3.685887644101634e-05</v>
       </c>
       <c r="O20" t="n">
-        <v>-1.982308317371669e-05</v>
+        <v>-1.982308317369073e-05</v>
       </c>
       <c r="P20" t="n">
         <v>1.093041396610646</v>
@@ -4907,16 +4907,16 @@
         <v>45299.39787037037</v>
       </c>
       <c r="BM20" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN20" t="b">
         <v>1</v>
       </c>
       <c r="BO20" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP20" t="n">
-        <v>1440.16</v>
+        <v>2920.729999999998</v>
       </c>
       <c r="BQ20" t="inlineStr"/>
       <c r="BR20" t="n">
@@ -4961,22 +4961,22 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>1.093293328600393</v>
+        <v>1.093293328600392</v>
       </c>
       <c r="K21" t="n">
         <v>1.093695469306475</v>
       </c>
       <c r="L21" t="n">
-        <v>-2.896314874937632e-05</v>
+        <v>-2.896314874935036e-05</v>
       </c>
       <c r="M21" t="n">
-        <v>-3.243122297719778e-05</v>
+        <v>-3.243122297717182e-05</v>
       </c>
       <c r="N21" t="n">
-        <v>7.287855792004942e-05</v>
+        <v>7.287855792006425e-05</v>
       </c>
       <c r="O21" t="n">
-        <v>9.978516543921928e-05</v>
+        <v>9.978516543923412e-05</v>
       </c>
       <c r="P21" t="n">
         <v>1.092911620236403</v>
@@ -5126,16 +5126,16 @@
         <v>45299.3978587963</v>
       </c>
       <c r="BM21" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN21" t="b">
         <v>1</v>
       </c>
       <c r="BO21" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP21" t="n">
-        <v>1454.82</v>
+        <v>2964.719999999998</v>
       </c>
       <c r="BQ21" t="inlineStr"/>
       <c r="BR21" t="n">
@@ -5186,16 +5186,16 @@
         <v>1.093565466262465</v>
       </c>
       <c r="L22" t="n">
-        <v>-2.744344210551127e-05</v>
+        <v>-2.74434421054853e-05</v>
       </c>
       <c r="M22" t="n">
-        <v>3.157853218710008e-05</v>
+        <v>3.157853218712605e-05</v>
       </c>
       <c r="N22" t="n">
-        <v>1.524138289269439e-05</v>
+        <v>1.524138289271076e-05</v>
       </c>
       <c r="O22" t="n">
-        <v>3.687107619642627e-05</v>
+        <v>3.687107619644264e-05</v>
       </c>
       <c r="P22" t="n">
         <v>1.093123602198057</v>
@@ -5219,10 +5219,10 @@
         <v>1.093561071428572</v>
       </c>
       <c r="W22" t="n">
-        <v>-0.0003199762793115579</v>
+        <v>-0.0003199762793115593</v>
       </c>
       <c r="X22" t="n">
-        <v>-0.0003611163247181727</v>
+        <v>-0.0003611163247181741</v>
       </c>
       <c r="Y22" t="n">
         <v>1.093680714285714</v>
@@ -5345,16 +5345,16 @@
         <v>45299.37511574074</v>
       </c>
       <c r="BM22" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN22" t="b">
         <v>1</v>
       </c>
       <c r="BO22" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP22" t="n">
-        <v>1469.48</v>
+        <v>3008.709999999998</v>
       </c>
       <c r="BQ22" t="inlineStr"/>
       <c r="BR22" t="n">
@@ -5405,16 +5405,16 @@
         <v>1.0936</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0001189005331077108</v>
+        <v>0.0001189005331077219</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0001185748598529551</v>
+        <v>0.0001185748598529662</v>
       </c>
       <c r="N23" t="n">
-        <v>-3.243122297719778e-05</v>
+        <v>-3.243122297717182e-05</v>
       </c>
       <c r="O23" t="n">
-        <v>-2.896314874937632e-05</v>
+        <v>-2.896314874935036e-05</v>
       </c>
       <c r="P23" t="n">
         <v>1.093290497385453</v>
@@ -5438,10 +5438,10 @@
         <v>1.093561071428572</v>
       </c>
       <c r="W23" t="n">
-        <v>-0.0003199762793115579</v>
+        <v>-0.0003199762793115593</v>
       </c>
       <c r="X23" t="n">
-        <v>-0.0003611163247181727</v>
+        <v>-0.0003611163247181741</v>
       </c>
       <c r="Y23" t="n">
         <v>1.093680714285714</v>
@@ -5564,16 +5564,16 @@
         <v>45299.39787037037</v>
       </c>
       <c r="BM23" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN23" t="b">
         <v>1</v>
       </c>
       <c r="BO23" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP23" t="n">
-        <v>1484.140000000001</v>
+        <v>3052.699999999998</v>
       </c>
       <c r="BQ23" t="inlineStr"/>
       <c r="BR23" t="n">
@@ -5624,16 +5624,16 @@
         <v>1.093759997546536</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0001924139507230765</v>
+        <v>0.0001924139507230891</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0002422259383578991</v>
+        <v>0.0002422259383579118</v>
       </c>
       <c r="N24" t="n">
-        <v>3.157853218710008e-05</v>
+        <v>3.157853218712605e-05</v>
       </c>
       <c r="O24" t="n">
-        <v>-2.744344210551127e-05</v>
+        <v>-2.74434421054853e-05</v>
       </c>
       <c r="P24" t="n">
         <v>1.093217315471899</v>
@@ -5657,10 +5657,10 @@
         <v>1.093561071428572</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.0003199762793115579</v>
+        <v>-0.0003199762793115593</v>
       </c>
       <c r="X24" t="n">
-        <v>-0.0003611163247181727</v>
+        <v>-0.0003611163247181741</v>
       </c>
       <c r="Y24" t="n">
         <v>1.093680714285714</v>
@@ -5783,16 +5783,16 @@
         <v>45299.38880787037</v>
       </c>
       <c r="BM24" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN24" t="b">
         <v>1</v>
       </c>
       <c r="BO24" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP24" t="n">
-        <v>1498.800000000001</v>
+        <v>3096.689999999997</v>
       </c>
       <c r="BQ24" t="inlineStr"/>
       <c r="BR24" t="n">
@@ -5843,16 +5843,16 @@
         <v>1.094121680698759</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0001924203948790484</v>
+        <v>0.000192420394879078</v>
       </c>
       <c r="M25" t="n">
-        <v>0.0001538278223032183</v>
+        <v>0.000153827822303248</v>
       </c>
       <c r="N25" t="n">
-        <v>0.0001185748598529551</v>
+        <v>0.0001185748598529662</v>
       </c>
       <c r="O25" t="n">
-        <v>0.0001189005331077108</v>
+        <v>0.0001189005331077219</v>
       </c>
       <c r="P25" t="n">
         <v>1.093041701594922</v>
@@ -5897,10 +5897,10 @@
         <v>1.09521458675974</v>
       </c>
       <c r="AD25" t="n">
-        <v>-0.0003611163247181727</v>
+        <v>-0.0003611163247181741</v>
       </c>
       <c r="AE25" t="n">
-        <v>-0.0003199762793115579</v>
+        <v>-0.0003199762793115593</v>
       </c>
       <c r="AF25" t="n">
         <v>1.094198955374123</v>
@@ -6002,16 +6002,16 @@
         <v>45299.3868287037</v>
       </c>
       <c r="BM25" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN25" t="b">
         <v>1</v>
       </c>
       <c r="BO25" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP25" t="n">
-        <v>1513.460000000001</v>
+        <v>3140.679999999997</v>
       </c>
       <c r="BQ25" t="inlineStr"/>
       <c r="BR25" t="n">
@@ -6062,16 +6062,16 @@
         <v>1.094279119107935</v>
       </c>
       <c r="L26" t="n">
-        <v>6.369896866889888e-05</v>
+        <v>6.369896866890999e-05</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0002682211871544195</v>
+        <v>0.0002682211871544305</v>
       </c>
       <c r="N26" t="n">
-        <v>0.0002373996167340236</v>
+        <v>0.0002373996167340496</v>
       </c>
       <c r="O26" t="n">
-        <v>0.0002057577608285906</v>
+        <v>0.0002057577608286166</v>
       </c>
       <c r="P26" t="n">
         <v>1.093140331974908</v>
@@ -6116,10 +6116,10 @@
         <v>1.09521458675974</v>
       </c>
       <c r="AD26" t="n">
-        <v>-0.0003611163247181727</v>
+        <v>-0.0003611163247181741</v>
       </c>
       <c r="AE26" t="n">
-        <v>-0.0003199762793115579</v>
+        <v>-0.0003199762793115593</v>
       </c>
       <c r="AF26" t="n">
         <v>1.094198955374123</v>
@@ -6221,16 +6221,16 @@
         <v>45299.86123842592</v>
       </c>
       <c r="BM26" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN26" t="b">
         <v>1</v>
       </c>
       <c r="BO26" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP26" t="n">
-        <v>1528.120000000001</v>
+        <v>3184.669999999997</v>
       </c>
       <c r="BQ26" t="inlineStr"/>
       <c r="BR26" t="n">
@@ -6281,16 +6281,16 @@
         <v>1.095248353735171</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.0001160558362192084</v>
+        <v>-0.0001160558362191825</v>
       </c>
       <c r="M27" t="n">
-        <v>-8.067330008922471e-05</v>
+        <v>-8.067330008919878e-05</v>
       </c>
       <c r="N27" t="n">
-        <v>0.0001538278223032183</v>
+        <v>0.000153827822303248</v>
       </c>
       <c r="O27" t="n">
-        <v>0.0001924203948790484</v>
+        <v>0.000192420394879078</v>
       </c>
       <c r="P27" t="n">
         <v>1.093589002983599</v>
@@ -6335,10 +6335,10 @@
         <v>1.09521458675974</v>
       </c>
       <c r="AD27" t="n">
-        <v>-0.0003611163247181727</v>
+        <v>-0.0003611163247181741</v>
       </c>
       <c r="AE27" t="n">
-        <v>-0.0003199762793115579</v>
+        <v>-0.0003199762793115593</v>
       </c>
       <c r="AF27" t="n">
         <v>1.094198955374123</v>
@@ -6440,16 +6440,16 @@
         <v>45299.70601851852</v>
       </c>
       <c r="BM27" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN27" t="b">
         <v>1</v>
       </c>
       <c r="BO27" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP27" t="n">
-        <v>1542.780000000001</v>
+        <v>3228.659999999997</v>
       </c>
       <c r="BQ27" t="inlineStr"/>
       <c r="BR27" t="n">
@@ -6500,16 +6500,16 @@
         <v>1.095638573347635</v>
       </c>
       <c r="L28" t="n">
-        <v>9.563114742288485e-06</v>
+        <v>9.563114742310739e-06</v>
       </c>
       <c r="M28" t="n">
-        <v>-3.607630203588998e-05</v>
+        <v>-3.607630203586772e-05</v>
       </c>
       <c r="N28" t="n">
-        <v>-0.0001827854208349958</v>
+        <v>-0.0001827854208349736</v>
       </c>
       <c r="O28" t="n">
-        <v>-7.756567496636651e-05</v>
+        <v>-7.756567496634426e-05</v>
       </c>
       <c r="P28" t="n">
         <v>1.095027200624277</v>
@@ -6659,16 +6659,16 @@
         <v>45300.24388888889</v>
       </c>
       <c r="BM28" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN28" t="b">
         <v>1</v>
       </c>
       <c r="BO28" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP28" t="n">
-        <v>1557.440000000001</v>
+        <v>3272.649999999996</v>
       </c>
       <c r="BQ28" t="inlineStr"/>
       <c r="BR28" t="n">
@@ -6719,16 +6719,16 @@
         <v>1.095720045085652</v>
       </c>
       <c r="L29" t="n">
-        <v>-3.624972089705441e-05</v>
+        <v>-3.624972089704327e-05</v>
       </c>
       <c r="M29" t="n">
-        <v>-9.129309527565865e-05</v>
+        <v>-9.129309527564751e-05</v>
       </c>
       <c r="N29" t="n">
-        <v>-0.0001219623907828859</v>
+        <v>-0.0001219623907828599</v>
       </c>
       <c r="O29" t="n">
-        <v>8.176172185259821e-05</v>
+        <v>8.176172185262418e-05</v>
       </c>
       <c r="P29" t="n">
         <v>1.094809585735438</v>
@@ -6878,16 +6878,16 @@
         <v>45301.75846064815</v>
       </c>
       <c r="BM29" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN29" t="b">
         <v>1</v>
       </c>
       <c r="BO29" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP29" t="n">
-        <v>1572.100000000001</v>
+        <v>3316.639999999996</v>
       </c>
       <c r="BQ29" t="inlineStr"/>
       <c r="BR29" t="n">
@@ -6938,16 +6938,16 @@
         <v>1.09573339108126</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.000117862977768851</v>
+        <v>-0.0001178629777688287</v>
       </c>
       <c r="M30" t="n">
-        <v>-0.0001947662308731603</v>
+        <v>-0.000194766230873138</v>
       </c>
       <c r="N30" t="n">
-        <v>3.043032568696051e-05</v>
+        <v>3.043032568699018e-05</v>
       </c>
       <c r="O30" t="n">
-        <v>9.174943842120116e-05</v>
+        <v>9.174943842123083e-05</v>
       </c>
       <c r="P30" t="n">
         <v>1.094889161676116</v>
@@ -7097,16 +7097,16 @@
         <v>45301.7578587963</v>
       </c>
       <c r="BM30" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN30" t="b">
         <v>1</v>
       </c>
       <c r="BO30" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP30" t="n">
-        <v>1586.760000000001</v>
+        <v>3360.629999999996</v>
       </c>
       <c r="BQ30" t="inlineStr"/>
       <c r="BR30" t="n">
@@ -7157,16 +7157,16 @@
         <v>1.09514863543961</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.0006403038162890631</v>
+        <v>-0.0006403038162890519</v>
       </c>
       <c r="M31" t="n">
-        <v>-0.0006755405133144737</v>
+        <v>-0.0006755405133144624</v>
       </c>
       <c r="N31" t="n">
-        <v>-0.0001263533251140032</v>
+        <v>-0.000126353325113981</v>
       </c>
       <c r="O31" t="n">
-        <v>-2.77105406614553e-06</v>
+        <v>-2.771054066123277e-06</v>
       </c>
       <c r="P31" t="n">
         <v>1.093829727465642</v>
@@ -7211,10 +7211,10 @@
         <v>1.094746974458865</v>
       </c>
       <c r="AD31" t="n">
-        <v>7.056829962460279e-05</v>
+        <v>7.056829962462052e-05</v>
       </c>
       <c r="AE31" t="n">
-        <v>0.0001399353254739333</v>
+        <v>0.0001399353254739511</v>
       </c>
       <c r="AF31" t="n">
         <v>1.092618177893134</v>
@@ -7314,16 +7314,16 @@
         <v>45300.78858796296</v>
       </c>
       <c r="BM31" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN31" t="b">
         <v>1</v>
       </c>
       <c r="BO31" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP31" t="n">
-        <v>1601.420000000001</v>
+        <v>3404.599999999996</v>
       </c>
       <c r="BQ31" t="inlineStr"/>
       <c r="BR31" t="n">
@@ -7374,16 +7374,16 @@
         <v>1.09442</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.0008058192201629285</v>
+        <v>-0.00080581922016291</v>
       </c>
       <c r="M32" t="n">
-        <v>-0.0006954670460662145</v>
+        <v>-0.0006954670460661958</v>
       </c>
       <c r="N32" t="n">
-        <v>-0.0001915516331722961</v>
+        <v>-0.0001915516331722909</v>
       </c>
       <c r="O32" t="n">
-        <v>-0.0002244265463311688</v>
+        <v>-0.0002244265463311636</v>
       </c>
       <c r="P32" t="n">
         <v>1.094164464865518</v>
@@ -7428,10 +7428,10 @@
         <v>1.094746974458865</v>
       </c>
       <c r="AD32" t="n">
-        <v>7.056829962460279e-05</v>
+        <v>7.056829962462052e-05</v>
       </c>
       <c r="AE32" t="n">
-        <v>0.0001399353254739333</v>
+        <v>0.0001399353254739511</v>
       </c>
       <c r="AF32" t="n">
         <v>1.092618177893134</v>
@@ -7531,16 +7531,16 @@
         <v>45300.77583333333</v>
       </c>
       <c r="BM32" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN32" t="b">
         <v>1</v>
       </c>
       <c r="BO32" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP32" t="n">
-        <v>1616.080000000001</v>
+        <v>3448.569999999996</v>
       </c>
       <c r="BQ32" t="inlineStr"/>
       <c r="BR32" t="n">
@@ -7591,16 +7591,16 @@
         <v>1.09367</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.0005815679933305868</v>
+        <v>-0.0005815679933305645</v>
       </c>
       <c r="M33" t="n">
-        <v>-0.0002868969213305711</v>
+        <v>-0.0002868969213305489</v>
       </c>
       <c r="N33" t="n">
-        <v>-0.0001934497241419134</v>
+        <v>-0.0001934497241419061</v>
       </c>
       <c r="O33" t="n">
-        <v>-0.0003442420061110125</v>
+        <v>-0.0003442420061110052</v>
       </c>
       <c r="P33" t="n">
         <v>1.093896585334983</v>
@@ -7645,10 +7645,10 @@
         <v>1.094746974458865</v>
       </c>
       <c r="AD33" t="n">
-        <v>7.056829962460279e-05</v>
+        <v>7.056829962462052e-05</v>
       </c>
       <c r="AE33" t="n">
-        <v>0.0001399353254739333</v>
+        <v>0.0001399353254739511</v>
       </c>
       <c r="AF33" t="n">
         <v>1.092618177893134</v>
@@ -7748,16 +7748,16 @@
         <v>45300.75185185186</v>
       </c>
       <c r="BM33" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN33" t="b">
         <v>1</v>
       </c>
       <c r="BO33" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP33" t="n">
-        <v>1630.740000000001</v>
+        <v>3492.539999999995</v>
       </c>
       <c r="BQ33" t="inlineStr"/>
       <c r="BR33" t="n">
@@ -7808,16 +7808,16 @@
         <v>1.09283</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0003435228761054585</v>
+        <v>0.0003435228761054734</v>
       </c>
       <c r="M34" t="n">
-        <v>2.412293530591065e-05</v>
+        <v>2.412293530592547e-05</v>
       </c>
       <c r="N34" t="n">
-        <v>-0.0006755405133144737</v>
+        <v>-0.0006755405133144624</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.0006403038162890631</v>
+        <v>-0.0006403038162890519</v>
       </c>
       <c r="P34" t="n">
         <v>1.093748541090671</v>
@@ -7862,10 +7862,10 @@
         <v>1.094746974458865</v>
       </c>
       <c r="AD34" t="n">
-        <v>7.056829962460279e-05</v>
+        <v>7.056829962462052e-05</v>
       </c>
       <c r="AE34" t="n">
-        <v>0.0001399353254739333</v>
+        <v>0.0001399353254739511</v>
       </c>
       <c r="AF34" t="n">
         <v>1.092618177893134</v>
@@ -7959,7 +7959,7 @@
       <c r="BK34" t="inlineStr"/>
       <c r="BL34" t="inlineStr"/>
       <c r="BM34" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN34" t="b">
         <v>0</v>
@@ -7968,7 +7968,7 @@
         <v>0</v>
       </c>
       <c r="BP34" t="n">
-        <v>1630.740000000001</v>
+        <v>3492.539999999995</v>
       </c>
       <c r="BQ34" s="2" t="n">
         <v>45300.86458333334</v>
@@ -8021,16 +8021,16 @@
         <v>1.093966613142731</v>
       </c>
       <c r="L35" t="n">
-        <v>-8.213300119571091e-05</v>
+        <v>-8.213300119569977e-05</v>
       </c>
       <c r="M35" t="n">
-        <v>0.000225452780854009</v>
+        <v>0.0002254527808540201</v>
       </c>
       <c r="N35" t="n">
-        <v>8.814554379891707e-05</v>
+        <v>8.81455437989319e-05</v>
       </c>
       <c r="O35" t="n">
-        <v>8.655188842349919e-05</v>
+        <v>8.655188842351401e-05</v>
       </c>
       <c r="P35" t="n">
         <v>1.092214792814043</v>
@@ -8182,16 +8182,16 @@
         <v>45301.66534722222</v>
       </c>
       <c r="BM35" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN35" t="b">
         <v>1</v>
       </c>
       <c r="BO35" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP35" t="n">
-        <v>1645.400000000001</v>
+        <v>3536.529999999995</v>
       </c>
       <c r="BQ35" t="inlineStr"/>
       <c r="BR35" t="n">
@@ -8242,16 +8242,16 @@
         <v>1.094620489071821</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.0002242252333959542</v>
+        <v>-0.0002242252333959283</v>
       </c>
       <c r="M36" t="n">
-        <v>-0.0001466269266115309</v>
+        <v>-0.000146626926611505</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0003289604077041182</v>
+        <v>0.0003289604077041293</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0001754285029585236</v>
+        <v>0.0001754285029585347</v>
       </c>
       <c r="P36" t="n">
         <v>1.092123959621022</v>
@@ -8403,16 +8403,16 @@
         <v>45301.52954861111</v>
       </c>
       <c r="BM36" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN36" t="b">
         <v>1</v>
       </c>
       <c r="BO36" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP36" t="n">
-        <v>1660.060000000002</v>
+        <v>3580.519999999995</v>
       </c>
       <c r="BQ36" t="inlineStr"/>
       <c r="BR36" t="n">
@@ -8463,16 +8463,16 @@
         <v>1.093936648842046</v>
       </c>
       <c r="L37" t="n">
-        <v>0.0004699312214960206</v>
+        <v>0.0004699312214960354</v>
       </c>
       <c r="M37" t="n">
-        <v>0.0001950116177921601</v>
+        <v>0.0001950116177921749</v>
       </c>
       <c r="N37" t="n">
-        <v>0.000225452780854009</v>
+        <v>0.0002254527808540201</v>
       </c>
       <c r="O37" t="n">
-        <v>-8.213300119571091e-05</v>
+        <v>-8.213300119569977e-05</v>
       </c>
       <c r="P37" t="n">
         <v>1.092482019084543</v>
@@ -8496,10 +8496,10 @@
         <v>1.09319119047619</v>
       </c>
       <c r="W37" t="n">
-        <v>-4.161634156853066e-05</v>
+        <v>-4.161634156852304e-05</v>
       </c>
       <c r="X37" t="n">
-        <v>0.0003750924659700856</v>
+        <v>0.0003750924659700932</v>
       </c>
       <c r="Y37" t="n">
         <v>1.092739285714285</v>
@@ -8624,16 +8624,16 @@
         <v>45301.43761574074</v>
       </c>
       <c r="BM37" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN37" t="b">
         <v>1</v>
       </c>
       <c r="BO37" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP37" t="n">
-        <v>1674.720000000002</v>
+        <v>3624.509999999995</v>
       </c>
       <c r="BQ37" t="inlineStr"/>
       <c r="BR37" t="n">
@@ -8684,19 +8684,19 @@
         <v>1.09415</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0003599733784138874</v>
+        <v>0.0003599733784138985</v>
       </c>
       <c r="M38" t="n">
-        <v>0.0002037752671927053</v>
+        <v>0.0002037752671927164</v>
       </c>
       <c r="N38" t="n">
-        <v>-0.0001466269266115309</v>
+        <v>-0.000146626926611505</v>
       </c>
       <c r="O38" t="n">
-        <v>-0.0002242252333959542</v>
+        <v>-0.0002242252333959283</v>
       </c>
       <c r="P38" t="n">
-        <v>1.092677893478819</v>
+        <v>1.092677893478818</v>
       </c>
       <c r="Q38" t="n">
         <v>1.094606065257322</v>
@@ -8717,10 +8717,10 @@
         <v>1.09319119047619</v>
       </c>
       <c r="W38" t="n">
-        <v>-4.161634156853066e-05</v>
+        <v>-4.161634156852304e-05</v>
       </c>
       <c r="X38" t="n">
-        <v>0.0003750924659700856</v>
+        <v>0.0003750924659700932</v>
       </c>
       <c r="Y38" t="n">
         <v>1.092739285714285</v>
@@ -8843,16 +8843,16 @@
         <v>45301.52885416667</v>
       </c>
       <c r="BM38" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN38" t="b">
         <v>1</v>
       </c>
       <c r="BO38" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP38" t="n">
-        <v>1689.380000000002</v>
+        <v>3668.499999999995</v>
       </c>
       <c r="BQ38" t="inlineStr"/>
       <c r="BR38" t="n">
@@ -8903,16 +8903,16 @@
         <v>1.094668641646441</v>
       </c>
       <c r="L39" t="n">
-        <v>0.000286627948482661</v>
+        <v>0.0002866279484826721</v>
       </c>
       <c r="M39" t="n">
-        <v>0.0001374130669863471</v>
+        <v>0.0001374130669863582</v>
       </c>
       <c r="N39" t="n">
-        <v>0.0001950116177921601</v>
+        <v>0.0001950116177921749</v>
       </c>
       <c r="O39" t="n">
-        <v>0.0004699312214960206</v>
+        <v>0.0004699312214960354</v>
       </c>
       <c r="P39" t="n">
         <v>1.092256244288922</v>
@@ -8936,10 +8936,10 @@
         <v>1.09319119047619</v>
       </c>
       <c r="W39" t="n">
-        <v>-4.161634156853066e-05</v>
+        <v>-4.161634156852304e-05</v>
       </c>
       <c r="X39" t="n">
-        <v>0.0003750924659700856</v>
+        <v>0.0003750924659700932</v>
       </c>
       <c r="Y39" t="n">
         <v>1.092739285714285</v>
@@ -9062,16 +9062,16 @@
         <v>45301.55368055555</v>
       </c>
       <c r="BM39" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN39" t="b">
         <v>1</v>
       </c>
       <c r="BO39" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP39" t="n">
-        <v>1704.040000000002</v>
+        <v>3712.489999999994</v>
       </c>
       <c r="BQ39" t="inlineStr"/>
       <c r="BR39" t="n">
@@ -9122,16 +9122,16 @@
         <v>1.093949275049066</v>
       </c>
       <c r="L40" t="n">
-        <v>0.0005160229926786801</v>
+        <v>0.0005160229926786912</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0007671974318361747</v>
+        <v>0.0007671974318361859</v>
       </c>
       <c r="N40" t="n">
-        <v>-4.293934864932879e-05</v>
+        <v>-4.293934864931395e-05</v>
       </c>
       <c r="O40" t="n">
-        <v>-0.0001014655067608644</v>
+        <v>-0.0001014655067608495</v>
       </c>
       <c r="P40" t="n">
         <v>1.093462838000153</v>
@@ -9283,16 +9283,16 @@
         <v>45302.64716435185</v>
       </c>
       <c r="BM40" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN40" t="b">
         <v>1</v>
       </c>
       <c r="BO40" t="n">
-        <v>91.62</v>
+        <v>274.96</v>
       </c>
       <c r="BP40" t="n">
-        <v>1795.660000000002</v>
+        <v>3987.449999999994</v>
       </c>
       <c r="BQ40" t="inlineStr"/>
       <c r="BR40" t="n">
@@ -9343,16 +9343,16 @@
         <v>1.094619128587409</v>
       </c>
       <c r="L41" t="n">
-        <v>0.0006395176794942715</v>
+        <v>0.00063951767949429</v>
       </c>
       <c r="M41" t="n">
-        <v>0.0008447268660506705</v>
+        <v>0.0008447268660506891</v>
       </c>
       <c r="N41" t="n">
-        <v>0.0002196074347078186</v>
+        <v>0.0002196074347078334</v>
       </c>
       <c r="O41" t="n">
-        <v>-6.097890499599546e-05</v>
+        <v>-6.097890499598063e-05</v>
       </c>
       <c r="P41" t="n">
         <v>1.093267311360706</v>
@@ -9502,16 +9502,16 @@
         <v>45301.77608796296</v>
       </c>
       <c r="BM41" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN41" t="b">
         <v>1</v>
       </c>
       <c r="BO41" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP41" t="n">
-        <v>1810.320000000002</v>
+        <v>4031.439999999994</v>
       </c>
       <c r="BQ41" t="inlineStr"/>
       <c r="BR41" t="n">
@@ -9562,16 +9562,16 @@
         <v>1.096006553956496</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0006714367380369944</v>
+        <v>0.000671436738037013</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0004227603251399778</v>
+        <v>0.0004227603251399964</v>
       </c>
       <c r="N42" t="n">
-        <v>0.0002965662372695397</v>
+        <v>0.0002965662372695509</v>
       </c>
       <c r="O42" t="n">
-        <v>0.0003392443626411938</v>
+        <v>0.000339244362641205</v>
       </c>
       <c r="P42" t="n">
         <v>1.092802747391172</v>
@@ -9721,16 +9721,16 @@
         <v>45301.77457175926</v>
       </c>
       <c r="BM42" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN42" t="b">
         <v>1</v>
       </c>
       <c r="BO42" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP42" t="n">
-        <v>1824.980000000002</v>
+        <v>4075.429999999994</v>
       </c>
       <c r="BQ42" t="inlineStr"/>
       <c r="BR42" t="n">
@@ -9781,16 +9781,16 @@
         <v>1.09679806625941</v>
       </c>
       <c r="L43" t="n">
-        <v>0.0003046273073458498</v>
+        <v>0.0003046273073458795</v>
       </c>
       <c r="M43" t="n">
-        <v>1.911607080493514e-05</v>
+        <v>1.911607080496482e-05</v>
       </c>
       <c r="N43" t="n">
-        <v>0.0007671974318361747</v>
+        <v>0.0007671974318361859</v>
       </c>
       <c r="O43" t="n">
-        <v>0.0005160229926786801</v>
+        <v>0.0005160229926786912</v>
       </c>
       <c r="P43" t="n">
         <v>1.0929985821775</v>
@@ -9940,16 +9940,16 @@
         <v>45302.46142361111</v>
       </c>
       <c r="BM43" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN43" t="b">
         <v>1</v>
       </c>
       <c r="BO43" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP43" t="n">
-        <v>1839.640000000002</v>
+        <v>4119.419999999994</v>
       </c>
       <c r="BQ43" t="inlineStr"/>
       <c r="BR43" t="n">
@@ -10000,16 +10000,16 @@
         <v>1.097236898269688</v>
       </c>
       <c r="L44" t="n">
-        <v>-0.0003313283486469271</v>
+        <v>-0.0003313283486469012</v>
       </c>
       <c r="M44" t="n">
-        <v>-0.0003617906686222876</v>
+        <v>-0.0003617906686222616</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0008447268660506705</v>
+        <v>0.0008447268660506891</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0006395176794942715</v>
+        <v>0.00063951767949429</v>
       </c>
       <c r="P44" t="n">
         <v>1.093305329726291</v>
@@ -10159,16 +10159,16 @@
         <v>45302.14809027778</v>
       </c>
       <c r="BM44" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN44" t="b">
         <v>1</v>
       </c>
       <c r="BO44" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP44" t="n">
-        <v>1854.300000000002</v>
+        <v>4163.409999999993</v>
       </c>
       <c r="BQ44" t="inlineStr"/>
       <c r="BR44" t="n">
@@ -10219,16 +10219,16 @@
         <v>1.096360001220172</v>
       </c>
       <c r="L45" t="n">
-        <v>0.0001505068231492556</v>
+        <v>0.0001505068231492815</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0001459156157301483</v>
+        <v>0.0001459156157301742</v>
       </c>
       <c r="N45" t="n">
-        <v>0.0003041324105882984</v>
+        <v>0.000304132410588317</v>
       </c>
       <c r="O45" t="n">
-        <v>0.0003103056322578072</v>
+        <v>0.0003103056322578257</v>
       </c>
       <c r="P45" t="n">
         <v>1.095101355488038</v>
@@ -10252,10 +10252,10 @@
         <v>1.095503928571429</v>
       </c>
       <c r="W45" t="n">
-        <v>0.000244794182467222</v>
+        <v>0.000244794182467217</v>
       </c>
       <c r="X45" t="n">
-        <v>0.0003557423958889447</v>
+        <v>0.0003557423958889396</v>
       </c>
       <c r="Y45" t="n">
         <v>1.094983333333334</v>
@@ -10378,16 +10378,16 @@
         <v>45306.59368055555</v>
       </c>
       <c r="BM45" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN45" t="b">
         <v>1</v>
       </c>
       <c r="BO45" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP45" t="n">
-        <v>1868.960000000002</v>
+        <v>4207.379999999994</v>
       </c>
       <c r="BQ45" t="inlineStr"/>
       <c r="BR45" t="n">
@@ -10438,16 +10438,16 @@
         <v>1.096706670008613</v>
       </c>
       <c r="L46" t="n">
-        <v>-0.0001044746927127453</v>
+        <v>-0.0001044746927127305</v>
       </c>
       <c r="M46" t="n">
-        <v>-5.319390227458066e-05</v>
+        <v>-5.319390227456582e-05</v>
       </c>
       <c r="N46" t="n">
-        <v>0.0001459156157301483</v>
+        <v>0.0001459156157301742</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0001505068231492556</v>
+        <v>0.0001505068231492815</v>
       </c>
       <c r="P46" t="n">
         <v>1.095960232955968</v>
@@ -10492,10 +10492,10 @@
         <v>1.094965858940674</v>
       </c>
       <c r="AD46" t="n">
-        <v>0.0003557423958889447</v>
+        <v>0.0003557423958889396</v>
       </c>
       <c r="AE46" t="n">
-        <v>0.000244794182467222</v>
+        <v>0.000244794182467217</v>
       </c>
       <c r="AF46" t="n">
         <v>1.096250211418649</v>
@@ -10597,16 +10597,16 @@
         <v>45306.41700231482</v>
       </c>
       <c r="BM46" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN46" t="b">
         <v>1</v>
       </c>
       <c r="BO46" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP46" t="n">
-        <v>1883.620000000002</v>
+        <v>4251.349999999994</v>
       </c>
       <c r="BQ46" t="inlineStr"/>
       <c r="BR46" t="n">
@@ -10657,16 +10657,16 @@
         <v>1.096778638112405</v>
       </c>
       <c r="L47" t="n">
-        <v>-0.0001365743121868875</v>
+        <v>-0.000136574312186869</v>
       </c>
       <c r="M47" t="n">
-        <v>-0.0001819879672668422</v>
+        <v>-0.0001819879672668236</v>
       </c>
       <c r="N47" t="n">
-        <v>-9.996058060133494e-06</v>
+        <v>-9.996058060117121e-06</v>
       </c>
       <c r="O47" t="n">
-        <v>5.806474138419917e-05</v>
+        <v>5.806474138421554e-05</v>
       </c>
       <c r="P47" t="n">
         <v>1.096115862073164</v>
@@ -10711,10 +10711,10 @@
         <v>1.094965858940674</v>
       </c>
       <c r="AD47" t="n">
-        <v>0.0003557423958889447</v>
+        <v>0.0003557423958889396</v>
       </c>
       <c r="AE47" t="n">
-        <v>0.000244794182467222</v>
+        <v>0.000244794182467217</v>
       </c>
       <c r="AF47" t="n">
         <v>1.096250211418649</v>
@@ -10816,16 +10816,16 @@
         <v>45306.41700231482</v>
       </c>
       <c r="BM47" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN47" t="b">
         <v>1</v>
       </c>
       <c r="BO47" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP47" t="n">
-        <v>1898.280000000002</v>
+        <v>4295.319999999994</v>
       </c>
       <c r="BQ47" t="inlineStr"/>
       <c r="BR47" t="n">
@@ -10876,16 +10876,16 @@
         <v>1.09659</v>
       </c>
       <c r="L48" t="n">
-        <v>-0.0001839923600832325</v>
+        <v>-0.0001839923600832102</v>
       </c>
       <c r="M48" t="n">
-        <v>-0.0001614257019392583</v>
+        <v>-0.000161425701939236</v>
       </c>
       <c r="N48" t="n">
-        <v>-3.60379597469401e-05</v>
+        <v>-3.603795974691414e-05</v>
       </c>
       <c r="O48" t="n">
-        <v>-5.4289861030031e-05</v>
+        <v>-5.428986103000504e-05</v>
       </c>
       <c r="P48" t="n">
         <v>1.096414524565379</v>
@@ -10930,10 +10930,10 @@
         <v>1.094965858940674</v>
       </c>
       <c r="AD48" t="n">
-        <v>0.0003557423958889447</v>
+        <v>0.0003557423958889396</v>
       </c>
       <c r="AE48" t="n">
-        <v>0.000244794182467222</v>
+        <v>0.000244794182467217</v>
       </c>
       <c r="AF48" t="n">
         <v>1.096250211418649</v>
@@ -11035,16 +11035,16 @@
         <v>45306.41686342593</v>
       </c>
       <c r="BM48" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN48" t="b">
         <v>1</v>
       </c>
       <c r="BO48" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP48" t="n">
-        <v>1912.940000000002</v>
+        <v>4339.289999999995</v>
       </c>
       <c r="BQ48" t="inlineStr"/>
       <c r="BR48" t="n">
@@ -11095,16 +11095,16 @@
         <v>1.09638</v>
       </c>
       <c r="L49" t="n">
-        <v>-3.737229806377704e-05</v>
+        <v>-3.737229806376591e-05</v>
       </c>
       <c r="M49" t="n">
-        <v>-4.89363987682059e-05</v>
+        <v>-4.893639876819477e-05</v>
       </c>
       <c r="N49" t="n">
-        <v>-5.319390227458066e-05</v>
+        <v>-5.319390227456582e-05</v>
       </c>
       <c r="O49" t="n">
-        <v>-0.0001044746927127453</v>
+        <v>-0.0001044746927127305</v>
       </c>
       <c r="P49" t="n">
         <v>1.096394027895432</v>
@@ -11128,10 +11128,10 @@
         <v>1.096172023809523</v>
       </c>
       <c r="W49" t="n">
-        <v>0.000404330496264879</v>
+        <v>0.0004043304962648714</v>
       </c>
       <c r="X49" t="n">
-        <v>0.000293815122697147</v>
+        <v>0.0002938151226971394</v>
       </c>
       <c r="Y49" t="n">
         <v>1.095915952380952</v>
@@ -11254,16 +11254,16 @@
         <v>45306.59296296296</v>
       </c>
       <c r="BM49" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN49" t="b">
         <v>1</v>
       </c>
       <c r="BO49" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP49" t="n">
-        <v>1927.600000000002</v>
+        <v>4383.259999999995</v>
       </c>
       <c r="BQ49" t="inlineStr"/>
       <c r="BR49" t="n">
@@ -11314,16 +11314,16 @@
         <v>1.09618</v>
       </c>
       <c r="L50" t="n">
-        <v>0.0001368621009930009</v>
+        <v>0.000136862100993021</v>
       </c>
       <c r="M50" t="n">
-        <v>3.619704912588819e-05</v>
+        <v>3.619704912590828e-05</v>
       </c>
       <c r="N50" t="n">
-        <v>-0.0001819879672668422</v>
+        <v>-0.0001819879672668236</v>
       </c>
       <c r="O50" t="n">
-        <v>-0.0001365743121868875</v>
+        <v>-0.000136574312186869</v>
       </c>
       <c r="P50" t="n">
         <v>1.096276295703993</v>
@@ -11347,10 +11347,10 @@
         <v>1.096172023809523</v>
       </c>
       <c r="W50" t="n">
-        <v>0.000404330496264879</v>
+        <v>0.0004043304962648714</v>
       </c>
       <c r="X50" t="n">
-        <v>0.000293815122697147</v>
+        <v>0.0002938151226971394</v>
       </c>
       <c r="Y50" t="n">
         <v>1.095915952380952</v>
@@ -11473,16 +11473,16 @@
         <v>45306.59012731481</v>
       </c>
       <c r="BM50" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN50" t="b">
         <v>1</v>
       </c>
       <c r="BO50" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP50" t="n">
-        <v>1942.260000000002</v>
+        <v>4427.229999999995</v>
       </c>
       <c r="BQ50" t="inlineStr"/>
       <c r="BR50" t="n">
@@ -11527,22 +11527,22 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>1.096030951107922</v>
+        <v>1.096030951107921</v>
       </c>
       <c r="K51" t="n">
         <v>1.096423331723136</v>
       </c>
       <c r="L51" t="n">
-        <v>4.836765876699152e-05</v>
+        <v>4.836765876700635e-05</v>
       </c>
       <c r="M51" t="n">
-        <v>5.168333328438203e-05</v>
+        <v>5.168333328439686e-05</v>
       </c>
       <c r="N51" t="n">
-        <v>8.210155514622798e-05</v>
+        <v>8.210155514623911e-05</v>
       </c>
       <c r="O51" t="n">
-        <v>7.024534684101715e-05</v>
+        <v>7.024534684102826e-05</v>
       </c>
       <c r="P51" t="n">
         <v>1.095807070838416</v>
@@ -11566,10 +11566,10 @@
         <v>1.096358928571429</v>
       </c>
       <c r="W51" t="n">
-        <v>0.0002603804570156963</v>
+        <v>0.0002603804570156887</v>
       </c>
       <c r="X51" t="n">
-        <v>0.0001660499423528917</v>
+        <v>0.0001660499423528841</v>
       </c>
       <c r="Y51" t="n">
         <v>1.096172023809523</v>
@@ -11587,10 +11587,10 @@
         <v>1.095885435587162</v>
       </c>
       <c r="AD51" t="n">
-        <v>0.000293815122697147</v>
+        <v>0.0002938151226971394</v>
       </c>
       <c r="AE51" t="n">
-        <v>0.000404330496264879</v>
+        <v>0.0004043304962648714</v>
       </c>
       <c r="AF51" t="n">
         <v>1.09629891237985</v>
@@ -11692,16 +11692,16 @@
         <v>45306.59368055555</v>
       </c>
       <c r="BM51" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN51" t="b">
         <v>1</v>
       </c>
       <c r="BO51" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP51" t="n">
-        <v>1956.920000000003</v>
+        <v>4471.199999999995</v>
       </c>
       <c r="BQ51" t="inlineStr"/>
       <c r="BR51" t="n">
@@ -11752,16 +11752,16 @@
         <v>1.09653</v>
       </c>
       <c r="L52" t="n">
-        <v>2.236728485216889e-05</v>
+        <v>2.236728485218372e-05</v>
       </c>
       <c r="M52" t="n">
-        <v>2.235942478839543e-05</v>
+        <v>2.235942478841026e-05</v>
       </c>
       <c r="N52" t="n">
-        <v>5.559526016092772e-05</v>
+        <v>5.559526016093143e-05</v>
       </c>
       <c r="O52" t="n">
-        <v>6.994076383339665e-05</v>
+        <v>6.994076383340035e-05</v>
       </c>
       <c r="P52" t="n">
         <v>1.095950395695311</v>
@@ -11785,10 +11785,10 @@
         <v>1.096358928571429</v>
       </c>
       <c r="W52" t="n">
-        <v>0.0002603804570156963</v>
+        <v>0.0002603804570156887</v>
       </c>
       <c r="X52" t="n">
-        <v>0.0001660499423528917</v>
+        <v>0.0001660499423528841</v>
       </c>
       <c r="Y52" t="n">
         <v>1.096172023809523</v>
@@ -11806,10 +11806,10 @@
         <v>1.095885435587162</v>
       </c>
       <c r="AD52" t="n">
-        <v>0.000293815122697147</v>
+        <v>0.0002938151226971394</v>
       </c>
       <c r="AE52" t="n">
-        <v>0.000404330496264879</v>
+        <v>0.0004043304962648714</v>
       </c>
       <c r="AF52" t="n">
         <v>1.09629891237985</v>
@@ -11911,16 +11911,16 @@
         <v>45306.41686342593</v>
       </c>
       <c r="BM52" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN52" t="b">
         <v>1</v>
       </c>
       <c r="BO52" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP52" t="n">
-        <v>1971.580000000003</v>
+        <v>4515.169999999996</v>
       </c>
       <c r="BQ52" t="inlineStr"/>
       <c r="BR52" t="n">
@@ -11971,16 +11971,16 @@
         <v>1.096579034624727</v>
       </c>
       <c r="L53" t="n">
-        <v>-8.543559485837587e-05</v>
+        <v>-8.543559485836103e-05</v>
       </c>
       <c r="M53" t="n">
-        <v>-8.825935993925996e-06</v>
+        <v>-8.825935993911159e-06</v>
       </c>
       <c r="N53" t="n">
-        <v>3.23575419934731e-05</v>
+        <v>3.235754199348423e-05</v>
       </c>
       <c r="O53" t="n">
-        <v>1.868122493647574e-05</v>
+        <v>1.868122493648687e-05</v>
       </c>
       <c r="P53" t="n">
         <v>1.096161883851813</v>
@@ -12025,10 +12025,10 @@
         <v>1.096332595487097</v>
       </c>
       <c r="AD53" t="n">
-        <v>0.0001660499423528917</v>
+        <v>0.0001660499423528841</v>
       </c>
       <c r="AE53" t="n">
-        <v>0.0002603804570156963</v>
+        <v>0.0002603804570156887</v>
       </c>
       <c r="AF53" t="n">
         <v>1.096312970793283</v>
@@ -12130,16 +12130,16 @@
         <v>45306.41686342593</v>
       </c>
       <c r="BM53" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN53" t="b">
         <v>1</v>
       </c>
       <c r="BO53" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP53" t="n">
-        <v>1986.240000000003</v>
+        <v>4559.139999999996</v>
       </c>
       <c r="BQ53" t="inlineStr"/>
       <c r="BR53" t="n">
@@ -12190,16 +12190,16 @@
         <v>1.096723605658021</v>
       </c>
       <c r="L54" t="n">
-        <v>-0.0002494087665880966</v>
+        <v>-0.0002494087665880854</v>
       </c>
       <c r="M54" t="n">
-        <v>-0.0001683029425453077</v>
+        <v>-0.0001683029425452966</v>
       </c>
       <c r="N54" t="n">
-        <v>-1.324013790311485e-05</v>
+        <v>-1.324013790310373e-05</v>
       </c>
       <c r="O54" t="n">
-        <v>2.765843803296942e-05</v>
+        <v>2.765843803298055e-05</v>
       </c>
       <c r="P54" t="n">
         <v>1.096192788103103</v>
@@ -12244,10 +12244,10 @@
         <v>1.096332595487097</v>
       </c>
       <c r="AD54" t="n">
-        <v>0.0001660499423528917</v>
+        <v>0.0001660499423528841</v>
       </c>
       <c r="AE54" t="n">
-        <v>0.0002603804570156963</v>
+        <v>0.0002603804570156887</v>
       </c>
       <c r="AF54" t="n">
         <v>1.096312970793283</v>
@@ -12349,16 +12349,16 @@
         <v>45306.41686342593</v>
       </c>
       <c r="BM54" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN54" t="b">
         <v>1</v>
       </c>
       <c r="BO54" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP54" t="n">
-        <v>2000.900000000003</v>
+        <v>4603.109999999996</v>
       </c>
       <c r="BQ54" t="inlineStr"/>
       <c r="BR54" t="n">
@@ -12409,16 +12409,16 @@
         <v>1.09228</v>
       </c>
       <c r="L55" t="n">
-        <v>-0.0002767635588450573</v>
+        <v>-0.0002767635588450462</v>
       </c>
       <c r="M55" t="n">
-        <v>-0.0005958883134139231</v>
+        <v>-0.0005958883134139119</v>
       </c>
       <c r="N55" t="n">
-        <v>-0.0001460426049436176</v>
+        <v>-0.0001460426049435916</v>
       </c>
       <c r="O55" t="n">
-        <v>-7.292088486141663e-05</v>
+        <v>-7.292088486139066e-05</v>
       </c>
       <c r="P55" t="n">
         <v>1.091153062017633</v>
@@ -12568,16 +12568,16 @@
         <v>45307.45105324074</v>
       </c>
       <c r="BM55" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN55" t="b">
         <v>1</v>
       </c>
       <c r="BO55" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP55" t="n">
-        <v>2015.560000000003</v>
+        <v>4647.079999999996</v>
       </c>
       <c r="BQ55" t="inlineStr"/>
       <c r="BR55" t="n">
@@ -12628,16 +12628,16 @@
         <v>1.09132</v>
       </c>
       <c r="L56" t="n">
-        <v>-0.0001648613191584336</v>
+        <v>-0.0001648613191584077</v>
       </c>
       <c r="M56" t="n">
-        <v>-0.0004541738068885561</v>
+        <v>-0.0004541738068885302</v>
       </c>
       <c r="N56" t="n">
-        <v>-0.0001693895553554306</v>
+        <v>-0.0001693895553554195</v>
       </c>
       <c r="O56" t="n">
-        <v>-0.0007154449307752633</v>
+        <v>-0.0007154449307752522</v>
       </c>
       <c r="P56" t="n">
         <v>1.091663347561052</v>
@@ -12787,16 +12787,16 @@
         <v>45307.56864583334</v>
       </c>
       <c r="BM56" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN56" t="b">
         <v>1</v>
       </c>
       <c r="BO56" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP56" t="n">
-        <v>2030.220000000003</v>
+        <v>4691.049999999997</v>
       </c>
       <c r="BQ56" t="inlineStr"/>
       <c r="BR56" t="n">
@@ -12847,16 +12847,16 @@
         <v>1.08794</v>
       </c>
       <c r="L57" t="n">
-        <v>-0.0002699998993990631</v>
+        <v>-0.000269999899399052</v>
       </c>
       <c r="M57" t="n">
-        <v>-0.0003374586790348291</v>
+        <v>-0.000337458679034818</v>
       </c>
       <c r="N57" t="n">
-        <v>0.0001110909454272636</v>
+        <v>0.0001110909454272747</v>
       </c>
       <c r="O57" t="n">
-        <v>0.0001106574189924306</v>
+        <v>0.0001106574189924417</v>
       </c>
       <c r="P57" t="n">
         <v>1.086690046914906</v>
@@ -12901,10 +12901,10 @@
         <v>1.087417481285464</v>
       </c>
       <c r="AD57" t="n">
-        <v>-2.778376145087322e-05</v>
+        <v>-2.77837614508616e-05</v>
       </c>
       <c r="AE57" t="n">
-        <v>-0.0002980033360290462</v>
+        <v>-0.0002980033360290346</v>
       </c>
       <c r="AF57" t="n">
         <v>1.086644038848923</v>
@@ -13004,16 +13004,16 @@
         <v>45308.6600462963</v>
       </c>
       <c r="BM57" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN57" t="b">
         <v>1</v>
       </c>
       <c r="BO57" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP57" t="n">
-        <v>2044.880000000003</v>
+        <v>4735.019999999997</v>
       </c>
       <c r="BQ57" t="inlineStr"/>
       <c r="BR57" t="n">
@@ -13064,16 +13064,16 @@
         <v>1.08722</v>
       </c>
       <c r="L58" t="n">
-        <v>0.000137323633903266</v>
+        <v>0.0001373236339032845</v>
       </c>
       <c r="M58" t="n">
-        <v>2.120354695060017e-05</v>
+        <v>2.120354695061871e-05</v>
       </c>
       <c r="N58" t="n">
-        <v>-0.0001501619504116558</v>
+        <v>-0.0001501619504116325</v>
       </c>
       <c r="O58" t="n">
-        <v>-0.0001163071741888403</v>
+        <v>-0.000116307174188817</v>
       </c>
       <c r="P58" t="n">
         <v>1.086929500509976</v>
@@ -13118,10 +13118,10 @@
         <v>1.087417481285464</v>
       </c>
       <c r="AD58" t="n">
-        <v>-2.778376145087322e-05</v>
+        <v>-2.77837614508616e-05</v>
       </c>
       <c r="AE58" t="n">
-        <v>-0.0002980033360290462</v>
+        <v>-0.0002980033360290346</v>
       </c>
       <c r="AF58" t="n">
         <v>1.086644038848923</v>
@@ -13221,16 +13221,16 @@
         <v>45308.71116898148</v>
       </c>
       <c r="BM58" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN58" t="b">
         <v>1</v>
       </c>
       <c r="BO58" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP58" t="n">
-        <v>2059.540000000003</v>
+        <v>4778.989999999997</v>
       </c>
       <c r="BQ58" t="inlineStr"/>
       <c r="BR58" t="n">
@@ -13275,22 +13275,22 @@
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>1.08589168108321</v>
+        <v>1.085891681083209</v>
       </c>
       <c r="K59" t="n">
         <v>1.08693</v>
       </c>
       <c r="L59" t="n">
-        <v>0.000137342403494458</v>
+        <v>0.0001373424034944692</v>
       </c>
       <c r="M59" t="n">
-        <v>0.0002664443240790494</v>
+        <v>0.0002664443240790605</v>
       </c>
       <c r="N59" t="n">
-        <v>-0.0004444435632736407</v>
+        <v>-0.0004444435632736185</v>
       </c>
       <c r="O59" t="n">
-        <v>-0.0003860208427366535</v>
+        <v>-0.0003860208427366312</v>
       </c>
       <c r="P59" t="n">
         <v>1.087365145802173</v>
@@ -13438,16 +13438,16 @@
         <v>45308.71114583333</v>
       </c>
       <c r="BM59" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN59" t="b">
         <v>1</v>
       </c>
       <c r="BO59" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP59" t="n">
-        <v>2074.200000000003</v>
+        <v>4822.959999999997</v>
       </c>
       <c r="BQ59" t="inlineStr"/>
       <c r="BR59" t="n">
@@ -13498,16 +13498,16 @@
         <v>1.08685</v>
       </c>
       <c r="L60" t="n">
-        <v>0.0005873396901347584</v>
+        <v>0.0005873396901347695</v>
       </c>
       <c r="M60" t="n">
-        <v>0.0004472448187847434</v>
+        <v>0.0004472448187847546</v>
       </c>
       <c r="N60" t="n">
-        <v>-0.0003374586790348291</v>
+        <v>-0.000337458679034818</v>
       </c>
       <c r="O60" t="n">
-        <v>-0.0002699998993990631</v>
+        <v>-0.000269999899399052</v>
       </c>
       <c r="P60" t="n">
         <v>1.086819144446534</v>
@@ -13655,16 +13655,16 @@
         <v>45308.70951388889</v>
       </c>
       <c r="BM60" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN60" t="b">
         <v>1</v>
       </c>
       <c r="BO60" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP60" t="n">
-        <v>2088.860000000003</v>
+        <v>4866.929999999998</v>
       </c>
       <c r="BQ60" t="inlineStr"/>
       <c r="BR60" t="n">
@@ -13715,22 +13715,22 @@
         <v>1.08822</v>
       </c>
       <c r="L61" t="n">
-        <v>1.689442772352505e-05</v>
+        <v>1.689442772354731e-05</v>
       </c>
       <c r="M61" t="n">
-        <v>-0.0002729877472858258</v>
+        <v>-0.0002729877472858036</v>
       </c>
       <c r="N61" t="n">
-        <v>0.0003753537959865728</v>
+        <v>0.000375353795986595</v>
       </c>
       <c r="O61" t="n">
-        <v>0.0003407027007048869</v>
+        <v>0.0003407027007049092</v>
       </c>
       <c r="P61" t="n">
         <v>1.086220987833058</v>
       </c>
       <c r="Q61" t="n">
-        <v>1.087537477275698</v>
+        <v>1.087537477275697</v>
       </c>
       <c r="R61" s="2" t="n">
         <v>45308.5</v>
@@ -13872,16 +13872,16 @@
         <v>45308.66042824074</v>
       </c>
       <c r="BM61" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN61" t="b">
         <v>1</v>
       </c>
       <c r="BO61" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP61" t="n">
-        <v>2103.520000000003</v>
+        <v>4910.899999999998</v>
       </c>
       <c r="BQ61" t="inlineStr"/>
       <c r="BR61" t="n">
@@ -13932,16 +13932,16 @@
         <v>1.0874</v>
       </c>
       <c r="L62" t="n">
-        <v>9.481500759835891e-05</v>
+        <v>9.481500759837265e-05</v>
       </c>
       <c r="M62" t="n">
-        <v>8.555815293494057e-05</v>
+        <v>8.555815293495432e-05</v>
       </c>
       <c r="N62" t="n">
-        <v>-8.191051832197071e-05</v>
+        <v>-8.191051832195696e-05</v>
       </c>
       <c r="O62" t="n">
-        <v>-0.0001469473317441356</v>
+        <v>-0.0001469473317441219</v>
       </c>
       <c r="P62" t="n">
         <v>1.087126661529335</v>
@@ -14089,16 +14089,16 @@
         <v>45308.65993055556</v>
       </c>
       <c r="BM62" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN62" t="b">
         <v>1</v>
       </c>
       <c r="BO62" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP62" t="n">
-        <v>2118.180000000003</v>
+        <v>4954.869999999998</v>
       </c>
       <c r="BQ62" t="inlineStr"/>
       <c r="BR62" t="n">
@@ -14149,16 +14149,16 @@
         <v>1.08643</v>
       </c>
       <c r="L63" t="n">
-        <v>0.0001611173345670897</v>
+        <v>0.0001611173345671008</v>
       </c>
       <c r="M63" t="n">
-        <v>9.861038494615833e-05</v>
+        <v>9.861038494616946e-05</v>
       </c>
       <c r="N63" t="n">
-        <v>-1.688234184080952e-05</v>
+        <v>-1.68823418408021e-05</v>
       </c>
       <c r="O63" t="n">
-        <v>-6.726313938965402e-05</v>
+        <v>-6.726313938964659e-05</v>
       </c>
       <c r="P63" t="n">
         <v>1.086173965087894</v>
@@ -14182,10 +14182,10 @@
         <v>1.085910595238095</v>
       </c>
       <c r="W63" t="n">
-        <v>0.0002819632505454501</v>
+        <v>0.0002819632505454425</v>
       </c>
       <c r="X63" t="n">
-        <v>0.0001648269140443464</v>
+        <v>0.0001648269140443388</v>
       </c>
       <c r="Y63" t="n">
         <v>1.085649523809524</v>
@@ -14300,7 +14300,7 @@
       <c r="BK63" t="inlineStr"/>
       <c r="BL63" t="inlineStr"/>
       <c r="BM63" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN63" t="b">
         <v>0</v>
@@ -14309,7 +14309,7 @@
         <v>0</v>
       </c>
       <c r="BP63" t="n">
-        <v>2118.180000000003</v>
+        <v>4954.869999999998</v>
       </c>
       <c r="BQ63" s="2" t="n">
         <v>45310.03125</v>
@@ -14362,16 +14362,16 @@
         <v>1.088648340580614</v>
       </c>
       <c r="L64" t="n">
-        <v>1.865315327086929e-05</v>
+        <v>1.865315327087933e-05</v>
       </c>
       <c r="M64" t="n">
-        <v>-6.277759604938446e-05</v>
+        <v>-6.277759604937441e-05</v>
       </c>
       <c r="N64" t="n">
-        <v>5.593962274520367e-05</v>
+        <v>5.593962274521479e-05</v>
       </c>
       <c r="O64" t="n">
-        <v>-4.557950643182563e-05</v>
+        <v>-4.55795064318145e-05</v>
       </c>
       <c r="P64" t="n">
         <v>1.087485829472383</v>
@@ -14521,16 +14521,16 @@
         <v>45310.5678587963</v>
       </c>
       <c r="BM64" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN64" t="b">
         <v>1</v>
       </c>
       <c r="BO64" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP64" t="n">
-        <v>2132.840000000002</v>
+        <v>4998.859999999998</v>
       </c>
       <c r="BQ64" t="inlineStr"/>
       <c r="BR64" t="n">
@@ -14581,16 +14581,16 @@
         <v>1.088778809595401</v>
       </c>
       <c r="L65" t="n">
-        <v>-0.0001928689520151634</v>
+        <v>-0.0001928689520151448</v>
       </c>
       <c r="M65" t="n">
-        <v>-0.0002752872560228209</v>
+        <v>-0.0002752872560228023</v>
       </c>
       <c r="N65" t="n">
-        <v>0.000119183909233442</v>
+        <v>0.0001191839092334568</v>
       </c>
       <c r="O65" t="n">
-        <v>7.049977018280137e-05</v>
+        <v>7.049977018281622e-05</v>
       </c>
       <c r="P65" t="n">
         <v>1.08730984233653</v>
@@ -14740,16 +14740,16 @@
         <v>45313.0034837963</v>
       </c>
       <c r="BM65" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN65" t="b">
         <v>1</v>
       </c>
       <c r="BO65" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP65" t="n">
-        <v>2147.500000000002</v>
+        <v>5042.849999999998</v>
       </c>
       <c r="BQ65" t="inlineStr"/>
       <c r="BR65" t="n">
@@ -14800,16 +14800,16 @@
         <v>1.08787914403001</v>
       </c>
       <c r="L66" t="n">
-        <v>0.0002240760935483843</v>
+        <v>0.0002240760935484103</v>
       </c>
       <c r="M66" t="n">
-        <v>0.0002347393385482906</v>
+        <v>0.0002347393385483166</v>
       </c>
       <c r="N66" t="n">
-        <v>-6.715414530737773e-05</v>
+        <v>-6.715414530736289e-05</v>
       </c>
       <c r="O66" t="n">
-        <v>-0.000305076719462427</v>
+        <v>-0.0003050767194624121</v>
       </c>
       <c r="P66" t="n">
         <v>1.087375408118936</v>
@@ -14833,10 +14833,10 @@
         <v>1.087883452380952</v>
       </c>
       <c r="W66" t="n">
-        <v>-0.0003499429851549042</v>
+        <v>-0.0003499429851549142</v>
       </c>
       <c r="X66" t="n">
-        <v>-8.545928960595716e-05</v>
+        <v>-8.54592896059673e-05</v>
       </c>
       <c r="Y66" t="n">
         <v>1.088159761904762</v>
@@ -14959,16 +14959,16 @@
         <v>45310.58532407408</v>
       </c>
       <c r="BM66" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN66" t="b">
         <v>1</v>
       </c>
       <c r="BO66" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP66" t="n">
-        <v>2162.160000000002</v>
+        <v>5086.839999999997</v>
       </c>
       <c r="BQ66" t="inlineStr"/>
       <c r="BR66" t="n">
@@ -15025,10 +15025,10 @@
         <v>-0.0001650313095126969</v>
       </c>
       <c r="N67" t="n">
-        <v>0.0001739570188085625</v>
+        <v>0.0001739570188085847</v>
       </c>
       <c r="O67" t="n">
-        <v>0.0001647376734383036</v>
+        <v>0.0001647376734383258</v>
       </c>
       <c r="P67" t="n">
         <v>1.089616970645408</v>
@@ -15052,10 +15052,10 @@
         <v>1.090371666666667</v>
       </c>
       <c r="W67" t="n">
-        <v>-3.643175845891594e-05</v>
+        <v>-3.643175845892354e-05</v>
       </c>
       <c r="X67" t="n">
-        <v>9.367648898294673e-06</v>
+        <v>9.36764889828707e-06</v>
       </c>
       <c r="Y67" t="n">
         <v>1.090335833333333</v>
@@ -15178,16 +15178,16 @@
         <v>45315.69791666666</v>
       </c>
       <c r="BM67" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN67" t="b">
         <v>1</v>
       </c>
       <c r="BO67" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP67" t="n">
-        <v>2176.820000000002</v>
+        <v>5130.829999999997</v>
       </c>
       <c r="BQ67" t="inlineStr"/>
       <c r="BR67" t="n">
@@ -15238,16 +15238,16 @@
         <v>1.088859137927411</v>
       </c>
       <c r="L68" t="n">
-        <v>0.0001898869701891442</v>
+        <v>0.000189886970189159</v>
       </c>
       <c r="M68" t="n">
-        <v>0.0001381356431922387</v>
+        <v>0.0001381356431922535</v>
       </c>
       <c r="N68" t="n">
-        <v>-0.0002653487397194297</v>
+        <v>-0.0002653487397194037</v>
       </c>
       <c r="O68" t="n">
-        <v>-0.0001283794907116906</v>
+        <v>-0.0001283794907116647</v>
       </c>
       <c r="P68" t="n">
         <v>1.088608153766601</v>
@@ -15397,16 +15397,16 @@
         <v>45315.4050462963</v>
       </c>
       <c r="BM68" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN68" t="b">
         <v>1</v>
       </c>
       <c r="BO68" t="n">
-        <v>91.59999999999999</v>
+        <v>274.83</v>
       </c>
       <c r="BP68" t="n">
-        <v>2268.420000000002</v>
+        <v>5405.659999999997</v>
       </c>
       <c r="BQ68" t="inlineStr"/>
       <c r="BR68" t="n">
@@ -15457,16 +15457,16 @@
         <v>1.088526666091105</v>
       </c>
       <c r="L69" t="n">
-        <v>0.0004012814196234476</v>
+        <v>0.0004012814196234587</v>
       </c>
       <c r="M69" t="n">
-        <v>0.0002510729460928106</v>
+        <v>0.0002510729460928217</v>
       </c>
       <c r="N69" t="n">
-        <v>-0.0001516282902885026</v>
+        <v>-0.0001516282902884915</v>
       </c>
       <c r="O69" t="n">
-        <v>-0.0001100464640523308</v>
+        <v>-0.0001100464640523196</v>
       </c>
       <c r="P69" t="n">
         <v>1.087969922930233</v>
@@ -15616,16 +15616,16 @@
         <v>45314.59231481481</v>
       </c>
       <c r="BM69" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN69" t="b">
         <v>1</v>
       </c>
       <c r="BO69" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP69" t="n">
-        <v>2283.080000000002</v>
+        <v>5449.629999999997</v>
       </c>
       <c r="BQ69" t="inlineStr"/>
       <c r="BR69" t="n">
@@ -15676,16 +15676,16 @@
         <v>1.0893</v>
       </c>
       <c r="L70" t="n">
-        <v>6.349955170663855e-05</v>
+        <v>6.349955170664969e-05</v>
       </c>
       <c r="M70" t="n">
-        <v>5.860432305845516e-06</v>
+        <v>5.860432305856657e-06</v>
       </c>
       <c r="N70" t="n">
-        <v>0.0001423166744041486</v>
+        <v>0.0001423166744041597</v>
       </c>
       <c r="O70" t="n">
-        <v>5.232205259376909e-05</v>
+        <v>5.232205259378021e-05</v>
       </c>
       <c r="P70" t="n">
         <v>1.088434838204518</v>
@@ -15835,16 +15835,16 @@
         <v>45315.40631944445</v>
       </c>
       <c r="BM70" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN70" t="b">
         <v>1</v>
       </c>
       <c r="BO70" t="n">
-        <v>91.59999999999999</v>
+        <v>274.83</v>
       </c>
       <c r="BP70" t="n">
-        <v>2374.680000000002</v>
+        <v>5724.459999999997</v>
       </c>
       <c r="BQ70" t="inlineStr"/>
       <c r="BR70" t="n">
@@ -15895,16 +15895,16 @@
         <v>1.08554</v>
       </c>
       <c r="L71" t="n">
-        <v>-0.0003088409320559346</v>
+        <v>-0.0003088409320559293</v>
       </c>
       <c r="M71" t="n">
-        <v>-6.027165874212962e-05</v>
+        <v>-6.027165874212438e-05</v>
       </c>
       <c r="N71" t="n">
-        <v>0.0001293651650291122</v>
+        <v>0.000129365165029127</v>
       </c>
       <c r="O71" t="n">
-        <v>0.0001876853000866244</v>
+        <v>0.0001876853000866393</v>
       </c>
       <c r="P71" t="n">
         <v>1.084506623907767</v>
@@ -16052,16 +16052,16 @@
         <v>45316.80274305555</v>
       </c>
       <c r="BM71" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN71" t="b">
         <v>1</v>
       </c>
       <c r="BO71" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP71" t="n">
-        <v>2389.340000000002</v>
+        <v>5768.429999999998</v>
       </c>
       <c r="BQ71" t="inlineStr"/>
       <c r="BR71" t="n">
@@ -16112,16 +16112,16 @@
         <v>1.08782</v>
       </c>
       <c r="L72" t="n">
-        <v>-9.635267139089107e-05</v>
+        <v>-9.635267139086513e-05</v>
       </c>
       <c r="M72" t="n">
-        <v>-0.0005276907869188702</v>
+        <v>-0.0005276907869188444</v>
       </c>
       <c r="N72" t="n">
-        <v>-0.0005263347235049277</v>
+        <v>-0.0005263347235049177</v>
       </c>
       <c r="O72" t="n">
-        <v>-0.0007361905193923054</v>
+        <v>-0.0007361905193922954</v>
       </c>
       <c r="P72" t="n">
         <v>1.087704180741968</v>
@@ -16271,16 +16271,16 @@
         <v>45317.50620370371</v>
       </c>
       <c r="BM72" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN72" t="b">
         <v>1</v>
       </c>
       <c r="BO72" t="n">
-        <v>91.59999999999999</v>
+        <v>274.83</v>
       </c>
       <c r="BP72" t="n">
-        <v>2480.940000000001</v>
+        <v>6043.259999999997</v>
       </c>
       <c r="BQ72" t="inlineStr"/>
       <c r="BR72" t="n">
@@ -16331,16 +16331,16 @@
         <v>1.084596667013578</v>
       </c>
       <c r="L73" t="n">
-        <v>-8.454410158035773e-05</v>
+        <v>-8.45441015803466e-05</v>
       </c>
       <c r="M73" t="n">
-        <v>4.302473614896926e-05</v>
+        <v>4.302473614898039e-05</v>
       </c>
       <c r="N73" t="n">
-        <v>-2.305045295242192e-05</v>
+        <v>-2.305045295240554e-05</v>
       </c>
       <c r="O73" t="n">
-        <v>-0.000113729608614082</v>
+        <v>-0.0001137296086140656</v>
       </c>
       <c r="P73" t="n">
         <v>1.084446637986344</v>
@@ -16488,16 +16488,16 @@
         <v>45317.45226851852</v>
       </c>
       <c r="BM73" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN73" t="b">
         <v>1</v>
       </c>
       <c r="BO73" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP73" t="n">
-        <v>2495.600000000001</v>
+        <v>6087.229999999998</v>
       </c>
       <c r="BQ73" t="inlineStr"/>
       <c r="BR73" t="n">
@@ -16548,16 +16548,16 @@
         <v>1.084838332410422</v>
       </c>
       <c r="L74" t="n">
-        <v>-0.0001473537159695313</v>
+        <v>-0.000147353715969525</v>
       </c>
       <c r="M74" t="n">
-        <v>-0.0001467403554085816</v>
+        <v>-0.0001467403554085753</v>
       </c>
       <c r="N74" t="n">
-        <v>-5.493208504987834e-05</v>
+        <v>-5.493208504985979e-05</v>
       </c>
       <c r="O74" t="n">
-        <v>1.229861895603879e-05</v>
+        <v>1.229861895605735e-05</v>
       </c>
       <c r="P74" t="n">
         <v>1.08419774474296</v>
@@ -16705,16 +16705,16 @@
         <v>45317.44694444445</v>
       </c>
       <c r="BM74" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN74" t="b">
         <v>1</v>
       </c>
       <c r="BO74" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP74" t="n">
-        <v>2510.260000000001</v>
+        <v>6131.199999999998</v>
       </c>
       <c r="BQ74" t="inlineStr"/>
       <c r="BR74" t="n">
@@ -16765,16 +16765,16 @@
         <v>1.084216662148805</v>
       </c>
       <c r="L75" t="n">
-        <v>7.074003174319477e-05</v>
+        <v>7.074003174320961e-05</v>
       </c>
       <c r="M75" t="n">
-        <v>7.993051694864062e-05</v>
+        <v>7.993051694865546e-05</v>
       </c>
       <c r="N75" t="n">
-        <v>-0.0001467403554085816</v>
+        <v>-0.0001467403554085753</v>
       </c>
       <c r="O75" t="n">
-        <v>-0.0001473537159695313</v>
+        <v>-0.000147353715969525</v>
       </c>
       <c r="P75" t="n">
         <v>1.084237147405597</v>
@@ -16922,16 +16922,16 @@
         <v>45317.44428240741</v>
       </c>
       <c r="BM75" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN75" t="b">
         <v>1</v>
       </c>
       <c r="BO75" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP75" t="n">
-        <v>2524.920000000001</v>
+        <v>6175.169999999998</v>
       </c>
       <c r="BQ75" t="inlineStr"/>
       <c r="BR75" t="n">
@@ -16982,16 +16982,16 @@
         <v>1.08439</v>
       </c>
       <c r="L76" t="n">
-        <v>0.0001007148998698613</v>
+        <v>0.0001007148998698761</v>
       </c>
       <c r="M76" t="n">
-        <v>5.50758939202299e-05</v>
+        <v>5.507589392024476e-05</v>
       </c>
       <c r="N76" t="n">
-        <v>-4.328355400389261e-05</v>
+        <v>-4.328355400388148e-05</v>
       </c>
       <c r="O76" t="n">
-        <v>-8.381752046966036e-05</v>
+        <v>-8.381752046964922e-05</v>
       </c>
       <c r="P76" t="n">
         <v>1.083854356363811</v>
@@ -17139,16 +17139,16 @@
         <v>45317.44435185185</v>
       </c>
       <c r="BM76" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN76" t="b">
         <v>1</v>
       </c>
       <c r="BO76" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP76" t="n">
-        <v>2539.580000000001</v>
+        <v>6219.139999999999</v>
       </c>
       <c r="BQ76" t="inlineStr"/>
       <c r="BR76" t="n">
@@ -17199,16 +17199,16 @@
         <v>1.08468</v>
       </c>
       <c r="L77" t="n">
-        <v>-6.406889722468916e-06</v>
+        <v>-6.406889722454079e-06</v>
       </c>
       <c r="M77" t="n">
-        <v>-9.99557388214501e-06</v>
+        <v>-9.995573882130173e-06</v>
       </c>
       <c r="N77" t="n">
-        <v>-3.609315467684786e-05</v>
+        <v>-3.609315467683302e-05</v>
       </c>
       <c r="O77" t="n">
-        <v>3.332572376274667e-06</v>
+        <v>3.332572376289507e-06</v>
       </c>
       <c r="P77" t="n">
         <v>1.084330292665992</v>
@@ -17356,16 +17356,16 @@
         <v>45317.44900462963</v>
       </c>
       <c r="BM77" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN77" t="b">
         <v>1</v>
       </c>
       <c r="BO77" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP77" t="n">
-        <v>2554.240000000001</v>
+        <v>6263.109999999999</v>
       </c>
       <c r="BQ77" t="inlineStr"/>
       <c r="BR77" t="n">
@@ -17416,16 +17416,16 @@
         <v>1.084677482244784</v>
       </c>
       <c r="L78" t="n">
-        <v>-7.35298883449287e-05</v>
+        <v>-7.352988834491387e-05</v>
       </c>
       <c r="M78" t="n">
-        <v>-7.298889914976349e-05</v>
+        <v>-7.298889914974866e-05</v>
       </c>
       <c r="N78" t="n">
-        <v>-5.685442160007611e-05</v>
+        <v>-5.685442160005974e-05</v>
       </c>
       <c r="O78" t="n">
-        <v>-3.842281680098009e-05</v>
+        <v>-3.842281680096372e-05</v>
       </c>
       <c r="P78" t="n">
         <v>1.084368286714039</v>
@@ -17449,10 +17449,10 @@
         <v>1.084368452380952</v>
       </c>
       <c r="W78" t="n">
-        <v>0.0001668512050274914</v>
+        <v>0.0001668512050275015</v>
       </c>
       <c r="X78" t="n">
-        <v>4.634792760407175e-05</v>
+        <v>4.634792760408189e-05</v>
       </c>
       <c r="Y78" t="n">
         <v>1.084397380952381</v>
@@ -17573,16 +17573,16 @@
         <v>45317.451875</v>
       </c>
       <c r="BM78" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN78" t="b">
         <v>1</v>
       </c>
       <c r="BO78" t="n">
-        <v>14.66</v>
+        <v>43.97</v>
       </c>
       <c r="BP78" t="n">
-        <v>2568.900000000001</v>
+        <v>6307.079999999999</v>
       </c>
       <c r="BQ78" t="inlineStr"/>
       <c r="BR78" t="n">
@@ -17633,16 +17633,16 @@
         <v>1.084149031485052</v>
       </c>
       <c r="L79" t="n">
-        <v>-0.0002924405146451338</v>
+        <v>-0.0002924405146451227</v>
       </c>
       <c r="M79" t="n">
-        <v>-0.0003596252865616362</v>
+        <v>-0.000359625286561625</v>
       </c>
       <c r="N79" t="n">
-        <v>-9.838876115918767e-05</v>
+        <v>-9.838876115916913e-05</v>
       </c>
       <c r="O79" t="n">
-        <v>-0.0001380349531237681</v>
+        <v>-0.0001380349531237495</v>
       </c>
       <c r="P79" t="n">
         <v>1.083807963603524</v>
@@ -17687,10 +17687,10 @@
         <v>1.084967306848545</v>
       </c>
       <c r="AD79" t="n">
-        <v>-0.0001376906105274169</v>
+        <v>-0.000137690610527427</v>
       </c>
       <c r="AE79" t="n">
-        <v>-3.358675051104162e-05</v>
+        <v>-3.358675051105176e-05</v>
       </c>
       <c r="AF79" t="n">
         <v>1.083287097288879</v>
@@ -17792,16 +17792,16 @@
         <v>45320.00349537037</v>
       </c>
       <c r="BM79" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN79" t="b">
         <v>1</v>
       </c>
       <c r="BO79" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP79" t="n">
-        <v>2583.56</v>
+        <v>6351.069999999999</v>
       </c>
       <c r="BQ79" t="inlineStr"/>
       <c r="BR79" t="n">
@@ -17852,16 +17852,16 @@
         <v>1.082286779532044</v>
       </c>
       <c r="L80" t="n">
-        <v>0.0004466859528581979</v>
+        <v>0.0004466859528582201</v>
       </c>
       <c r="M80" t="n">
-        <v>0.0003909663768079895</v>
+        <v>0.0003909663768080117</v>
       </c>
       <c r="N80" t="n">
-        <v>-0.0003297433527697997</v>
+        <v>-0.0003297433527697774</v>
       </c>
       <c r="O80" t="n">
-        <v>-0.0002110678364731794</v>
+        <v>-0.0002110678364731572</v>
       </c>
       <c r="P80" t="n">
         <v>1.08166031358037</v>
@@ -17885,10 +17885,10 @@
         <v>1.0830575</v>
       </c>
       <c r="W80" t="n">
-        <v>-0.0007159414236435653</v>
+        <v>-0.0007159414236435526</v>
       </c>
       <c r="X80" t="n">
-        <v>-0.0001974063047646891</v>
+        <v>-0.0001974063047646764</v>
       </c>
       <c r="Y80" t="n">
         <v>1.083722023809523</v>
@@ -18013,16 +18013,16 @@
         <v>45320.47018518519</v>
       </c>
       <c r="BM80" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN80" t="b">
         <v>1</v>
       </c>
       <c r="BO80" t="n">
-        <v>91.62</v>
+        <v>274.95</v>
       </c>
       <c r="BP80" t="n">
-        <v>2675.18</v>
+        <v>6626.019999999999</v>
       </c>
       <c r="BQ80" t="inlineStr"/>
       <c r="BR80" t="n">
@@ -18073,16 +18073,16 @@
         <v>1.085855047134534</v>
       </c>
       <c r="L81" t="n">
-        <v>0.000510147478706203</v>
+        <v>0.0005101474787062217</v>
       </c>
       <c r="M81" t="n">
-        <v>0.0002255597940001753</v>
+        <v>0.0002255597940001938</v>
       </c>
       <c r="N81" t="n">
-        <v>0.0004162866921833151</v>
+        <v>0.0004162866921833251</v>
       </c>
       <c r="O81" t="n">
-        <v>0.0003073049455700355</v>
+        <v>0.0003073049455700456</v>
       </c>
       <c r="P81" t="n">
         <v>1.083388095812372</v>
@@ -18232,16 +18232,16 @@
         <v>45317.64806712963</v>
       </c>
       <c r="BM81" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN81" t="b">
         <v>1</v>
       </c>
       <c r="BO81" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP81" t="n">
-        <v>2689.84</v>
+        <v>6670.009999999998</v>
       </c>
       <c r="BQ81" t="inlineStr"/>
       <c r="BR81" t="n">
@@ -18292,16 +18292,16 @@
         <v>1.086950433126484</v>
       </c>
       <c r="L82" t="n">
-        <v>1.341841110362991e-05</v>
+        <v>1.341841110365216e-05</v>
       </c>
       <c r="M82" t="n">
-        <v>-5.56003334734509e-05</v>
+        <v>-5.560033347342865e-05</v>
       </c>
       <c r="N82" t="n">
-        <v>0.0001062210418154794</v>
+        <v>0.000106221041815498</v>
       </c>
       <c r="O82" t="n">
-        <v>0.0001477674285609826</v>
+        <v>0.0001477674285610011</v>
       </c>
       <c r="P82" t="n">
         <v>1.085523317694237</v>
@@ -18346,10 +18346,10 @@
         <v>1.088540314171624</v>
       </c>
       <c r="AD82" t="n">
-        <v>-1.931777360131826e-05</v>
+        <v>-1.931777360130813e-05</v>
       </c>
       <c r="AE82" t="n">
-        <v>-0.000211781585088158</v>
+        <v>-0.0002117815850881479</v>
       </c>
       <c r="AF82" t="n">
         <v>1.086497449357267</v>
@@ -18451,16 +18451,16 @@
         <v>45322.71143518519</v>
       </c>
       <c r="BM82" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN82" t="b">
         <v>1</v>
       </c>
       <c r="BO82" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP82" t="n">
-        <v>2704.5</v>
+        <v>6713.999999999998</v>
       </c>
       <c r="BQ82" t="inlineStr"/>
       <c r="BR82" t="n">
@@ -18511,16 +18511,16 @@
         <v>1.086849990307265</v>
       </c>
       <c r="L83" t="n">
-        <v>-0.0001132972256291768</v>
+        <v>-0.0001132972256291619</v>
       </c>
       <c r="M83" t="n">
-        <v>5.980674361389748e-05</v>
+        <v>5.98067436139123e-05</v>
       </c>
       <c r="N83" t="n">
-        <v>0.0001020094894602029</v>
+        <v>0.0001020094894602214</v>
       </c>
       <c r="O83" t="n">
-        <v>0.0001293109763268944</v>
+        <v>0.0001293109763269129</v>
       </c>
       <c r="P83" t="n">
         <v>1.085831639514052</v>
@@ -18565,10 +18565,10 @@
         <v>1.088540314171624</v>
       </c>
       <c r="AD83" t="n">
-        <v>-1.931777360131826e-05</v>
+        <v>-1.931777360130813e-05</v>
       </c>
       <c r="AE83" t="n">
-        <v>-0.000211781585088158</v>
+        <v>-0.0002117815850881479</v>
       </c>
       <c r="AF83" t="n">
         <v>1.086497449357267</v>
@@ -18670,16 +18670,16 @@
         <v>45322.70023148148</v>
       </c>
       <c r="BM83" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN83" t="b">
         <v>1</v>
       </c>
       <c r="BO83" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP83" t="n">
-        <v>2719.16</v>
+        <v>6757.989999999998</v>
       </c>
       <c r="BQ83" t="inlineStr"/>
       <c r="BR83" t="n">
@@ -18730,16 +18730,16 @@
         <v>1.086048730509265</v>
       </c>
       <c r="L84" t="n">
-        <v>5.105058764825697e-05</v>
+        <v>5.10505876482596e-05</v>
       </c>
       <c r="M84" t="n">
-        <v>3.721831789101097e-05</v>
+        <v>3.72183178910136e-05</v>
       </c>
       <c r="N84" t="n">
-        <v>2.807409927074805e-06</v>
+        <v>2.807409927085931e-06</v>
       </c>
       <c r="O84" t="n">
-        <v>6.423015288197401e-05</v>
+        <v>6.423015288198515e-05</v>
       </c>
       <c r="P84" t="n">
         <v>1.085346591196924</v>
@@ -18763,10 +18763,10 @@
         <v>1.085907142857143</v>
       </c>
       <c r="W84" t="n">
-        <v>-3.659905441116271e-05</v>
+        <v>-3.659905441117789e-05</v>
       </c>
       <c r="X84" t="n">
-        <v>-0.0002392706821506122</v>
+        <v>-0.0002392706821506273</v>
       </c>
       <c r="Y84" t="n">
         <v>1.08609880952381</v>
@@ -18889,16 +18889,16 @@
         <v>45322.72554398148</v>
       </c>
       <c r="BM84" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="BN84" t="b">
         <v>1</v>
       </c>
       <c r="BO84" t="n">
-        <v>14.66</v>
+        <v>43.99</v>
       </c>
       <c r="BP84" t="n">
-        <v>2733.82</v>
+        <v>6801.979999999998</v>
       </c>
       <c r="BQ84" t="inlineStr"/>
       <c r="BR84" t="n">

</xml_diff>

<commit_message>
trade failing when it is actually winning
</commit_message>
<xml_diff>
--- a/filtered_excel_df.xlsx
+++ b/filtered_excel_df.xlsx
@@ -1759,13 +1759,13 @@
         <v>1.09076</v>
       </c>
       <c r="EX2" t="n">
-        <v>1.08096</v>
+        <v>1.08276</v>
       </c>
       <c r="EY2" t="n">
-        <v>1.08296</v>
+        <v>1.08476</v>
       </c>
       <c r="EZ2" t="n">
-        <v>1.08426</v>
+        <v>1.08626</v>
       </c>
       <c r="FA2" t="n">
         <v>0</v>
@@ -1777,13 +1777,13 @@
         <v>1</v>
       </c>
       <c r="FD2" s="2" t="n">
-        <v>45481.66666666666</v>
+        <v>45484.66666666666</v>
       </c>
       <c r="FE2" s="2" t="n">
         <v>45485.74561342593</v>
       </c>
       <c r="FF2" s="2" t="n">
-        <v>45478.64584490741</v>
+        <v>45481.00001157408</v>
       </c>
       <c r="FG2" s="2" t="n">
         <v>45477.75</v>
@@ -1792,10 +1792,10 @@
         <v>1.08076</v>
       </c>
       <c r="FI2" s="2" t="n">
-        <v>45478.64584490741</v>
+        <v>45481.00001157408</v>
       </c>
       <c r="FJ2" t="n">
-        <v>1.08255</v>
+        <v>1.08009</v>
       </c>
       <c r="FK2" t="inlineStr">
         <is>
@@ -1811,10 +1811,10 @@
         </is>
       </c>
       <c r="FN2" t="n">
-        <v>93.84</v>
+        <v>-35.13</v>
       </c>
       <c r="FO2" t="n">
-        <v>793.84</v>
+        <v>664.87</v>
       </c>
       <c r="FP2" t="b">
         <v>1</v>
@@ -2279,13 +2279,13 @@
         <v>1.09285</v>
       </c>
       <c r="EX3" t="n">
-        <v>1.08305</v>
+        <v>1.08485</v>
       </c>
       <c r="EY3" t="n">
-        <v>1.08505</v>
+        <v>1.08685</v>
       </c>
       <c r="EZ3" t="n">
-        <v>1.08635</v>
+        <v>1.08835</v>
       </c>
       <c r="FA3" t="n">
         <v>0</v>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="FE3" t="inlineStr"/>
       <c r="FF3" s="2" t="n">
-        <v>45481.56739583334</v>
+        <v>45484.63805555556</v>
       </c>
       <c r="FG3" s="2" t="n">
         <v>45481.20833333334</v>
@@ -2310,14 +2310,14 @@
         <v>1.08285</v>
       </c>
       <c r="FI3" s="2" t="n">
-        <v>45481.56739583334</v>
+        <v>45482.625</v>
       </c>
       <c r="FJ3" t="n">
-        <v>1.08308</v>
+        <v>1.08131</v>
       </c>
       <c r="FK3" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL3" t="n">
@@ -2325,23 +2325,23 @@
       </c>
       <c r="FM3" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN3" t="n">
-        <v>12.06</v>
+        <v>-80.73999999999999</v>
       </c>
       <c r="FO3" t="n">
-        <v>805.9</v>
+        <v>584.13</v>
       </c>
       <c r="FP3" t="b">
+        <v>0</v>
+      </c>
+      <c r="FQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="FR3" t="n">
         <v>1</v>
-      </c>
-      <c r="FQ3" t="n">
-        <v>2</v>
-      </c>
-      <c r="FR3" t="n">
-        <v>0</v>
       </c>
       <c r="FS3" t="n">
         <v>28</v>
@@ -2797,13 +2797,13 @@
         <v>1.09308</v>
       </c>
       <c r="EX4" t="n">
-        <v>1.08328</v>
+        <v>1.08708</v>
       </c>
       <c r="EY4" t="n">
-        <v>1.08528</v>
+        <v>1.08908</v>
       </c>
       <c r="EZ4" t="n">
-        <v>1.08658</v>
+        <v>1.09158</v>
       </c>
       <c r="FA4" t="n">
         <v>0</v>
@@ -2815,11 +2815,11 @@
         <v>1</v>
       </c>
       <c r="FD4" s="2" t="n">
-        <v>45484.66666666666</v>
+        <v>45488.75</v>
       </c>
       <c r="FE4" t="inlineStr"/>
       <c r="FF4" s="2" t="n">
-        <v>45481.54785879629</v>
+        <v>45484.72371527777</v>
       </c>
       <c r="FG4" s="2" t="n">
         <v>45481.29166666666</v>
@@ -2828,14 +2828,14 @@
         <v>1.08308</v>
       </c>
       <c r="FI4" s="2" t="n">
-        <v>45481.54785879629</v>
+        <v>45482.625</v>
       </c>
       <c r="FJ4" t="n">
-        <v>1.0833</v>
+        <v>1.08131</v>
       </c>
       <c r="FK4" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL4" t="n">
@@ -2843,23 +2843,23 @@
       </c>
       <c r="FM4" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN4" t="n">
-        <v>11.53</v>
+        <v>-92.79000000000001</v>
       </c>
       <c r="FO4" t="n">
-        <v>817.4299999999999</v>
+        <v>491.34</v>
       </c>
       <c r="FP4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="FR4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="FS4" t="n">
         <v>28</v>
@@ -3315,13 +3315,13 @@
         <v>1.09362</v>
       </c>
       <c r="EX5" t="n">
-        <v>1.08382</v>
+        <v>1.08762</v>
       </c>
       <c r="EY5" t="n">
-        <v>1.08582</v>
+        <v>1.08962</v>
       </c>
       <c r="EZ5" t="n">
-        <v>1.08712</v>
+        <v>1.09212</v>
       </c>
       <c r="FA5" t="n">
         <v>0</v>
@@ -3332,13 +3332,9 @@
       <c r="FC5" t="b">
         <v>1</v>
       </c>
-      <c r="FD5" s="2" t="n">
-        <v>45484.66666666666</v>
-      </c>
+      <c r="FD5" t="inlineStr"/>
       <c r="FE5" t="inlineStr"/>
-      <c r="FF5" s="2" t="n">
-        <v>45481.67283564815</v>
-      </c>
+      <c r="FF5" t="inlineStr"/>
       <c r="FG5" s="2" t="n">
         <v>45481.45833333334</v>
       </c>
@@ -3346,14 +3342,14 @@
         <v>1.08362</v>
       </c>
       <c r="FI5" s="2" t="n">
-        <v>45481.67283564815</v>
+        <v>45482.625</v>
       </c>
       <c r="FJ5" t="n">
-        <v>1.08384</v>
+        <v>1.08131</v>
       </c>
       <c r="FK5" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL5" t="n">
@@ -3361,23 +3357,23 @@
       </c>
       <c r="FM5" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN5" t="n">
-        <v>11.53</v>
+        <v>-121.1</v>
       </c>
       <c r="FO5" t="n">
-        <v>828.9599999999999</v>
+        <v>370.24</v>
       </c>
       <c r="FP5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="FR5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="FS5" t="n">
         <v>28</v>
@@ -3833,13 +3829,13 @@
         <v>1.09298</v>
       </c>
       <c r="EX6" t="n">
-        <v>1.08318</v>
+        <v>1.08698</v>
       </c>
       <c r="EY6" t="n">
-        <v>1.08518</v>
+        <v>1.08898</v>
       </c>
       <c r="EZ6" t="n">
-        <v>1.08648</v>
+        <v>1.09148</v>
       </c>
       <c r="FA6" t="n">
         <v>0</v>
@@ -3851,11 +3847,11 @@
         <v>1</v>
       </c>
       <c r="FD6" s="2" t="n">
-        <v>45484.66666666666</v>
+        <v>45488.75</v>
       </c>
       <c r="FE6" t="inlineStr"/>
       <c r="FF6" s="2" t="n">
-        <v>45484.40765046296</v>
+        <v>45484.76202546297</v>
       </c>
       <c r="FG6" s="2" t="n">
         <v>45482.125</v>
@@ -3886,7 +3882,7 @@
         <v>-87.55</v>
       </c>
       <c r="FO6" t="n">
-        <v>741.41</v>
+        <v>282.69</v>
       </c>
       <c r="FP6" t="b">
         <v>0</v>
@@ -3895,7 +3891,7 @@
         <v>0</v>
       </c>
       <c r="FR6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="FS6" t="n">
         <v>28</v>
@@ -4351,13 +4347,13 @@
         <v>1.0929</v>
       </c>
       <c r="EX7" t="n">
-        <v>1.0871</v>
+        <v>1.0869</v>
       </c>
       <c r="EY7" t="n">
-        <v>1.0891</v>
+        <v>1.0889</v>
       </c>
       <c r="EZ7" t="n">
-        <v>1.0924</v>
+        <v>1.0914</v>
       </c>
       <c r="FA7" t="n">
         <v>0</v>
@@ -4368,10 +4364,12 @@
       <c r="FC7" t="b">
         <v>1</v>
       </c>
-      <c r="FD7" t="inlineStr"/>
+      <c r="FD7" s="2" t="n">
+        <v>45488.70833333334</v>
+      </c>
       <c r="FE7" t="inlineStr"/>
       <c r="FF7" s="2" t="n">
-        <v>45489.67371527778</v>
+        <v>45484.76215277778</v>
       </c>
       <c r="FG7" s="2" t="n">
         <v>45482.33333333334</v>
@@ -4402,7 +4400,7 @@
         <v>-83.36</v>
       </c>
       <c r="FO7" t="n">
-        <v>658.05</v>
+        <v>199.33</v>
       </c>
       <c r="FP7" t="b">
         <v>0</v>
@@ -4411,7 +4409,7 @@
         <v>0</v>
       </c>
       <c r="FR7" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="FS7" t="n">
         <v>28</v>
@@ -4872,10 +4870,10 @@
         <v>1.08631</v>
       </c>
       <c r="EY8" t="n">
-        <v>1.08111</v>
+        <v>1.07931</v>
       </c>
       <c r="EZ8" t="n">
-        <v>1.08081</v>
+        <v>1.07881</v>
       </c>
       <c r="FA8" t="n">
         <v>1</v>
@@ -4920,7 +4918,7 @@
         <v>-4.71</v>
       </c>
       <c r="FO8" t="n">
-        <v>653.3399999999999</v>
+        <v>194.62</v>
       </c>
       <c r="FP8" t="b">
         <v>0</v>
@@ -4929,7 +4927,7 @@
         <v>0</v>
       </c>
       <c r="FR8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="FS8" t="n">
         <v>28</v>
@@ -5388,10 +5386,10 @@
         <v>1.08594</v>
       </c>
       <c r="EY9" t="n">
-        <v>1.08074</v>
+        <v>1.07894</v>
       </c>
       <c r="EZ9" t="n">
-        <v>1.08044</v>
+        <v>1.07844</v>
       </c>
       <c r="FA9" t="n">
         <v>1</v>
@@ -5436,7 +5434,7 @@
         <v>-24.07</v>
       </c>
       <c r="FO9" t="n">
-        <v>629.2699999999999</v>
+        <v>170.55</v>
       </c>
       <c r="FP9" t="b">
         <v>0</v>
@@ -5445,7 +5443,7 @@
         <v>0</v>
       </c>
       <c r="FR9" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="FS9" t="n">
         <v>28</v>
@@ -5899,13 +5897,13 @@
         <v>1.09139</v>
       </c>
       <c r="EX10" t="n">
-        <v>1.08159</v>
+        <v>1.08739</v>
       </c>
       <c r="EY10" t="n">
-        <v>1.08359</v>
+        <v>1.08939</v>
       </c>
       <c r="EZ10" t="n">
-        <v>1.08489</v>
+        <v>1.09289</v>
       </c>
       <c r="FA10" t="n">
         <v>0</v>
@@ -5917,13 +5915,13 @@
         <v>1</v>
       </c>
       <c r="FD10" s="2" t="n">
-        <v>45484.625</v>
+        <v>45490.5</v>
       </c>
       <c r="FE10" s="2" t="n">
         <v>45488.5390162037</v>
       </c>
       <c r="FF10" s="2" t="n">
-        <v>45483.36490740741</v>
+        <v>45489.67251157408</v>
       </c>
       <c r="FG10" s="2" t="n">
         <v>45483.20833333334</v>
@@ -5932,10 +5930,10 @@
         <v>1.08139</v>
       </c>
       <c r="FI10" s="2" t="n">
-        <v>45483.36490740741</v>
+        <v>45488.5390162037</v>
       </c>
       <c r="FJ10" t="n">
-        <v>1.08161</v>
+        <v>1.09135</v>
       </c>
       <c r="FK10" t="inlineStr">
         <is>
@@ -5947,14 +5945,14 @@
       </c>
       <c r="FM10" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>success</t>
         </is>
       </c>
       <c r="FN10" t="n">
-        <v>11.53</v>
+        <v>522.16</v>
       </c>
       <c r="FO10" t="n">
-        <v>640.7999999999998</v>
+        <v>692.7099999999999</v>
       </c>
       <c r="FP10" t="b">
         <v>1</v>
@@ -6421,13 +6419,13 @@
         <v>1.09295</v>
       </c>
       <c r="EX11" t="n">
-        <v>1.08315</v>
+        <v>1.08695</v>
       </c>
       <c r="EY11" t="n">
-        <v>1.08515</v>
+        <v>1.08895</v>
       </c>
       <c r="EZ11" t="n">
-        <v>1.08645</v>
+        <v>1.09145</v>
       </c>
       <c r="FA11" t="n">
         <v>0</v>
@@ -6439,13 +6437,13 @@
         <v>1</v>
       </c>
       <c r="FD11" s="2" t="n">
-        <v>45484.66666666666</v>
+        <v>45488.70833333334</v>
       </c>
       <c r="FE11" s="2" t="n">
         <v>45490.48670138889</v>
       </c>
       <c r="FF11" s="2" t="n">
-        <v>45484.40766203704</v>
+        <v>45484.76212962963</v>
       </c>
       <c r="FG11" s="2" t="n">
         <v>45484</v>
@@ -6454,10 +6452,10 @@
         <v>1.08295</v>
       </c>
       <c r="FI11" s="2" t="n">
-        <v>45484.40766203704</v>
+        <v>45484.76212962963</v>
       </c>
       <c r="FJ11" t="n">
-        <v>1.08315</v>
+        <v>1.08698</v>
       </c>
       <c r="FK11" t="inlineStr">
         <is>
@@ -6473,10 +6471,10 @@
         </is>
       </c>
       <c r="FN11" t="n">
-        <v>10.49</v>
+        <v>211.27</v>
       </c>
       <c r="FO11" t="n">
-        <v>651.2899999999998</v>
+        <v>903.9799999999999</v>
       </c>
       <c r="FP11" t="b">
         <v>1</v>
@@ -6943,13 +6941,13 @@
         <v>1.09321</v>
       </c>
       <c r="EX12" t="n">
-        <v>1.08341</v>
+        <v>1.08721</v>
       </c>
       <c r="EY12" t="n">
-        <v>1.08541</v>
+        <v>1.08921</v>
       </c>
       <c r="EZ12" t="n">
-        <v>1.08671</v>
+        <v>1.09171</v>
       </c>
       <c r="FA12" t="n">
         <v>0</v>
@@ -6961,13 +6959,13 @@
         <v>1</v>
       </c>
       <c r="FD12" s="2" t="n">
-        <v>45484.66666666666</v>
+        <v>45490.5</v>
       </c>
       <c r="FE12" s="2" t="n">
         <v>45490.48873842593</v>
       </c>
       <c r="FF12" s="2" t="n">
-        <v>45484.37494212963</v>
+        <v>45489.67362268519</v>
       </c>
       <c r="FG12" s="2" t="n">
         <v>45484.08333333334</v>
@@ -6976,10 +6974,10 @@
         <v>1.08321</v>
       </c>
       <c r="FI12" s="2" t="n">
-        <v>45484.37494212963</v>
+        <v>45489.67362268519</v>
       </c>
       <c r="FJ12" t="n">
-        <v>1.08341</v>
+        <v>1.08723</v>
       </c>
       <c r="FK12" t="inlineStr">
         <is>
@@ -6995,10 +6993,10 @@
         </is>
       </c>
       <c r="FN12" t="n">
-        <v>10.49</v>
+        <v>210.75</v>
       </c>
       <c r="FO12" t="n">
-        <v>661.7799999999999</v>
+        <v>1114.73</v>
       </c>
       <c r="FP12" t="b">
         <v>1</v>
@@ -7465,13 +7463,13 @@
         <v>1.09466</v>
       </c>
       <c r="EX13" t="n">
-        <v>1.08486</v>
+        <v>1.08666</v>
       </c>
       <c r="EY13" t="n">
-        <v>1.08686</v>
+        <v>1.08866</v>
       </c>
       <c r="EZ13" t="n">
-        <v>1.08816</v>
+        <v>1.09016</v>
       </c>
       <c r="FA13" t="n">
         <v>0</v>
@@ -7483,13 +7481,13 @@
         <v>1</v>
       </c>
       <c r="FD13" s="2" t="n">
-        <v>45484.66666666666</v>
+        <v>45485.75</v>
       </c>
       <c r="FE13" s="2" t="n">
         <v>45490.69358796296</v>
       </c>
       <c r="FF13" s="2" t="n">
-        <v>45484.63805555556</v>
+        <v>45484.77487268519</v>
       </c>
       <c r="FG13" s="2" t="n">
         <v>45484.5</v>
@@ -7498,10 +7496,10 @@
         <v>1.08466</v>
       </c>
       <c r="FI13" s="2" t="n">
-        <v>45484.63805555556</v>
+        <v>45484.77487268519</v>
       </c>
       <c r="FJ13" t="n">
-        <v>1.08485</v>
+        <v>1.08666</v>
       </c>
       <c r="FK13" t="inlineStr">
         <is>
@@ -7517,10 +7515,10 @@
         </is>
       </c>
       <c r="FN13" t="n">
-        <v>9.960000000000001</v>
+        <v>104.85</v>
       </c>
       <c r="FO13" t="n">
-        <v>671.7399999999999</v>
+        <v>1219.58</v>
       </c>
       <c r="FP13" t="b">
         <v>1</v>
@@ -7989,13 +7987,13 @@
         <v>1.09893</v>
       </c>
       <c r="EX14" t="n">
-        <v>1.08913</v>
+        <v>1.09093</v>
       </c>
       <c r="EY14" t="n">
-        <v>1.09113</v>
+        <v>1.09293</v>
       </c>
       <c r="EZ14" t="n">
-        <v>1.09243</v>
+        <v>1.09443</v>
       </c>
       <c r="FA14" t="n">
         <v>0</v>
@@ -8006,12 +8004,10 @@
       <c r="FC14" t="b">
         <v>1</v>
       </c>
-      <c r="FD14" s="2" t="n">
-        <v>45490.5</v>
-      </c>
+      <c r="FD14" t="inlineStr"/>
       <c r="FE14" t="inlineStr"/>
       <c r="FF14" s="2" t="n">
-        <v>45488.00005787037</v>
+        <v>45488.73413194445</v>
       </c>
       <c r="FG14" s="2" t="n">
         <v>45485.58333333334</v>
@@ -8020,10 +8016,10 @@
         <v>1.08893</v>
       </c>
       <c r="FI14" s="2" t="n">
-        <v>45488.00005787037</v>
+        <v>45488.73413194445</v>
       </c>
       <c r="FJ14" t="n">
-        <v>1.08821</v>
+        <v>1.09094</v>
       </c>
       <c r="FK14" t="inlineStr">
         <is>
@@ -8039,10 +8035,10 @@
         </is>
       </c>
       <c r="FN14" t="n">
-        <v>-37.75</v>
+        <v>105.38</v>
       </c>
       <c r="FO14" t="n">
-        <v>633.9899999999999</v>
+        <v>1324.96</v>
       </c>
       <c r="FP14" t="b">
         <v>1</v>
@@ -8511,13 +8507,13 @@
         <v>1.09877</v>
       </c>
       <c r="EX15" t="n">
-        <v>1.08897</v>
+        <v>1.09077</v>
       </c>
       <c r="EY15" t="n">
-        <v>1.09097</v>
+        <v>1.09277</v>
       </c>
       <c r="EZ15" t="n">
-        <v>1.09227</v>
+        <v>1.09427</v>
       </c>
       <c r="FA15" t="n">
         <v>0</v>
@@ -8529,11 +8525,11 @@
         <v>1</v>
       </c>
       <c r="FD15" s="2" t="n">
-        <v>45490.5</v>
+        <v>45490.54166666666</v>
       </c>
       <c r="FE15" t="inlineStr"/>
       <c r="FF15" s="2" t="n">
-        <v>45488.38890046296</v>
+        <v>45488.7349537037</v>
       </c>
       <c r="FG15" s="2" t="n">
         <v>45488.16666666666</v>
@@ -8542,10 +8538,10 @@
         <v>1.08877</v>
       </c>
       <c r="FI15" s="2" t="n">
-        <v>45488.38890046296</v>
+        <v>45488.7349537037</v>
       </c>
       <c r="FJ15" t="n">
-        <v>1.08897</v>
+        <v>1.09078</v>
       </c>
       <c r="FK15" t="inlineStr">
         <is>
@@ -8561,10 +8557,10 @@
         </is>
       </c>
       <c r="FN15" t="n">
-        <v>10.49</v>
+        <v>105.38</v>
       </c>
       <c r="FO15" t="n">
-        <v>644.4799999999999</v>
+        <v>1430.34</v>
       </c>
       <c r="FP15" t="b">
         <v>1</v>
@@ -9035,13 +9031,13 @@
         <v>1.10121</v>
       </c>
       <c r="EX16" t="n">
-        <v>1.09141</v>
+        <v>1.09321</v>
       </c>
       <c r="EY16" t="n">
-        <v>1.09341</v>
+        <v>1.09521</v>
       </c>
       <c r="EZ16" t="n">
-        <v>1.09471</v>
+        <v>1.09671</v>
       </c>
       <c r="FA16" t="n">
         <v>0</v>
@@ -9055,7 +9051,7 @@
       <c r="FD16" t="inlineStr"/>
       <c r="FE16" t="inlineStr"/>
       <c r="FF16" s="2" t="n">
-        <v>45491.6875</v>
+        <v>45490.57293981482</v>
       </c>
       <c r="FG16" s="2" t="n">
         <v>45488.54166666666</v>
@@ -9086,7 +9082,7 @@
         <v>-166.71</v>
       </c>
       <c r="FO16" t="n">
-        <v>477.7699999999999</v>
+        <v>1263.63</v>
       </c>
       <c r="FP16" t="b">
         <v>0</v>
@@ -9557,13 +9553,13 @@
         <v>1.10146</v>
       </c>
       <c r="EX17" t="n">
-        <v>1.09166</v>
+        <v>1.09346</v>
       </c>
       <c r="EY17" t="n">
-        <v>1.09366</v>
+        <v>1.09546</v>
       </c>
       <c r="EZ17" t="n">
-        <v>1.09496</v>
+        <v>1.09696</v>
       </c>
       <c r="FA17" t="n">
         <v>0</v>
@@ -9577,7 +9573,7 @@
       <c r="FD17" t="inlineStr"/>
       <c r="FE17" t="inlineStr"/>
       <c r="FF17" s="2" t="n">
-        <v>45491.68225694444</v>
+        <v>45490.57129629629</v>
       </c>
       <c r="FG17" s="2" t="n">
         <v>45488.70833333334</v>
@@ -9608,7 +9604,7 @@
         <v>-179.82</v>
       </c>
       <c r="FO17" t="n">
-        <v>297.9499999999999</v>
+        <v>1083.81</v>
       </c>
       <c r="FP17" t="b">
         <v>0</v>
@@ -10082,10 +10078,10 @@
         <v>1.093</v>
       </c>
       <c r="EY18" t="n">
-        <v>1.0878</v>
+        <v>1.086</v>
       </c>
       <c r="EZ18" t="n">
-        <v>1.0875</v>
+        <v>1.0855</v>
       </c>
       <c r="FA18" t="n">
         <v>1</v>
@@ -10097,7 +10093,7 @@
         <v>0</v>
       </c>
       <c r="FD18" s="2" t="n">
-        <v>45496.54166666666</v>
+        <v>45496.70833333334</v>
       </c>
       <c r="FE18" t="inlineStr"/>
       <c r="FF18" s="2" t="n">
@@ -10132,7 +10128,7 @@
         <v>-42.92</v>
       </c>
       <c r="FO18" t="n">
-        <v>255.0299999999999</v>
+        <v>1040.89</v>
       </c>
       <c r="FP18" t="b">
         <v>0</v>
@@ -10601,13 +10597,13 @@
         <v>1.09881</v>
       </c>
       <c r="EX19" t="n">
-        <v>1.09101</v>
+        <v>1.09281</v>
       </c>
       <c r="EY19" t="n">
-        <v>1.09301</v>
+        <v>1.09481</v>
       </c>
       <c r="EZ19" t="n">
-        <v>1.09531</v>
+        <v>1.09731</v>
       </c>
       <c r="FA19" t="n">
         <v>0</v>
@@ -10621,7 +10617,7 @@
       <c r="FD19" t="inlineStr"/>
       <c r="FE19" t="inlineStr"/>
       <c r="FF19" s="2" t="n">
-        <v>45491.70299768518</v>
+        <v>45490.75840277778</v>
       </c>
       <c r="FG19" s="2" t="n">
         <v>45489.83333333334</v>
@@ -10630,10 +10626,10 @@
         <v>1.08881</v>
       </c>
       <c r="FI19" s="2" t="n">
-        <v>45491.70299768518</v>
+        <v>45490.75840277778</v>
       </c>
       <c r="FJ19" t="n">
-        <v>1.09103</v>
+        <v>1.09281</v>
       </c>
       <c r="FK19" t="inlineStr">
         <is>
@@ -10649,10 +10645,10 @@
         </is>
       </c>
       <c r="FN19" t="n">
-        <v>116.38</v>
+        <v>209.7</v>
       </c>
       <c r="FO19" t="n">
-        <v>371.4099999999999</v>
+        <v>1250.59</v>
       </c>
       <c r="FP19" t="b">
         <v>1</v>
@@ -11123,13 +11119,13 @@
         <v>1.10016</v>
       </c>
       <c r="EX20" t="n">
-        <v>1.09236</v>
+        <v>1.09216</v>
       </c>
       <c r="EY20" t="n">
-        <v>1.09436</v>
+        <v>1.09416</v>
       </c>
       <c r="EZ20" t="n">
-        <v>1.09666</v>
+        <v>1.09566</v>
       </c>
       <c r="FA20" t="n">
         <v>0</v>
@@ -11143,7 +11139,7 @@
       <c r="FD20" t="inlineStr"/>
       <c r="FE20" t="inlineStr"/>
       <c r="FF20" s="2" t="n">
-        <v>45490.80766203703</v>
+        <v>45491.67153935185</v>
       </c>
       <c r="FG20" s="2" t="n">
         <v>45490.20833333334</v>
@@ -11152,10 +11148,10 @@
         <v>1.09016</v>
       </c>
       <c r="FI20" s="2" t="n">
-        <v>45490.80766203703</v>
+        <v>45491.67153935185</v>
       </c>
       <c r="FJ20" t="n">
-        <v>1.09238</v>
+        <v>1.09219</v>
       </c>
       <c r="FK20" t="inlineStr">
         <is>
@@ -11171,10 +11167,10 @@
         </is>
       </c>
       <c r="FN20" t="n">
-        <v>116.38</v>
+        <v>106.42</v>
       </c>
       <c r="FO20" t="n">
-        <v>487.7899999999998</v>
+        <v>1357.01</v>
       </c>
       <c r="FP20" t="b">
         <v>1</v>
@@ -11645,13 +11641,13 @@
         <v>1.10076</v>
       </c>
       <c r="EX21" t="n">
-        <v>1.09296</v>
+        <v>1.09276</v>
       </c>
       <c r="EY21" t="n">
-        <v>1.09496</v>
+        <v>1.09476</v>
       </c>
       <c r="EZ21" t="n">
-        <v>1.09726</v>
+        <v>1.09626</v>
       </c>
       <c r="FA21" t="n">
         <v>0</v>
@@ -11665,7 +11661,7 @@
       <c r="FD21" t="inlineStr"/>
       <c r="FE21" t="inlineStr"/>
       <c r="FF21" s="2" t="n">
-        <v>45490.57976851852</v>
+        <v>45490.75863425926</v>
       </c>
       <c r="FG21" s="2" t="n">
         <v>45490.45833333334</v>
@@ -11674,10 +11670,10 @@
         <v>1.09076</v>
       </c>
       <c r="FI21" s="2" t="n">
-        <v>45490.57976851852</v>
+        <v>45490.75863425926</v>
       </c>
       <c r="FJ21" t="n">
-        <v>1.09296</v>
+        <v>1.09279</v>
       </c>
       <c r="FK21" t="inlineStr">
         <is>
@@ -11693,10 +11689,10 @@
         </is>
       </c>
       <c r="FN21" t="n">
-        <v>115.34</v>
+        <v>106.42</v>
       </c>
       <c r="FO21" t="n">
-        <v>603.1299999999999</v>
+        <v>1463.43</v>
       </c>
       <c r="FP21" t="b">
         <v>1</v>
@@ -12170,10 +12166,10 @@
         <v>1.08913</v>
       </c>
       <c r="EY22" t="n">
-        <v>1.09433</v>
+        <v>1.09613</v>
       </c>
       <c r="EZ22" t="n">
-        <v>1.09463</v>
+        <v>1.09663</v>
       </c>
       <c r="FA22" t="n">
         <v>0</v>
@@ -12218,7 +12214,7 @@
         <v>-235.39</v>
       </c>
       <c r="FO22" t="n">
-        <v>367.7399999999999</v>
+        <v>1228.04</v>
       </c>
       <c r="FP22" t="b">
         <v>0</v>
@@ -12685,13 +12681,13 @@
         <v>1.07965</v>
       </c>
       <c r="EX23" t="n">
-        <v>1.08945</v>
+        <v>1.08565</v>
       </c>
       <c r="EY23" t="n">
-        <v>1.08745</v>
+        <v>1.08365</v>
       </c>
       <c r="EZ23" t="n">
-        <v>1.08615</v>
+        <v>1.08115</v>
       </c>
       <c r="FA23" t="n">
         <v>1</v>
@@ -12702,12 +12698,10 @@
       <c r="FC23" t="b">
         <v>1</v>
       </c>
-      <c r="FD23" s="2" t="n">
-        <v>45496.58333333334</v>
-      </c>
+      <c r="FD23" t="inlineStr"/>
       <c r="FE23" t="inlineStr"/>
       <c r="FF23" s="2" t="n">
-        <v>45495.06579861111</v>
+        <v>45497.665</v>
       </c>
       <c r="FG23" s="2" t="n">
         <v>45491.95833333334</v>
@@ -12716,10 +12710,10 @@
         <v>1.08965</v>
       </c>
       <c r="FI23" s="2" t="n">
-        <v>45495.06579861111</v>
+        <v>45497.665</v>
       </c>
       <c r="FJ23" t="n">
-        <v>1.08942</v>
+        <v>1.08564</v>
       </c>
       <c r="FK23" t="inlineStr">
         <is>
@@ -12735,10 +12729,10 @@
         </is>
       </c>
       <c r="FN23" t="n">
-        <v>12.04</v>
+        <v>209.87</v>
       </c>
       <c r="FO23" t="n">
-        <v>379.7799999999999</v>
+        <v>1437.91</v>
       </c>
       <c r="FP23" t="b">
         <v>1</v>
@@ -13205,13 +13199,13 @@
         <v>1.07914</v>
       </c>
       <c r="EX24" t="n">
-        <v>1.08894</v>
+        <v>1.08514</v>
       </c>
       <c r="EY24" t="n">
-        <v>1.08694</v>
+        <v>1.08314</v>
       </c>
       <c r="EZ24" t="n">
-        <v>1.08564</v>
+        <v>1.08064</v>
       </c>
       <c r="FA24" t="n">
         <v>1</v>
@@ -13222,12 +13216,10 @@
       <c r="FC24" t="b">
         <v>1</v>
       </c>
-      <c r="FD24" s="2" t="n">
-        <v>45496.66666666666</v>
-      </c>
+      <c r="FD24" t="inlineStr"/>
       <c r="FE24" t="inlineStr"/>
       <c r="FF24" s="2" t="n">
-        <v>45492.37384259259</v>
+        <v>45497.65738425926</v>
       </c>
       <c r="FG24" s="2" t="n">
         <v>45492.16666666666</v>
@@ -13236,14 +13228,14 @@
         <v>1.08914</v>
       </c>
       <c r="FI24" s="2" t="n">
-        <v>45492.37384259259</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ24" t="n">
-        <v>1.08894</v>
+        <v>1.08935</v>
       </c>
       <c r="FK24" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL24" t="n">
@@ -13251,23 +13243,23 @@
       </c>
       <c r="FM24" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN24" t="n">
-        <v>10.47</v>
+        <v>-10.99</v>
       </c>
       <c r="FO24" t="n">
-        <v>390.2499999999999</v>
+        <v>1426.92</v>
       </c>
       <c r="FP24" t="b">
+        <v>0</v>
+      </c>
+      <c r="FQ24" t="n">
+        <v>0</v>
+      </c>
+      <c r="FR24" t="n">
         <v>1</v>
-      </c>
-      <c r="FQ24" t="n">
-        <v>2</v>
-      </c>
-      <c r="FR24" t="n">
-        <v>0</v>
       </c>
       <c r="FS24" t="n">
         <v>29</v>
@@ -13725,13 +13717,13 @@
         <v>1.07869</v>
       </c>
       <c r="EX25" t="n">
-        <v>1.08849</v>
+        <v>1.08669</v>
       </c>
       <c r="EY25" t="n">
-        <v>1.08649</v>
+        <v>1.08469</v>
       </c>
       <c r="EZ25" t="n">
-        <v>1.08519</v>
+        <v>1.08319</v>
       </c>
       <c r="FA25" t="n">
         <v>1</v>
@@ -13743,11 +13735,11 @@
         <v>1</v>
       </c>
       <c r="FD25" s="2" t="n">
-        <v>45496.70833333334</v>
+        <v>45497.45833333334</v>
       </c>
       <c r="FE25" t="inlineStr"/>
       <c r="FF25" s="2" t="n">
-        <v>45492.56184027778</v>
+        <v>45496.5972800926</v>
       </c>
       <c r="FG25" s="2" t="n">
         <v>45492.20833333334</v>
@@ -13756,14 +13748,14 @@
         <v>1.08869</v>
       </c>
       <c r="FI25" s="2" t="n">
-        <v>45492.56184027778</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ25" t="n">
-        <v>1.08848</v>
+        <v>1.08935</v>
       </c>
       <c r="FK25" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL25" t="n">
@@ -13771,23 +13763,23 @@
       </c>
       <c r="FM25" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN25" t="n">
-        <v>10.99</v>
+        <v>-34.54</v>
       </c>
       <c r="FO25" t="n">
-        <v>401.24</v>
+        <v>1392.38</v>
       </c>
       <c r="FP25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="FR25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="FS25" t="n">
         <v>29</v>
@@ -14245,13 +14237,13 @@
         <v>1.07877</v>
       </c>
       <c r="EX26" t="n">
-        <v>1.08857</v>
+        <v>1.08677</v>
       </c>
       <c r="EY26" t="n">
-        <v>1.08657</v>
+        <v>1.08477</v>
       </c>
       <c r="EZ26" t="n">
-        <v>1.08527</v>
+        <v>1.08327</v>
       </c>
       <c r="FA26" t="n">
         <v>1</v>
@@ -14263,11 +14255,11 @@
         <v>1</v>
       </c>
       <c r="FD26" s="2" t="n">
-        <v>45496.70833333334</v>
+        <v>45497.45833333334</v>
       </c>
       <c r="FE26" t="inlineStr"/>
       <c r="FF26" s="2" t="n">
-        <v>45492.57520833334</v>
+        <v>45496.60076388889</v>
       </c>
       <c r="FG26" s="2" t="n">
         <v>45492.29166666666</v>
@@ -14276,14 +14268,14 @@
         <v>1.08877</v>
       </c>
       <c r="FI26" s="2" t="n">
-        <v>45492.57520833334</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ26" t="n">
-        <v>1.08856</v>
+        <v>1.08935</v>
       </c>
       <c r="FK26" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL26" t="n">
@@ -14291,23 +14283,23 @@
       </c>
       <c r="FM26" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN26" t="n">
-        <v>10.99</v>
+        <v>-30.35</v>
       </c>
       <c r="FO26" t="n">
-        <v>412.23</v>
+        <v>1362.03</v>
       </c>
       <c r="FP26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ26" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="FR26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="FS26" t="n">
         <v>29</v>
@@ -14765,13 +14757,13 @@
         <v>1.07843</v>
       </c>
       <c r="EX27" t="n">
-        <v>1.08823</v>
+        <v>1.08443</v>
       </c>
       <c r="EY27" t="n">
-        <v>1.08623</v>
+        <v>1.08243</v>
       </c>
       <c r="EZ27" t="n">
-        <v>1.08493</v>
+        <v>1.07993</v>
       </c>
       <c r="FA27" t="n">
         <v>1</v>
@@ -14782,12 +14774,10 @@
       <c r="FC27" t="b">
         <v>1</v>
       </c>
-      <c r="FD27" s="2" t="n">
-        <v>45496.70833333334</v>
-      </c>
+      <c r="FD27" t="inlineStr"/>
       <c r="FE27" t="inlineStr"/>
       <c r="FF27" s="2" t="n">
-        <v>45492.531875</v>
+        <v>45497.56241898148</v>
       </c>
       <c r="FG27" s="2" t="n">
         <v>45492.41666666666</v>
@@ -14796,14 +14786,14 @@
         <v>1.08843</v>
       </c>
       <c r="FI27" s="2" t="n">
-        <v>45492.531875</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ27" t="n">
-        <v>1.08823</v>
+        <v>1.08935</v>
       </c>
       <c r="FK27" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL27" t="n">
@@ -14811,23 +14801,23 @@
       </c>
       <c r="FM27" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN27" t="n">
-        <v>10.47</v>
+        <v>-48.15</v>
       </c>
       <c r="FO27" t="n">
-        <v>422.7</v>
+        <v>1313.88</v>
       </c>
       <c r="FP27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ27" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="FR27" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="FS27" t="n">
         <v>29</v>
@@ -15285,13 +15275,13 @@
         <v>1.07784</v>
       </c>
       <c r="EX28" t="n">
-        <v>1.08564</v>
+        <v>1.08584</v>
       </c>
       <c r="EY28" t="n">
-        <v>1.08364</v>
+        <v>1.08384</v>
       </c>
       <c r="EZ28" t="n">
-        <v>1.08134</v>
+        <v>1.08234</v>
       </c>
       <c r="FA28" t="n">
         <v>1</v>
@@ -15305,7 +15295,7 @@
       <c r="FD28" t="inlineStr"/>
       <c r="FE28" t="inlineStr"/>
       <c r="FF28" s="2" t="n">
-        <v>45497.66497685185</v>
+        <v>45497.66546296296</v>
       </c>
       <c r="FG28" s="2" t="n">
         <v>45492.5</v>
@@ -15336,7 +15326,7 @@
         <v>-79.03</v>
       </c>
       <c r="FO28" t="n">
-        <v>343.67</v>
+        <v>1234.85</v>
       </c>
       <c r="FP28" t="b">
         <v>0</v>
@@ -15345,7 +15335,7 @@
         <v>0</v>
       </c>
       <c r="FR28" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="FS28" t="n">
         <v>29</v>
@@ -15805,13 +15795,13 @@
         <v>1.07884</v>
       </c>
       <c r="EX29" t="n">
-        <v>1.08864</v>
+        <v>1.08484</v>
       </c>
       <c r="EY29" t="n">
-        <v>1.08664</v>
+        <v>1.08284</v>
       </c>
       <c r="EZ29" t="n">
-        <v>1.08534</v>
+        <v>1.08034</v>
       </c>
       <c r="FA29" t="n">
         <v>1</v>
@@ -15822,12 +15812,10 @@
       <c r="FC29" t="b">
         <v>1</v>
       </c>
-      <c r="FD29" s="2" t="n">
-        <v>45496.70833333334</v>
-      </c>
+      <c r="FD29" t="inlineStr"/>
       <c r="FE29" t="inlineStr"/>
       <c r="FF29" s="2" t="n">
-        <v>45492.71457175926</v>
+        <v>45497.62979166667</v>
       </c>
       <c r="FG29" s="2" t="n">
         <v>45492.66666666666</v>
@@ -15836,14 +15824,14 @@
         <v>1.08884</v>
       </c>
       <c r="FI29" s="2" t="n">
-        <v>45492.71457175926</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ29" t="n">
-        <v>1.08864</v>
+        <v>1.08935</v>
       </c>
       <c r="FK29" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL29" t="n">
@@ -15851,23 +15839,23 @@
       </c>
       <c r="FM29" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN29" t="n">
-        <v>10.47</v>
+        <v>-26.69</v>
       </c>
       <c r="FO29" t="n">
-        <v>354.14</v>
+        <v>1208.16</v>
       </c>
       <c r="FP29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FR29" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="FS29" t="n">
         <v>29</v>
@@ -16329,13 +16317,13 @@
         <v>1.07808</v>
       </c>
       <c r="EX30" t="n">
-        <v>1.08788</v>
+        <v>1.08608</v>
       </c>
       <c r="EY30" t="n">
-        <v>1.08588</v>
+        <v>1.08408</v>
       </c>
       <c r="EZ30" t="n">
-        <v>1.08458</v>
+        <v>1.08258</v>
       </c>
       <c r="FA30" t="n">
         <v>1</v>
@@ -16346,12 +16334,10 @@
       <c r="FC30" t="b">
         <v>1</v>
       </c>
-      <c r="FD30" s="2" t="n">
-        <v>45496.75</v>
-      </c>
+      <c r="FD30" t="inlineStr"/>
       <c r="FE30" t="inlineStr"/>
       <c r="FF30" s="2" t="n">
-        <v>45496.48717592593</v>
+        <v>45497.67377314815</v>
       </c>
       <c r="FG30" s="2" t="n">
         <v>45492.70833333334</v>
@@ -16382,7 +16368,7 @@
         <v>-66.47</v>
       </c>
       <c r="FO30" t="n">
-        <v>287.67</v>
+        <v>1141.69</v>
       </c>
       <c r="FP30" t="b">
         <v>0</v>
@@ -16391,7 +16377,7 @@
         <v>0</v>
       </c>
       <c r="FR30" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="FS30" t="n">
         <v>29</v>
@@ -16853,13 +16839,13 @@
         <v>1.07874</v>
       </c>
       <c r="EX31" t="n">
-        <v>1.08854</v>
+        <v>1.08674</v>
       </c>
       <c r="EY31" t="n">
-        <v>1.08654</v>
+        <v>1.08474</v>
       </c>
       <c r="EZ31" t="n">
-        <v>1.08524</v>
+        <v>1.08324</v>
       </c>
       <c r="FA31" t="n">
         <v>1</v>
@@ -16871,11 +16857,11 @@
         <v>1</v>
       </c>
       <c r="FD31" s="2" t="n">
-        <v>45496.70833333334</v>
+        <v>45497.45833333334</v>
       </c>
       <c r="FE31" t="inlineStr"/>
       <c r="FF31" s="2" t="n">
-        <v>45495.04167824074</v>
+        <v>45496.60041666667</v>
       </c>
       <c r="FG31" s="2" t="n">
         <v>45492.79166666666</v>
@@ -16884,14 +16870,14 @@
         <v>1.08874</v>
       </c>
       <c r="FI31" s="2" t="n">
-        <v>45495.04167824074</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ31" t="n">
-        <v>1.08865</v>
+        <v>1.08935</v>
       </c>
       <c r="FK31" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL31" t="n">
@@ -16899,23 +16885,23 @@
       </c>
       <c r="FM31" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN31" t="n">
-        <v>4.71</v>
+        <v>-31.92</v>
       </c>
       <c r="FO31" t="n">
-        <v>292.3799999999999</v>
+        <v>1109.77</v>
       </c>
       <c r="FP31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FR31" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="FS31" t="n">
         <v>29</v>
@@ -17377,13 +17363,13 @@
         <v>1.07843</v>
       </c>
       <c r="EX32" t="n">
-        <v>1.08823</v>
+        <v>1.08443</v>
       </c>
       <c r="EY32" t="n">
-        <v>1.08623</v>
+        <v>1.08243</v>
       </c>
       <c r="EZ32" t="n">
-        <v>1.08493</v>
+        <v>1.07993</v>
       </c>
       <c r="FA32" t="n">
         <v>1</v>
@@ -17394,12 +17380,10 @@
       <c r="FC32" t="b">
         <v>1</v>
       </c>
-      <c r="FD32" s="2" t="n">
-        <v>45496.70833333334</v>
-      </c>
+      <c r="FD32" t="inlineStr"/>
       <c r="FE32" t="inlineStr"/>
       <c r="FF32" s="2" t="n">
-        <v>45492.98961805556</v>
+        <v>45497.56241898148</v>
       </c>
       <c r="FG32" s="2" t="n">
         <v>45492.83333333334</v>
@@ -17408,14 +17392,14 @@
         <v>1.08843</v>
       </c>
       <c r="FI32" s="2" t="n">
-        <v>45492.98961805556</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ32" t="n">
-        <v>1.08822</v>
+        <v>1.08935</v>
       </c>
       <c r="FK32" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL32" t="n">
@@ -17423,23 +17407,23 @@
       </c>
       <c r="FM32" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN32" t="n">
-        <v>10.99</v>
+        <v>-48.15</v>
       </c>
       <c r="FO32" t="n">
-        <v>303.3699999999999</v>
+        <v>1061.62</v>
       </c>
       <c r="FP32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ32" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="FR32" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="FS32" t="n">
         <v>29</v>
@@ -17901,13 +17885,13 @@
         <v>1.07781</v>
       </c>
       <c r="EX33" t="n">
-        <v>1.08561</v>
+        <v>1.08581</v>
       </c>
       <c r="EY33" t="n">
-        <v>1.08361</v>
+        <v>1.08381</v>
       </c>
       <c r="EZ33" t="n">
-        <v>1.08131</v>
+        <v>1.08231</v>
       </c>
       <c r="FA33" t="n">
         <v>1</v>
@@ -17921,7 +17905,7 @@
       <c r="FD33" t="inlineStr"/>
       <c r="FE33" t="inlineStr"/>
       <c r="FF33" s="2" t="n">
-        <v>45497.66459490741</v>
+        <v>45497.66530092592</v>
       </c>
       <c r="FG33" s="2" t="n">
         <v>45492.91666666666</v>
@@ -17952,7 +17936,7 @@
         <v>-80.59999999999999</v>
       </c>
       <c r="FO33" t="n">
-        <v>222.77</v>
+        <v>981.0200000000001</v>
       </c>
       <c r="FP33" t="b">
         <v>0</v>
@@ -17961,7 +17945,7 @@
         <v>0</v>
       </c>
       <c r="FR33" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="FS33" t="n">
         <v>29</v>
@@ -18423,13 +18407,13 @@
         <v>1.07932</v>
       </c>
       <c r="EX34" t="n">
-        <v>1.08912</v>
+        <v>1.08532</v>
       </c>
       <c r="EY34" t="n">
-        <v>1.08712</v>
+        <v>1.08332</v>
       </c>
       <c r="EZ34" t="n">
-        <v>1.08582</v>
+        <v>1.08082</v>
       </c>
       <c r="FA34" t="n">
         <v>1</v>
@@ -18440,12 +18424,10 @@
       <c r="FC34" t="b">
         <v>1</v>
       </c>
-      <c r="FD34" s="2" t="n">
-        <v>45496.625</v>
-      </c>
+      <c r="FD34" t="inlineStr"/>
       <c r="FE34" t="inlineStr"/>
       <c r="FF34" s="2" t="n">
-        <v>45495.24118055555</v>
+        <v>45497.65844907407</v>
       </c>
       <c r="FG34" s="2" t="n">
         <v>45495.16666666666</v>
@@ -18454,14 +18436,14 @@
         <v>1.08932</v>
       </c>
       <c r="FI34" s="2" t="n">
-        <v>45495.24118055555</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ34" t="n">
-        <v>1.08914</v>
+        <v>1.08935</v>
       </c>
       <c r="FK34" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL34" t="n">
@@ -18469,23 +18451,23 @@
       </c>
       <c r="FM34" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN34" t="n">
-        <v>9.42</v>
+        <v>-1.57</v>
       </c>
       <c r="FO34" t="n">
-        <v>232.1899999999999</v>
+        <v>979.45</v>
       </c>
       <c r="FP34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FR34" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="FS34" t="n">
         <v>30</v>
@@ -18947,13 +18929,13 @@
         <v>1.07859</v>
       </c>
       <c r="EX35" t="n">
-        <v>1.08839</v>
+        <v>1.08659</v>
       </c>
       <c r="EY35" t="n">
-        <v>1.08639</v>
+        <v>1.08459</v>
       </c>
       <c r="EZ35" t="n">
-        <v>1.08509</v>
+        <v>1.08309</v>
       </c>
       <c r="FA35" t="n">
         <v>1</v>
@@ -18965,11 +18947,11 @@
         <v>1</v>
       </c>
       <c r="FD35" s="2" t="n">
-        <v>45496.70833333334</v>
+        <v>45497.45833333334</v>
       </c>
       <c r="FE35" t="inlineStr"/>
       <c r="FF35" s="2" t="n">
-        <v>45495.42172453704</v>
+        <v>45496.59525462963</v>
       </c>
       <c r="FG35" s="2" t="n">
         <v>45495.20833333334</v>
@@ -18978,14 +18960,14 @@
         <v>1.08859</v>
       </c>
       <c r="FI35" s="2" t="n">
-        <v>45495.42172453704</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ35" t="n">
-        <v>1.08834</v>
+        <v>1.08935</v>
       </c>
       <c r="FK35" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL35" t="n">
@@ -18993,23 +18975,23 @@
       </c>
       <c r="FM35" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN35" t="n">
-        <v>13.08</v>
+        <v>-39.77</v>
       </c>
       <c r="FO35" t="n">
-        <v>245.27</v>
+        <v>939.6800000000001</v>
       </c>
       <c r="FP35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ35" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="FR35" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="FS35" t="n">
         <v>30</v>
@@ -19471,13 +19453,13 @@
         <v>1.07868</v>
       </c>
       <c r="EX36" t="n">
-        <v>1.08848</v>
+        <v>1.08668</v>
       </c>
       <c r="EY36" t="n">
-        <v>1.08648</v>
+        <v>1.08468</v>
       </c>
       <c r="EZ36" t="n">
-        <v>1.08518</v>
+        <v>1.08318</v>
       </c>
       <c r="FA36" t="n">
         <v>1</v>
@@ -19489,11 +19471,11 @@
         <v>1</v>
       </c>
       <c r="FD36" s="2" t="n">
-        <v>45496.70833333334</v>
+        <v>45497.45833333334</v>
       </c>
       <c r="FE36" t="inlineStr"/>
       <c r="FF36" s="2" t="n">
-        <v>45495.42186342592</v>
+        <v>45496.59726851852</v>
       </c>
       <c r="FG36" s="2" t="n">
         <v>45495.33333333334</v>
@@ -19502,14 +19484,14 @@
         <v>1.08868</v>
       </c>
       <c r="FI36" s="2" t="n">
-        <v>45495.42186342592</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ36" t="n">
-        <v>1.08848</v>
+        <v>1.08935</v>
       </c>
       <c r="FK36" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL36" t="n">
@@ -19517,23 +19499,23 @@
       </c>
       <c r="FM36" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN36" t="n">
-        <v>10.47</v>
+        <v>-35.06</v>
       </c>
       <c r="FO36" t="n">
-        <v>255.74</v>
+        <v>904.6200000000001</v>
       </c>
       <c r="FP36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="FR36" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="FS36" t="n">
         <v>30</v>
@@ -19995,13 +19977,13 @@
         <v>1.0784</v>
       </c>
       <c r="EX37" t="n">
-        <v>1.0882</v>
+        <v>1.0844</v>
       </c>
       <c r="EY37" t="n">
-        <v>1.0862</v>
+        <v>1.0824</v>
       </c>
       <c r="EZ37" t="n">
-        <v>1.0849</v>
+        <v>1.0799</v>
       </c>
       <c r="FA37" t="n">
         <v>1</v>
@@ -20012,12 +19994,10 @@
       <c r="FC37" t="b">
         <v>1</v>
       </c>
-      <c r="FD37" s="2" t="n">
-        <v>45496.70833333334</v>
-      </c>
+      <c r="FD37" t="inlineStr"/>
       <c r="FE37" t="inlineStr"/>
       <c r="FF37" s="2" t="n">
-        <v>45495.6890162037</v>
+        <v>45497.56193287037</v>
       </c>
       <c r="FG37" s="2" t="n">
         <v>45495.375</v>
@@ -20026,14 +20006,14 @@
         <v>1.0884</v>
       </c>
       <c r="FI37" s="2" t="n">
-        <v>45495.6890162037</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ37" t="n">
-        <v>1.08817</v>
+        <v>1.08935</v>
       </c>
       <c r="FK37" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL37" t="n">
@@ -20041,23 +20021,23 @@
       </c>
       <c r="FM37" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN37" t="n">
-        <v>12.04</v>
+        <v>-49.72</v>
       </c>
       <c r="FO37" t="n">
-        <v>267.78</v>
+        <v>854.9000000000001</v>
       </c>
       <c r="FP37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ37" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="FR37" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="FS37" t="n">
         <v>30</v>
@@ -20517,13 +20497,13 @@
         <v>1.07888</v>
       </c>
       <c r="EX38" t="n">
-        <v>1.08868</v>
+        <v>1.08488</v>
       </c>
       <c r="EY38" t="n">
-        <v>1.08668</v>
+        <v>1.08288</v>
       </c>
       <c r="EZ38" t="n">
-        <v>1.08538</v>
+        <v>1.08038</v>
       </c>
       <c r="FA38" t="n">
         <v>1</v>
@@ -20534,12 +20514,10 @@
       <c r="FC38" t="b">
         <v>1</v>
       </c>
-      <c r="FD38" s="2" t="n">
-        <v>45496.70833333334</v>
-      </c>
+      <c r="FD38" t="inlineStr"/>
       <c r="FE38" t="inlineStr"/>
       <c r="FF38" s="2" t="n">
-        <v>45495.83534722222</v>
+        <v>45497.63539351852</v>
       </c>
       <c r="FG38" s="2" t="n">
         <v>45495.58333333334</v>
@@ -20548,14 +20526,14 @@
         <v>1.08888</v>
       </c>
       <c r="FI38" s="2" t="n">
-        <v>45495.83534722222</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ38" t="n">
-        <v>1.08868</v>
+        <v>1.08935</v>
       </c>
       <c r="FK38" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL38" t="n">
@@ -20563,23 +20541,23 @@
       </c>
       <c r="FM38" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN38" t="n">
-        <v>10.47</v>
+        <v>-24.6</v>
       </c>
       <c r="FO38" t="n">
-        <v>278.25</v>
+        <v>830.3000000000001</v>
       </c>
       <c r="FP38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ38" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="FR38" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="FS38" t="n">
         <v>30</v>
@@ -21039,13 +21017,13 @@
         <v>1.0785</v>
       </c>
       <c r="EX39" t="n">
-        <v>1.0883</v>
+        <v>1.0845</v>
       </c>
       <c r="EY39" t="n">
-        <v>1.0863</v>
+        <v>1.0825</v>
       </c>
       <c r="EZ39" t="n">
-        <v>1.085</v>
+        <v>1.08</v>
       </c>
       <c r="FA39" t="n">
         <v>1</v>
@@ -21056,12 +21034,10 @@
       <c r="FC39" t="b">
         <v>1</v>
       </c>
-      <c r="FD39" s="2" t="n">
-        <v>45496.70833333334</v>
-      </c>
+      <c r="FD39" t="inlineStr"/>
       <c r="FE39" t="inlineStr"/>
       <c r="FF39" s="2" t="n">
-        <v>45495.69039351852</v>
+        <v>45497.56318287037</v>
       </c>
       <c r="FG39" s="2" t="n">
         <v>45495.625</v>
@@ -21070,14 +21046,14 @@
         <v>1.0885</v>
       </c>
       <c r="FI39" s="2" t="n">
-        <v>45495.69039351852</v>
+        <v>45496.29166666666</v>
       </c>
       <c r="FJ39" t="n">
-        <v>1.0883</v>
+        <v>1.08935</v>
       </c>
       <c r="FK39" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL39" t="n">
@@ -21085,23 +21061,23 @@
       </c>
       <c r="FM39" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN39" t="n">
-        <v>10.47</v>
+        <v>-44.49</v>
       </c>
       <c r="FO39" t="n">
-        <v>288.72</v>
+        <v>785.8100000000001</v>
       </c>
       <c r="FP39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ39" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="FR39" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="FS39" t="n">
         <v>30</v>
@@ -21561,13 +21537,13 @@
         <v>1.07775</v>
       </c>
       <c r="EX40" t="n">
-        <v>1.08555</v>
+        <v>1.08575</v>
       </c>
       <c r="EY40" t="n">
-        <v>1.08355</v>
+        <v>1.08375</v>
       </c>
       <c r="EZ40" t="n">
-        <v>1.08125</v>
+        <v>1.08225</v>
       </c>
       <c r="FA40" t="n">
         <v>1</v>
@@ -21579,11 +21555,11 @@
         <v>1</v>
       </c>
       <c r="FD40" s="2" t="n">
-        <v>45502.70833333334</v>
+        <v>45502.625</v>
       </c>
       <c r="FE40" t="inlineStr"/>
       <c r="FF40" s="2" t="n">
-        <v>45497.66390046296</v>
+        <v>45497.66524305556</v>
       </c>
       <c r="FG40" s="2" t="n">
         <v>45495.66666666666</v>
@@ -21614,7 +21590,7 @@
         <v>-83.73999999999999</v>
       </c>
       <c r="FO40" t="n">
-        <v>204.98</v>
+        <v>702.0700000000001</v>
       </c>
       <c r="FP40" t="b">
         <v>0</v>
@@ -21623,7 +21599,7 @@
         <v>0</v>
       </c>
       <c r="FR40" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="FS40" t="n">
         <v>30</v>
@@ -22083,13 +22059,13 @@
         <v>1.07888</v>
       </c>
       <c r="EX41" t="n">
-        <v>1.08668</v>
+        <v>1.08488</v>
       </c>
       <c r="EY41" t="n">
-        <v>1.08468</v>
+        <v>1.08288</v>
       </c>
       <c r="EZ41" t="n">
-        <v>1.08238</v>
+        <v>1.08038</v>
       </c>
       <c r="FA41" t="n">
         <v>1</v>
@@ -22101,11 +22077,11 @@
         <v>1</v>
       </c>
       <c r="FD41" s="2" t="n">
-        <v>45502.625</v>
+        <v>45503.66666666666</v>
       </c>
       <c r="FE41" t="inlineStr"/>
       <c r="FF41" s="2" t="n">
-        <v>45498.83989583333</v>
+        <v>45497.63539351852</v>
       </c>
       <c r="FG41" s="2" t="n">
         <v>45495.91666666666</v>
@@ -22136,7 +22112,7 @@
         <v>-24.6</v>
       </c>
       <c r="FO41" t="n">
-        <v>180.38</v>
+        <v>677.47</v>
       </c>
       <c r="FP41" t="b">
         <v>0</v>
@@ -22145,7 +22121,7 @@
         <v>0</v>
       </c>
       <c r="FR41" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="FS41" t="n">
         <v>30</v>
@@ -22605,13 +22581,13 @@
         <v>1.07866</v>
       </c>
       <c r="EX42" t="n">
-        <v>1.08646</v>
+        <v>1.08666</v>
       </c>
       <c r="EY42" t="n">
-        <v>1.08446</v>
+        <v>1.08466</v>
       </c>
       <c r="EZ42" t="n">
-        <v>1.08216</v>
+        <v>1.08316</v>
       </c>
       <c r="FA42" t="n">
         <v>1</v>
@@ -22623,11 +22599,11 @@
         <v>1</v>
       </c>
       <c r="FD42" s="2" t="n">
-        <v>45502.625</v>
+        <v>45497.45833333334</v>
       </c>
       <c r="FE42" t="inlineStr"/>
       <c r="FF42" s="2" t="n">
-        <v>45497.719375</v>
+        <v>45496.59717592593</v>
       </c>
       <c r="FG42" s="2" t="n">
         <v>45495.95833333334</v>
@@ -22658,7 +22634,7 @@
         <v>-36.11</v>
       </c>
       <c r="FO42" t="n">
-        <v>144.27</v>
+        <v>641.36</v>
       </c>
       <c r="FP42" t="b">
         <v>0</v>
@@ -22667,7 +22643,7 @@
         <v>0</v>
       </c>
       <c r="FR42" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="FS42" t="n">
         <v>30</v>
@@ -23129,13 +23105,13 @@
         <v>1.07884</v>
       </c>
       <c r="EX43" t="n">
-        <v>1.08664</v>
+        <v>1.08484</v>
       </c>
       <c r="EY43" t="n">
-        <v>1.08464</v>
+        <v>1.08284</v>
       </c>
       <c r="EZ43" t="n">
-        <v>1.08234</v>
+        <v>1.08034</v>
       </c>
       <c r="FA43" t="n">
         <v>1</v>
@@ -23147,11 +23123,11 @@
         <v>1</v>
       </c>
       <c r="FD43" s="2" t="n">
-        <v>45502.625</v>
+        <v>45503.66666666666</v>
       </c>
       <c r="FE43" t="inlineStr"/>
       <c r="FF43" s="2" t="n">
-        <v>45498.83988425926</v>
+        <v>45497.62979166667</v>
       </c>
       <c r="FG43" s="2" t="n">
         <v>45496.125</v>
@@ -23182,7 +23158,7 @@
         <v>-26.69</v>
       </c>
       <c r="FO43" t="n">
-        <v>117.58</v>
+        <v>614.67</v>
       </c>
       <c r="FP43" t="b">
         <v>0</v>
@@ -23191,7 +23167,7 @@
         <v>0</v>
       </c>
       <c r="FR43" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="FS43" t="n">
         <v>30</v>
@@ -23653,13 +23629,13 @@
         <v>1.0788</v>
       </c>
       <c r="EX44" t="n">
-        <v>1.0866</v>
+        <v>1.0848</v>
       </c>
       <c r="EY44" t="n">
-        <v>1.0846</v>
+        <v>1.0828</v>
       </c>
       <c r="EZ44" t="n">
-        <v>1.0823</v>
+        <v>1.0803</v>
       </c>
       <c r="FA44" t="n">
         <v>1</v>
@@ -23671,11 +23647,11 @@
         <v>1</v>
       </c>
       <c r="FD44" s="2" t="n">
-        <v>45502.625</v>
+        <v>45503.66666666666</v>
       </c>
       <c r="FE44" t="inlineStr"/>
       <c r="FF44" s="2" t="n">
-        <v>45498.83983796297</v>
+        <v>45497.62109953703</v>
       </c>
       <c r="FG44" s="2" t="n">
         <v>45496.20833333334</v>
@@ -23706,7 +23682,7 @@
         <v>-28.78</v>
       </c>
       <c r="FO44" t="n">
-        <v>88.80000000000004</v>
+        <v>585.89</v>
       </c>
       <c r="FP44" t="b">
         <v>0</v>
@@ -23715,7 +23691,7 @@
         <v>0</v>
       </c>
       <c r="FR44" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="FS44" t="n">
         <v>30</v>
@@ -24180,10 +24156,10 @@
         <v>1.08436</v>
       </c>
       <c r="EY45" t="n">
-        <v>1.08956</v>
+        <v>1.09136</v>
       </c>
       <c r="EZ45" t="n">
-        <v>1.08986</v>
+        <v>1.09186</v>
       </c>
       <c r="FA45" t="n">
         <v>0</v>
@@ -24228,7 +24204,7 @@
         <v>-48.76</v>
       </c>
       <c r="FO45" t="n">
-        <v>40.04000000000004</v>
+        <v>537.13</v>
       </c>
       <c r="FP45" t="b">
         <v>0</v>
@@ -24237,7 +24213,7 @@
         <v>0</v>
       </c>
       <c r="FR45" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="FS45" t="n">
         <v>30</v>
@@ -24699,13 +24675,13 @@
         <v>1.07843</v>
       </c>
       <c r="EX46" t="n">
-        <v>1.08623</v>
+        <v>1.08443</v>
       </c>
       <c r="EY46" t="n">
-        <v>1.08423</v>
+        <v>1.08243</v>
       </c>
       <c r="EZ46" t="n">
-        <v>1.08193</v>
+        <v>1.07993</v>
       </c>
       <c r="FA46" t="n">
         <v>1</v>
@@ -24716,12 +24692,10 @@
       <c r="FC46" t="b">
         <v>1</v>
       </c>
-      <c r="FD46" s="2" t="n">
-        <v>45502.625</v>
-      </c>
+      <c r="FD46" t="inlineStr"/>
       <c r="FE46" t="inlineStr"/>
       <c r="FF46" s="2" t="n">
-        <v>45497.69756944444</v>
+        <v>45497.56241898148</v>
       </c>
       <c r="FG46" s="2" t="n">
         <v>45496.41666666666</v>
@@ -24730,10 +24704,10 @@
         <v>1.08843</v>
       </c>
       <c r="FI46" s="2" t="n">
-        <v>45497.69756944444</v>
+        <v>45497.56241898148</v>
       </c>
       <c r="FJ46" t="n">
-        <v>1.08619</v>
+        <v>1.08444</v>
       </c>
       <c r="FK46" t="inlineStr">
         <is>
@@ -24749,10 +24723,10 @@
         </is>
       </c>
       <c r="FN46" t="n">
-        <v>117.23</v>
+        <v>208.82</v>
       </c>
       <c r="FO46" t="n">
-        <v>157.27</v>
+        <v>745.95</v>
       </c>
       <c r="FP46" t="b">
         <v>1</v>
@@ -25221,13 +25195,13 @@
         <v>1.07756</v>
       </c>
       <c r="EX47" t="n">
-        <v>1.08536</v>
+        <v>1.08556</v>
       </c>
       <c r="EY47" t="n">
-        <v>1.08336</v>
+        <v>1.08356</v>
       </c>
       <c r="EZ47" t="n">
-        <v>1.08106</v>
+        <v>1.08206</v>
       </c>
       <c r="FA47" t="n">
         <v>1</v>
@@ -25239,11 +25213,11 @@
         <v>1</v>
       </c>
       <c r="FD47" s="2" t="n">
-        <v>45503.66666666666</v>
+        <v>45502.625</v>
       </c>
       <c r="FE47" t="inlineStr"/>
       <c r="FF47" s="2" t="n">
-        <v>45497.66150462963</v>
+        <v>45496.77591435185</v>
       </c>
       <c r="FG47" s="2" t="n">
         <v>45496.45833333334</v>
@@ -25252,10 +25226,10 @@
         <v>1.08756</v>
       </c>
       <c r="FI47" s="2" t="n">
-        <v>45497.66150462963</v>
+        <v>45496.77591435185</v>
       </c>
       <c r="FJ47" t="n">
-        <v>1.08537</v>
+        <v>1.08553</v>
       </c>
       <c r="FK47" t="inlineStr">
         <is>
@@ -25271,10 +25245,10 @@
         </is>
       </c>
       <c r="FN47" t="n">
-        <v>114.61</v>
+        <v>106.24</v>
       </c>
       <c r="FO47" t="n">
-        <v>271.8800000000001</v>
+        <v>852.1900000000001</v>
       </c>
       <c r="FP47" t="b">
         <v>1</v>
@@ -25743,13 +25717,13 @@
         <v>1.07609</v>
       </c>
       <c r="EX48" t="n">
-        <v>1.08589</v>
+        <v>1.08409</v>
       </c>
       <c r="EY48" t="n">
-        <v>1.08389</v>
+        <v>1.08209</v>
       </c>
       <c r="EZ48" t="n">
-        <v>1.08259</v>
+        <v>1.08059</v>
       </c>
       <c r="FA48" t="n">
         <v>1</v>
@@ -25761,11 +25735,11 @@
         <v>1</v>
       </c>
       <c r="FD48" s="2" t="n">
-        <v>45502.625</v>
+        <v>45503.66666666666</v>
       </c>
       <c r="FE48" t="inlineStr"/>
       <c r="FF48" s="2" t="n">
-        <v>45497.6725</v>
+        <v>45497.54267361111</v>
       </c>
       <c r="FG48" s="2" t="n">
         <v>45496.58333333334</v>
@@ -25774,10 +25748,10 @@
         <v>1.08609</v>
       </c>
       <c r="FI48" s="2" t="n">
-        <v>45497.6725</v>
+        <v>45497.54267361111</v>
       </c>
       <c r="FJ48" t="n">
-        <v>1.08589</v>
+        <v>1.0841</v>
       </c>
       <c r="FK48" t="inlineStr">
         <is>
@@ -25793,10 +25767,10 @@
         </is>
       </c>
       <c r="FN48" t="n">
-        <v>10.47</v>
+        <v>104.15</v>
       </c>
       <c r="FO48" t="n">
-        <v>282.3500000000001</v>
+        <v>956.34</v>
       </c>
       <c r="FP48" t="b">
         <v>1</v>
@@ -26265,13 +26239,13 @@
         <v>1.07566</v>
       </c>
       <c r="EX49" t="n">
-        <v>1.08546</v>
+        <v>1.08366</v>
       </c>
       <c r="EY49" t="n">
-        <v>1.08346</v>
+        <v>1.08166</v>
       </c>
       <c r="EZ49" t="n">
-        <v>1.08216</v>
+        <v>1.08016</v>
       </c>
       <c r="FA49" t="n">
         <v>1</v>
@@ -26283,11 +26257,11 @@
         <v>1</v>
       </c>
       <c r="FD49" s="2" t="n">
-        <v>45502.625</v>
+        <v>45503.66666666666</v>
       </c>
       <c r="FE49" t="inlineStr"/>
       <c r="FF49" s="2" t="n">
-        <v>45496.71552083334</v>
+        <v>45497.49517361111</v>
       </c>
       <c r="FG49" s="2" t="n">
         <v>45496.625</v>
@@ -26296,10 +26270,10 @@
         <v>1.08566</v>
       </c>
       <c r="FI49" s="2" t="n">
-        <v>45496.71552083334</v>
+        <v>45497.49517361111</v>
       </c>
       <c r="FJ49" t="n">
-        <v>1.08542</v>
+        <v>1.08366</v>
       </c>
       <c r="FK49" t="inlineStr">
         <is>
@@ -26315,10 +26289,10 @@
         </is>
       </c>
       <c r="FN49" t="n">
-        <v>12.56</v>
+        <v>104.67</v>
       </c>
       <c r="FO49" t="n">
-        <v>294.9100000000001</v>
+        <v>1061.01</v>
       </c>
       <c r="FP49" t="b">
         <v>1</v>
@@ -26789,13 +26763,13 @@
         <v>1.07423</v>
       </c>
       <c r="EX50" t="n">
-        <v>1.08403</v>
+        <v>1.08223</v>
       </c>
       <c r="EY50" t="n">
-        <v>1.08203</v>
+        <v>1.08023</v>
       </c>
       <c r="EZ50" t="n">
-        <v>1.08073</v>
+        <v>1.07873</v>
       </c>
       <c r="FA50" t="n">
         <v>1</v>
@@ -26806,12 +26780,10 @@
       <c r="FC50" t="b">
         <v>1</v>
       </c>
-      <c r="FD50" s="2" t="n">
-        <v>45503.66666666666</v>
-      </c>
+      <c r="FD50" t="inlineStr"/>
       <c r="FE50" t="inlineStr"/>
       <c r="FF50" s="2" t="n">
-        <v>45497.53380787037</v>
+        <v>45502.75628472222</v>
       </c>
       <c r="FG50" s="2" t="n">
         <v>45497.25</v>
@@ -26820,14 +26792,14 @@
         <v>1.08423</v>
       </c>
       <c r="FI50" s="2" t="n">
-        <v>45497.53380787037</v>
+        <v>45498.79166666666</v>
       </c>
       <c r="FJ50" t="n">
-        <v>1.08401</v>
+        <v>1.08593</v>
       </c>
       <c r="FK50" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL50" t="n">
@@ -26835,23 +26807,23 @@
       </c>
       <c r="FM50" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN50" t="n">
-        <v>11.51</v>
+        <v>-88.97</v>
       </c>
       <c r="FO50" t="n">
-        <v>306.4200000000001</v>
+        <v>972.04</v>
       </c>
       <c r="FP50" t="b">
+        <v>0</v>
+      </c>
+      <c r="FQ50" t="n">
+        <v>0</v>
+      </c>
+      <c r="FR50" t="n">
         <v>1</v>
-      </c>
-      <c r="FQ50" t="n">
-        <v>5</v>
-      </c>
-      <c r="FR50" t="n">
-        <v>0</v>
       </c>
       <c r="FS50" t="n">
         <v>30</v>
@@ -27311,13 +27283,13 @@
         <v>1.07426</v>
       </c>
       <c r="EX51" t="n">
-        <v>1.08406</v>
+        <v>1.08226</v>
       </c>
       <c r="EY51" t="n">
-        <v>1.08206</v>
+        <v>1.08026</v>
       </c>
       <c r="EZ51" t="n">
-        <v>1.08076</v>
+        <v>1.07876</v>
       </c>
       <c r="FA51" t="n">
         <v>1</v>
@@ -27328,12 +27300,10 @@
       <c r="FC51" t="b">
         <v>1</v>
       </c>
-      <c r="FD51" s="2" t="n">
-        <v>45503.66666666666</v>
-      </c>
+      <c r="FD51" t="inlineStr"/>
       <c r="FE51" t="inlineStr"/>
       <c r="FF51" s="2" t="n">
-        <v>45497.53383101852</v>
+        <v>45502.76416666667</v>
       </c>
       <c r="FG51" s="2" t="n">
         <v>45497.41666666666</v>
@@ -27342,14 +27312,14 @@
         <v>1.08426</v>
       </c>
       <c r="FI51" s="2" t="n">
-        <v>45497.53383101852</v>
+        <v>45498.79166666666</v>
       </c>
       <c r="FJ51" t="n">
-        <v>1.08406</v>
+        <v>1.08593</v>
       </c>
       <c r="FK51" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL51" t="n">
@@ -27357,23 +27327,23 @@
       </c>
       <c r="FM51" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN51" t="n">
-        <v>10.47</v>
+        <v>-87.40000000000001</v>
       </c>
       <c r="FO51" t="n">
-        <v>316.8900000000001</v>
+        <v>884.64</v>
       </c>
       <c r="FP51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ51" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="FR51" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="FS51" t="n">
         <v>30</v>
@@ -27833,13 +27803,13 @@
         <v>1.07287</v>
       </c>
       <c r="EX52" t="n">
-        <v>1.08267</v>
+        <v>1.08087</v>
       </c>
       <c r="EY52" t="n">
-        <v>1.08067</v>
+        <v>1.07887</v>
       </c>
       <c r="EZ52" t="n">
-        <v>1.07937</v>
+        <v>1.07737</v>
       </c>
       <c r="FA52" t="n">
         <v>1</v>
@@ -27850,12 +27820,10 @@
       <c r="FC52" t="b">
         <v>1</v>
       </c>
-      <c r="FD52" s="2" t="n">
-        <v>45505.5</v>
-      </c>
+      <c r="FD52" t="inlineStr"/>
       <c r="FE52" t="inlineStr"/>
       <c r="FF52" s="2" t="n">
-        <v>45503.46453703703</v>
+        <v>45503.67709490741</v>
       </c>
       <c r="FG52" s="2" t="n">
         <v>45497.45833333334</v>
@@ -27886,7 +27854,7 @@
         <v>-160.15</v>
       </c>
       <c r="FO52" t="n">
-        <v>156.7400000000001</v>
+        <v>724.49</v>
       </c>
       <c r="FP52" t="b">
         <v>0</v>
@@ -27895,7 +27863,7 @@
         <v>0</v>
       </c>
       <c r="FR52" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="FS52" t="n">
         <v>30</v>
@@ -28357,13 +28325,13 @@
         <v>1.07369</v>
       </c>
       <c r="EX53" t="n">
-        <v>1.08349</v>
+        <v>1.08169</v>
       </c>
       <c r="EY53" t="n">
-        <v>1.08149</v>
+        <v>1.07969</v>
       </c>
       <c r="EZ53" t="n">
-        <v>1.08019</v>
+        <v>1.07819</v>
       </c>
       <c r="FA53" t="n">
         <v>1</v>
@@ -28375,11 +28343,11 @@
         <v>1</v>
       </c>
       <c r="FD53" s="2" t="n">
-        <v>45503.66666666666</v>
+        <v>45505.54166666666</v>
       </c>
       <c r="FE53" t="inlineStr"/>
       <c r="FF53" s="2" t="n">
-        <v>45502.52984953704</v>
+        <v>45502.75050925926</v>
       </c>
       <c r="FG53" s="2" t="n">
         <v>45497.91666666666</v>
@@ -28410,7 +28378,7 @@
         <v>-117.23</v>
       </c>
       <c r="FO53" t="n">
-        <v>39.51000000000009</v>
+        <v>607.26</v>
       </c>
       <c r="FP53" t="b">
         <v>0</v>
@@ -28419,7 +28387,7 @@
         <v>0</v>
       </c>
       <c r="FR53" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="FS53" t="n">
         <v>30</v>
@@ -28879,13 +28847,13 @@
         <v>1.07342</v>
       </c>
       <c r="EX54" t="n">
-        <v>1.08322</v>
+        <v>1.08142</v>
       </c>
       <c r="EY54" t="n">
-        <v>1.08122</v>
+        <v>1.07942</v>
       </c>
       <c r="EZ54" t="n">
-        <v>1.07992</v>
+        <v>1.07792</v>
       </c>
       <c r="FA54" t="n">
         <v>1</v>
@@ -28897,11 +28865,11 @@
         <v>1</v>
       </c>
       <c r="FD54" s="2" t="n">
-        <v>45505.5</v>
+        <v>45505.54166666666</v>
       </c>
       <c r="FE54" t="inlineStr"/>
       <c r="FF54" s="2" t="n">
-        <v>45503.48103009259</v>
+        <v>45503.6845949074</v>
       </c>
       <c r="FG54" s="2" t="n">
         <v>45498.41666666666</v>
@@ -28932,7 +28900,7 @@
         <v>-131.36</v>
       </c>
       <c r="FO54" t="n">
-        <v>-91.84999999999992</v>
+        <v>475.9</v>
       </c>
       <c r="FP54" t="b">
         <v>0</v>
@@ -28941,7 +28909,7 @@
         <v>0</v>
       </c>
       <c r="FR54" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="FS54" t="n">
         <v>30</v>
@@ -29401,13 +29369,13 @@
         <v>1.07385</v>
       </c>
       <c r="EX55" t="n">
-        <v>1.08365</v>
+        <v>1.08185</v>
       </c>
       <c r="EY55" t="n">
-        <v>1.08165</v>
+        <v>1.07985</v>
       </c>
       <c r="EZ55" t="n">
-        <v>1.08035</v>
+        <v>1.07835</v>
       </c>
       <c r="FA55" t="n">
         <v>1</v>
@@ -29419,11 +29387,11 @@
         <v>1</v>
       </c>
       <c r="FD55" s="2" t="n">
-        <v>45503.66666666666</v>
+        <v>45505.54166666666</v>
       </c>
       <c r="FE55" t="inlineStr"/>
       <c r="FF55" s="2" t="n">
-        <v>45502.53194444445</v>
+        <v>45502.75199074074</v>
       </c>
       <c r="FG55" s="2" t="n">
         <v>45498.70833333334</v>
@@ -29454,7 +29422,7 @@
         <v>-108.86</v>
       </c>
       <c r="FO55" t="n">
-        <v>-200.7099999999999</v>
+        <v>367.04</v>
       </c>
       <c r="FP55" t="b">
         <v>0</v>
@@ -29463,7 +29431,7 @@
         <v>0</v>
       </c>
       <c r="FR55" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="FS55" t="n">
         <v>30</v>
@@ -29923,13 +29891,13 @@
         <v>1.09593</v>
       </c>
       <c r="EX56" t="n">
-        <v>1.08613</v>
+        <v>1.08093</v>
       </c>
       <c r="EY56" t="n">
-        <v>1.08813</v>
+        <v>1.08793</v>
       </c>
       <c r="EZ56" t="n">
-        <v>1.08943</v>
+        <v>1.08843</v>
       </c>
       <c r="FA56" t="n">
         <v>0</v>
@@ -29938,14 +29906,14 @@
         <v>0.03</v>
       </c>
       <c r="FC56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FD56" s="2" t="n">
-        <v>45506.70833333334</v>
+        <v>45506.66666666666</v>
       </c>
       <c r="FE56" t="inlineStr"/>
       <c r="FF56" s="2" t="n">
-        <v>45499.71210648148</v>
+        <v>45502.72559027778</v>
       </c>
       <c r="FG56" s="2" t="n">
         <v>45498.79166666666</v>
@@ -29976,7 +29944,7 @@
         <v>-29.88</v>
       </c>
       <c r="FO56" t="n">
-        <v>-230.5899999999999</v>
+        <v>337.16</v>
       </c>
       <c r="FP56" t="b">
         <v>0</v>
@@ -29985,7 +29953,7 @@
         <v>0</v>
       </c>
       <c r="FR56" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="FS56" t="n">
         <v>30</v>
@@ -30447,13 +30415,13 @@
         <v>1.07537</v>
       </c>
       <c r="EX57" t="n">
-        <v>1.08517</v>
+        <v>1.08337</v>
       </c>
       <c r="EY57" t="n">
-        <v>1.08317</v>
+        <v>1.08137</v>
       </c>
       <c r="EZ57" t="n">
-        <v>1.08187</v>
+        <v>1.07987</v>
       </c>
       <c r="FA57" t="n">
         <v>1</v>
@@ -30465,11 +30433,11 @@
         <v>1</v>
       </c>
       <c r="FD57" s="2" t="n">
-        <v>45502.625</v>
+        <v>45505.5</v>
       </c>
       <c r="FE57" t="inlineStr"/>
       <c r="FF57" s="2" t="n">
-        <v>45498.93435185185</v>
+        <v>45503.48611111111</v>
       </c>
       <c r="FG57" s="2" t="n">
         <v>45498.875</v>
@@ -30478,14 +30446,14 @@
         <v>1.08537</v>
       </c>
       <c r="FI57" s="2" t="n">
-        <v>45498.93435185185</v>
+        <v>45499.20833333334</v>
       </c>
       <c r="FJ57" t="n">
-        <v>1.08516</v>
+        <v>1.08575</v>
       </c>
       <c r="FK57" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL57" t="n">
@@ -30493,23 +30461,23 @@
       </c>
       <c r="FM57" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN57" t="n">
-        <v>10.99</v>
+        <v>-19.89</v>
       </c>
       <c r="FO57" t="n">
-        <v>-219.5999999999999</v>
+        <v>317.27</v>
       </c>
       <c r="FP57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FR57" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="FS57" t="n">
         <v>30</v>
@@ -30971,13 +30939,13 @@
         <v>1.09574</v>
       </c>
       <c r="EX58" t="n">
-        <v>1.08594</v>
+        <v>1.08074</v>
       </c>
       <c r="EY58" t="n">
-        <v>1.08794</v>
+        <v>1.08774</v>
       </c>
       <c r="EZ58" t="n">
-        <v>1.08924</v>
+        <v>1.08824</v>
       </c>
       <c r="FA58" t="n">
         <v>0</v>
@@ -30986,14 +30954,14 @@
         <v>0.03</v>
       </c>
       <c r="FC58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FD58" s="2" t="n">
-        <v>45506.70833333334</v>
+        <v>45506.66666666666</v>
       </c>
       <c r="FE58" t="inlineStr"/>
       <c r="FF58" s="2" t="n">
-        <v>45499.72556712963</v>
+        <v>45502.72667824074</v>
       </c>
       <c r="FG58" s="2" t="n">
         <v>45499.20833333334</v>
@@ -31002,14 +30970,14 @@
         <v>1.08574</v>
       </c>
       <c r="FI58" s="2" t="n">
-        <v>45499.72556712963</v>
+        <v>45499.75</v>
       </c>
       <c r="FJ58" t="n">
-        <v>1.08593</v>
+        <v>1.08552</v>
       </c>
       <c r="FK58" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL58" t="n">
@@ -31017,23 +30985,23 @@
       </c>
       <c r="FM58" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN58" t="n">
-        <v>9.960000000000001</v>
+        <v>-11.53</v>
       </c>
       <c r="FO58" t="n">
-        <v>-209.6399999999999</v>
+        <v>305.74</v>
       </c>
       <c r="FP58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ58" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="FR58" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="FS58" t="n">
         <v>30</v>
@@ -31495,13 +31463,13 @@
         <v>1.09576</v>
       </c>
       <c r="EX59" t="n">
-        <v>1.08596</v>
+        <v>1.08076</v>
       </c>
       <c r="EY59" t="n">
-        <v>1.08796</v>
+        <v>1.08776</v>
       </c>
       <c r="EZ59" t="n">
-        <v>1.08926</v>
+        <v>1.08826</v>
       </c>
       <c r="FA59" t="n">
         <v>0</v>
@@ -31510,14 +31478,14 @@
         <v>0.03</v>
       </c>
       <c r="FC59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FD59" s="2" t="n">
-        <v>45506.70833333334</v>
+        <v>45506.66666666666</v>
       </c>
       <c r="FE59" t="inlineStr"/>
       <c r="FF59" s="2" t="n">
-        <v>45499.72549768518</v>
+        <v>45502.72664351852</v>
       </c>
       <c r="FG59" s="2" t="n">
         <v>45499.29166666666</v>
@@ -31526,14 +31494,14 @@
         <v>1.08576</v>
       </c>
       <c r="FI59" s="2" t="n">
-        <v>45499.72549768518</v>
+        <v>45499.75</v>
       </c>
       <c r="FJ59" t="n">
-        <v>1.08599</v>
+        <v>1.08552</v>
       </c>
       <c r="FK59" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL59" t="n">
@@ -31541,23 +31509,23 @@
       </c>
       <c r="FM59" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN59" t="n">
-        <v>12.06</v>
+        <v>-12.58</v>
       </c>
       <c r="FO59" t="n">
-        <v>-197.5799999999999</v>
+        <v>293.16</v>
       </c>
       <c r="FP59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ59" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="FR59" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="FS59" t="n">
         <v>30</v>
@@ -32017,13 +31985,13 @@
         <v>1.09556</v>
       </c>
       <c r="EX60" t="n">
-        <v>1.08576</v>
+        <v>1.08056</v>
       </c>
       <c r="EY60" t="n">
-        <v>1.08776</v>
+        <v>1.08756</v>
       </c>
       <c r="EZ60" t="n">
-        <v>1.08906</v>
+        <v>1.08806</v>
       </c>
       <c r="FA60" t="n">
         <v>0</v>
@@ -32032,14 +32000,14 @@
         <v>0.03</v>
       </c>
       <c r="FC60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FD60" s="2" t="n">
-        <v>45506.70833333334</v>
+        <v>45506.66666666666</v>
       </c>
       <c r="FE60" t="inlineStr"/>
       <c r="FF60" s="2" t="n">
-        <v>45499.72581018518</v>
+        <v>45502.73018518519</v>
       </c>
       <c r="FG60" s="2" t="n">
         <v>45499.58333333334</v>
@@ -32048,14 +32016,14 @@
         <v>1.08556</v>
       </c>
       <c r="FI60" s="2" t="n">
-        <v>45499.72581018518</v>
+        <v>45499.75</v>
       </c>
       <c r="FJ60" t="n">
-        <v>1.08576</v>
+        <v>1.08552</v>
       </c>
       <c r="FK60" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="FL60" t="n">
@@ -32063,23 +32031,23 @@
       </c>
       <c r="FM60" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="FN60" t="n">
-        <v>10.49</v>
+        <v>-2.1</v>
       </c>
       <c r="FO60" t="n">
-        <v>-187.0899999999999</v>
+        <v>291.06</v>
       </c>
       <c r="FP60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FQ60" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="FR60" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="FS60" t="n">
         <v>30</v>
@@ -32542,10 +32510,10 @@
         <v>1.08104</v>
       </c>
       <c r="EY61" t="n">
-        <v>1.08624</v>
+        <v>1.08804</v>
       </c>
       <c r="EZ61" t="n">
-        <v>1.08654</v>
+        <v>1.08854</v>
       </c>
       <c r="FA61" t="n">
         <v>0</v>
@@ -32592,7 +32560,7 @@
         <v>-27.26</v>
       </c>
       <c r="FO61" t="n">
-        <v>-214.3499999999999</v>
+        <v>263.8</v>
       </c>
       <c r="FP61" t="b">
         <v>0</v>
@@ -32601,7 +32569,7 @@
         <v>0</v>
       </c>
       <c r="FR61" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="FS61" t="n">
         <v>30</v>
@@ -33066,10 +33034,10 @@
         <v>1.08146</v>
       </c>
       <c r="EY62" t="n">
-        <v>1.08666</v>
+        <v>1.08846</v>
       </c>
       <c r="EZ62" t="n">
-        <v>1.08696</v>
+        <v>1.08896</v>
       </c>
       <c r="FA62" t="n">
         <v>0</v>
@@ -33116,7 +33084,7 @@
         <v>-49.28</v>
       </c>
       <c r="FO62" t="n">
-        <v>-263.6299999999999</v>
+        <v>214.52</v>
       </c>
       <c r="FP62" t="b">
         <v>0</v>
@@ -33125,7 +33093,7 @@
         <v>0</v>
       </c>
       <c r="FR62" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="FS62" t="n">
         <v>30</v>
@@ -33587,13 +33555,13 @@
         <v>1.07552</v>
       </c>
       <c r="EX63" t="n">
-        <v>1.08332</v>
+        <v>1.08352</v>
       </c>
       <c r="EY63" t="n">
-        <v>1.08132</v>
+        <v>1.08152</v>
       </c>
       <c r="EZ63" t="n">
-        <v>1.07902</v>
+        <v>1.08002</v>
       </c>
       <c r="FA63" t="n">
         <v>1</v>
@@ -33609,7 +33577,7 @@
       </c>
       <c r="FE63" t="inlineStr"/>
       <c r="FF63" s="2" t="n">
-        <v>45503.48373842592</v>
+        <v>45503.56547453703</v>
       </c>
       <c r="FG63" s="2" t="n">
         <v>45499.75</v>
@@ -33640,7 +33608,7 @@
         <v>-49.72</v>
       </c>
       <c r="FO63" t="n">
-        <v>-313.3499999999999</v>
+        <v>164.8</v>
       </c>
       <c r="FP63" t="b">
         <v>0</v>
@@ -33649,7 +33617,7 @@
         <v>0</v>
       </c>
       <c r="FR63" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="FS63" t="n">
         <v>30</v>
@@ -34114,10 +34082,10 @@
         <v>1.08146</v>
       </c>
       <c r="EY64" t="n">
-        <v>1.08666</v>
+        <v>1.08846</v>
       </c>
       <c r="EZ64" t="n">
-        <v>1.08696</v>
+        <v>1.08896</v>
       </c>
       <c r="FA64" t="n">
         <v>0</v>
@@ -34164,7 +34132,7 @@
         <v>-260.55</v>
       </c>
       <c r="FO64" t="n">
-        <v>-573.8999999999999</v>
+        <v>-95.75</v>
       </c>
       <c r="FP64" t="b">
         <v>0</v>
@@ -34173,7 +34141,7 @@
         <v>0</v>
       </c>
       <c r="FR64" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="FS64" t="n">
         <v>30</v>

</xml_diff>

<commit_message>
fixed bugsfinal update on backtest
</commit_message>
<xml_diff>
--- a/filtered_excel_df.xlsx
+++ b/filtered_excel_df.xlsx
@@ -1732,7 +1732,7 @@
         <v>0.01</v>
       </c>
       <c r="FM2" t="n">
-        <v>74.76000000000001</v>
+        <v>74.87</v>
       </c>
       <c r="FN2" t="inlineStr">
         <is>
@@ -1743,7 +1743,7 @@
         <v>0.4375</v>
       </c>
       <c r="FP2" t="n">
-        <v>774.76</v>
+        <v>774.87</v>
       </c>
       <c r="FQ2" t="b">
         <v>1</v>
@@ -2183,7 +2183,7 @@
         <v>0.01</v>
       </c>
       <c r="FM3" t="n">
-        <v>531.15</v>
+        <v>531.89</v>
       </c>
       <c r="FN3" t="inlineStr">
         <is>
@@ -2194,7 +2194,7 @@
         <v>1.460659722222222</v>
       </c>
       <c r="FP3" t="n">
-        <v>1305.91</v>
+        <v>1306.76</v>
       </c>
       <c r="FQ3" t="b">
         <v>1</v>
@@ -2690,7 +2690,7 @@
         <v>0.01</v>
       </c>
       <c r="FM4" t="n">
-        <v>-132.59</v>
+        <v>-132.79</v>
       </c>
       <c r="FN4" t="inlineStr">
         <is>
@@ -2701,7 +2701,7 @@
         <v>0.2708333333333333</v>
       </c>
       <c r="FP4" t="n">
-        <v>1173.32</v>
+        <v>1173.97</v>
       </c>
       <c r="FQ4" t="b">
         <v>0</v>
@@ -3201,7 +3201,7 @@
         <v>0.01</v>
       </c>
       <c r="FM5" t="n">
-        <v>302.24</v>
+        <v>302.68</v>
       </c>
       <c r="FN5" t="inlineStr">
         <is>
@@ -3212,7 +3212,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="FP5" t="n">
-        <v>1475.56</v>
+        <v>1476.65</v>
       </c>
       <c r="FQ5" t="b">
         <v>1</v>
@@ -3710,7 +3710,7 @@
         <v>0.01</v>
       </c>
       <c r="FM6" t="n">
-        <v>126.73</v>
+        <v>126.91</v>
       </c>
       <c r="FN6" t="inlineStr">
         <is>
@@ -3721,7 +3721,7 @@
         <v>0.46875</v>
       </c>
       <c r="FP6" t="n">
-        <v>1602.29</v>
+        <v>1603.56</v>
       </c>
       <c r="FQ6" t="b">
         <v>1</v>
@@ -4223,7 +4223,7 @@
         <v>0.01</v>
       </c>
       <c r="FM7" t="n">
-        <v>36.41</v>
+        <v>36.46</v>
       </c>
       <c r="FN7" t="inlineStr">
         <is>
@@ -4234,7 +4234,7 @@
         <v>0.125</v>
       </c>
       <c r="FP7" t="n">
-        <v>1638.7</v>
+        <v>1640.02</v>
       </c>
       <c r="FQ7" t="b">
         <v>1</v>
@@ -4732,7 +4732,7 @@
         <v>0.01</v>
       </c>
       <c r="FM8" t="n">
-        <v>16.79</v>
+        <v>16.82</v>
       </c>
       <c r="FN8" t="inlineStr">
         <is>
@@ -4743,7 +4743,7 @@
         <v>0.02083333333333333</v>
       </c>
       <c r="FP8" t="n">
-        <v>1655.49</v>
+        <v>1656.84</v>
       </c>
       <c r="FQ8" t="b">
         <v>1</v>
@@ -5245,7 +5245,7 @@
         <v>0.01</v>
       </c>
       <c r="FM9" t="n">
-        <v>-28.11</v>
+        <v>-28.15</v>
       </c>
       <c r="FN9" t="inlineStr">
         <is>
@@ -5256,7 +5256,7 @@
         <v>0.07291666666666667</v>
       </c>
       <c r="FP9" t="n">
-        <v>1627.38</v>
+        <v>1628.69</v>
       </c>
       <c r="FQ9" t="b">
         <v>0</v>
@@ -5752,7 +5752,7 @@
         <v>0.01</v>
       </c>
       <c r="FM10" t="n">
-        <v>83.59999999999999</v>
+        <v>83.72</v>
       </c>
       <c r="FN10" t="inlineStr">
         <is>
@@ -5763,7 +5763,7 @@
         <v>0.3541666666666667</v>
       </c>
       <c r="FP10" t="n">
-        <v>1710.98</v>
+        <v>1712.41</v>
       </c>
       <c r="FQ10" t="b">
         <v>1</v>
@@ -6269,7 +6269,7 @@
         <v>0.01</v>
       </c>
       <c r="FM11" t="n">
-        <v>542.09</v>
+        <v>542.87</v>
       </c>
       <c r="FN11" t="inlineStr">
         <is>
@@ -6280,7 +6280,7 @@
         <v>2.626863425925926</v>
       </c>
       <c r="FP11" t="n">
-        <v>2253.07</v>
+        <v>2255.28</v>
       </c>
       <c r="FQ11" t="b">
         <v>1</v>
@@ -6780,7 +6780,7 @@
         <v>0.01</v>
       </c>
       <c r="FM12" t="n">
-        <v>-524.51</v>
+        <v>-525.3200000000001</v>
       </c>
       <c r="FN12" t="inlineStr">
         <is>
@@ -6791,7 +6791,7 @@
         <v>0.1505787037037037</v>
       </c>
       <c r="FP12" t="n">
-        <v>1728.56</v>
+        <v>1729.96</v>
       </c>
       <c r="FQ12" t="b">
         <v>0</v>
@@ -7293,7 +7293,7 @@
         <v>0.01</v>
       </c>
       <c r="FM13" t="n">
-        <v>-337.65</v>
+        <v>-338.17</v>
       </c>
       <c r="FN13" t="inlineStr">
         <is>
@@ -7304,7 +7304,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="FP13" t="n">
-        <v>1390.91</v>
+        <v>1391.79</v>
       </c>
       <c r="FQ13" t="b">
         <v>0</v>
@@ -7806,7 +7806,7 @@
         <v>0.01</v>
       </c>
       <c r="FM14" t="n">
-        <v>-166.7</v>
+        <v>-166.96</v>
       </c>
       <c r="FN14" t="inlineStr">
         <is>
@@ -7817,7 +7817,7 @@
         <v>0.21875</v>
       </c>
       <c r="FP14" t="n">
-        <v>1224.21</v>
+        <v>1224.83</v>
       </c>
       <c r="FQ14" t="b">
         <v>0</v>
@@ -8321,7 +8321,7 @@
         <v>0.01</v>
       </c>
       <c r="FM15" t="n">
-        <v>288.63</v>
+        <v>289.05</v>
       </c>
       <c r="FN15" t="inlineStr">
         <is>
@@ -8332,7 +8332,7 @@
         <v>0.8125</v>
       </c>
       <c r="FP15" t="n">
-        <v>1512.84</v>
+        <v>1513.88</v>
       </c>
       <c r="FQ15" t="b">
         <v>1</v>
@@ -8834,7 +8834,7 @@
         <v>0.01</v>
       </c>
       <c r="FM16" t="n">
-        <v>16.44</v>
+        <v>16.46</v>
       </c>
       <c r="FN16" t="inlineStr">
         <is>
@@ -8845,7 +8845,7 @@
         <v>0.2916666666666667</v>
       </c>
       <c r="FP16" t="n">
-        <v>1529.28</v>
+        <v>1530.34</v>
       </c>
       <c r="FQ16" t="b">
         <v>1</v>
@@ -9347,7 +9347,7 @@
         <v>0.01</v>
       </c>
       <c r="FM17" t="n">
-        <v>-58.69</v>
+        <v>-58.78</v>
       </c>
       <c r="FN17" t="inlineStr">
         <is>
@@ -9358,7 +9358,7 @@
         <v>0.2395833333333333</v>
       </c>
       <c r="FP17" t="n">
-        <v>1470.59</v>
+        <v>1471.56</v>
       </c>
       <c r="FQ17" t="b">
         <v>0</v>
@@ -9860,7 +9860,7 @@
         <v>0.01</v>
       </c>
       <c r="FM18" t="n">
-        <v>-67.34999999999999</v>
+        <v>-67.45999999999999</v>
       </c>
       <c r="FN18" t="inlineStr">
         <is>
@@ -9871,7 +9871,7 @@
         <v>0.09375</v>
       </c>
       <c r="FP18" t="n">
-        <v>1403.24</v>
+        <v>1404.1</v>
       </c>
       <c r="FQ18" t="b">
         <v>0</v>
@@ -10373,7 +10373,7 @@
         <v>0.01</v>
       </c>
       <c r="FM19" t="n">
-        <v>-93.69</v>
+        <v>-93.84</v>
       </c>
       <c r="FN19" t="inlineStr">
         <is>
@@ -10384,7 +10384,7 @@
         <v>0.2083333333333333</v>
       </c>
       <c r="FP19" t="n">
-        <v>1309.55</v>
+        <v>1310.26</v>
       </c>
       <c r="FQ19" t="b">
         <v>0</v>
@@ -10888,7 +10888,7 @@
         <v>0.01</v>
       </c>
       <c r="FM20" t="n">
-        <v>182.94</v>
+        <v>183.2</v>
       </c>
       <c r="FN20" t="inlineStr">
         <is>
@@ -10899,7 +10899,7 @@
         <v>0.6458333333333334</v>
       </c>
       <c r="FP20" t="n">
-        <v>1492.49</v>
+        <v>1493.46</v>
       </c>
       <c r="FQ20" t="b">
         <v>1</v>
@@ -11403,7 +11403,7 @@
         <v>0.01</v>
       </c>
       <c r="FM21" t="n">
-        <v>3.53</v>
+        <v>3.54</v>
       </c>
       <c r="FN21" t="inlineStr">
         <is>
@@ -11414,7 +11414,7 @@
         <v>0.2604166666666667</v>
       </c>
       <c r="FP21" t="n">
-        <v>1496.02</v>
+        <v>1497</v>
       </c>
       <c r="FQ21" t="b">
         <v>1</v>
@@ -11914,7 +11914,7 @@
         <v>0.01</v>
       </c>
       <c r="FM22" t="n">
-        <v>-45.08</v>
+        <v>-45.15</v>
       </c>
       <c r="FN22" t="inlineStr">
         <is>
@@ -11925,7 +11925,7 @@
         <v>0.2291666666666667</v>
       </c>
       <c r="FP22" t="n">
-        <v>1450.94</v>
+        <v>1451.85</v>
       </c>
       <c r="FQ22" t="b">
         <v>0</v>
@@ -12433,7 +12433,7 @@
         <v>0.01</v>
       </c>
       <c r="FM23" t="n">
-        <v>530.4299999999999</v>
+        <v>531.2</v>
       </c>
       <c r="FN23" t="inlineStr">
         <is>
@@ -12444,7 +12444,7 @@
         <v>0.3751851851851852</v>
       </c>
       <c r="FP23" t="n">
-        <v>1981.37</v>
+        <v>1983.05</v>
       </c>
       <c r="FQ23" t="b">
         <v>1</v>
@@ -12946,7 +12946,7 @@
         <v>0.01</v>
       </c>
       <c r="FM24" t="n">
-        <v>282.8</v>
+        <v>283.21</v>
       </c>
       <c r="FN24" t="inlineStr">
         <is>
@@ -12957,7 +12957,7 @@
         <v>2.333333333333333</v>
       </c>
       <c r="FP24" t="n">
-        <v>2264.170000000001</v>
+        <v>2266.26</v>
       </c>
       <c r="FQ24" t="b">
         <v>1</v>
@@ -13463,7 +13463,7 @@
         <v>0.01</v>
       </c>
       <c r="FM25" t="n">
-        <v>91.91</v>
+        <v>92.04000000000001</v>
       </c>
       <c r="FN25" t="inlineStr">
         <is>
@@ -13474,7 +13474,7 @@
         <v>0.125</v>
       </c>
       <c r="FP25" t="n">
-        <v>2356.08</v>
+        <v>2358.3</v>
       </c>
       <c r="FQ25" t="b">
         <v>1</v>
@@ -13980,7 +13980,7 @@
         <v>0.01</v>
       </c>
       <c r="FM26" t="n">
-        <v>8.66</v>
+        <v>8.67</v>
       </c>
       <c r="FN26" t="inlineStr">
         <is>
@@ -13991,7 +13991,7 @@
         <v>0.1145833333333333</v>
       </c>
       <c r="FP26" t="n">
-        <v>2364.74</v>
+        <v>2366.97</v>
       </c>
       <c r="FQ26" t="b">
         <v>1</v>
@@ -14497,7 +14497,7 @@
         <v>0.01</v>
       </c>
       <c r="FM27" t="n">
-        <v>-57.1</v>
+        <v>-57.19</v>
       </c>
       <c r="FN27" t="inlineStr">
         <is>
@@ -14508,7 +14508,7 @@
         <v>0.01041666666666667</v>
       </c>
       <c r="FP27" t="n">
-        <v>2307.64</v>
+        <v>2309.78</v>
       </c>
       <c r="FQ27" t="b">
         <v>0</v>
@@ -15014,7 +15014,7 @@
         <v>0.01</v>
       </c>
       <c r="FM28" t="n">
-        <v>-36.06</v>
+        <v>-36.12</v>
       </c>
       <c r="FN28" t="inlineStr">
         <is>
@@ -15025,7 +15025,7 @@
         <v>0.2395833333333333</v>
       </c>
       <c r="FP28" t="n">
-        <v>2271.58</v>
+        <v>2273.66</v>
       </c>
       <c r="FQ28" t="b">
         <v>0</v>
@@ -15533,7 +15533,7 @@
         <v>0.01</v>
       </c>
       <c r="FM29" t="n">
-        <v>-508.07</v>
+        <v>-508.87</v>
       </c>
       <c r="FN29" t="inlineStr">
         <is>
@@ -15544,7 +15544,7 @@
         <v>0.05802083333333333</v>
       </c>
       <c r="FP29" t="n">
-        <v>1763.51</v>
+        <v>1764.79</v>
       </c>
       <c r="FQ29" t="b">
         <v>0</v>
@@ -16052,7 +16052,7 @@
         <v>0.01</v>
       </c>
       <c r="FM30" t="n">
-        <v>-530.6900000000001</v>
+        <v>-531.54</v>
       </c>
       <c r="FN30" t="inlineStr">
         <is>
@@ -16063,7 +16063,7 @@
         <v>0.1334606481481481</v>
       </c>
       <c r="FP30" t="n">
-        <v>1232.82</v>
+        <v>1233.25</v>
       </c>
       <c r="FQ30" t="b">
         <v>0</v>
@@ -16569,7 +16569,7 @@
         <v>0.01</v>
       </c>
       <c r="FM31" t="n">
-        <v>109.23</v>
+        <v>109.39</v>
       </c>
       <c r="FN31" t="inlineStr">
         <is>
@@ -16580,7 +16580,7 @@
         <v>0.5625</v>
       </c>
       <c r="FP31" t="n">
-        <v>1342.05</v>
+        <v>1342.64</v>
       </c>
       <c r="FQ31" t="b">
         <v>1</v>
@@ -17088,7 +17088,7 @@
         <v>0.01</v>
       </c>
       <c r="FM32" t="n">
-        <v>-110.15</v>
+        <v>-110.31</v>
       </c>
       <c r="FN32" t="inlineStr">
         <is>
@@ -17099,7 +17099,7 @@
         <v>0.2604166666666667</v>
       </c>
       <c r="FP32" t="n">
-        <v>1231.9</v>
+        <v>1232.33</v>
       </c>
       <c r="FQ32" t="b">
         <v>0</v>
@@ -17603,7 +17603,7 @@
         <v>0.01</v>
       </c>
       <c r="FM33" t="n">
-        <v>-211.1</v>
+        <v>-211.41</v>
       </c>
       <c r="FN33" t="inlineStr">
         <is>
@@ -17614,7 +17614,7 @@
         <v>0.04166666666666666</v>
       </c>
       <c r="FP33" t="n">
-        <v>1020.8</v>
+        <v>1020.92</v>
       </c>
       <c r="FQ33" t="b">
         <v>0</v>
@@ -18120,7 +18120,7 @@
         <v>0.01</v>
       </c>
       <c r="FM34" t="n">
-        <v>-288.71</v>
+        <v>-289.14</v>
       </c>
       <c r="FN34" t="inlineStr">
         <is>
@@ -18131,7 +18131,7 @@
         <v>0.02083333333333333</v>
       </c>
       <c r="FP34" t="n">
-        <v>732.0900000000004</v>
+        <v>731.7800000000002</v>
       </c>
       <c r="FQ34" t="b">
         <v>0</v>
@@ -18635,7 +18635,7 @@
         <v>0.01</v>
       </c>
       <c r="FM35" t="n">
-        <v>34.65</v>
+        <v>34.69</v>
       </c>
       <c r="FN35" t="inlineStr">
         <is>
@@ -18646,7 +18646,7 @@
         <v>0.34375</v>
       </c>
       <c r="FP35" t="n">
-        <v>766.7400000000004</v>
+        <v>766.4700000000003</v>
       </c>
       <c r="FQ35" t="b">
         <v>1</v>
@@ -19154,7 +19154,7 @@
         <v>0.01</v>
       </c>
       <c r="FM36" t="n">
-        <v>-144.26</v>
+        <v>-144.48</v>
       </c>
       <c r="FN36" t="inlineStr">
         <is>
@@ -19165,7 +19165,7 @@
         <v>0.40625</v>
       </c>
       <c r="FP36" t="n">
-        <v>622.4800000000004</v>
+        <v>621.9900000000002</v>
       </c>
       <c r="FQ36" t="b">
         <v>0</v>
@@ -19671,7 +19671,7 @@
         <v>0.01</v>
       </c>
       <c r="FM37" t="n">
-        <v>-227.71</v>
+        <v>-228.05</v>
       </c>
       <c r="FN37" t="inlineStr">
         <is>
@@ -19682,7 +19682,7 @@
         <v>0.3125</v>
       </c>
       <c r="FP37" t="n">
-        <v>394.7700000000003</v>
+        <v>393.9400000000002</v>
       </c>
       <c r="FQ37" t="b">
         <v>0</v>
@@ -20190,7 +20190,7 @@
         <v>0.01</v>
       </c>
       <c r="FM38" t="n">
-        <v>95.09999999999999</v>
+        <v>95.23</v>
       </c>
       <c r="FN38" t="inlineStr">
         <is>
@@ -20201,7 +20201,7 @@
         <v>0.4583333333333333</v>
       </c>
       <c r="FP38" t="n">
-        <v>489.8700000000003</v>
+        <v>489.1700000000002</v>
       </c>
       <c r="FQ38" t="b">
         <v>1</v>
@@ -20705,7 +20705,7 @@
         <v>0.01</v>
       </c>
       <c r="FM39" t="n">
-        <v>58.33</v>
+        <v>58.41</v>
       </c>
       <c r="FN39" t="inlineStr">
         <is>
@@ -20716,7 +20716,7 @@
         <v>0.71875</v>
       </c>
       <c r="FP39" t="n">
-        <v>548.2000000000004</v>
+        <v>547.5800000000003</v>
       </c>
       <c r="FQ39" t="b">
         <v>1</v>
@@ -21220,7 +21220,7 @@
         <v>0.01</v>
       </c>
       <c r="FM40" t="n">
-        <v>-316.81</v>
+        <v>-317.29</v>
       </c>
       <c r="FN40" t="inlineStr">
         <is>
@@ -21231,7 +21231,7 @@
         <v>0.1979166666666667</v>
       </c>
       <c r="FP40" t="n">
-        <v>231.3900000000004</v>
+        <v>230.2900000000002</v>
       </c>
       <c r="FQ40" t="b">
         <v>0</v>
@@ -21735,7 +21735,7 @@
         <v>0.01</v>
       </c>
       <c r="FM41" t="n">
-        <v>-216.04</v>
+        <v>-216.37</v>
       </c>
       <c r="FN41" t="inlineStr">
         <is>
@@ -21746,7 +21746,7 @@
         <v>0.1979166666666667</v>
       </c>
       <c r="FP41" t="n">
-        <v>15.35000000000039</v>
+        <v>13.92000000000024</v>
       </c>
       <c r="FQ41" t="b">
         <v>0</v>
@@ -22254,7 +22254,7 @@
         <v>0.01</v>
       </c>
       <c r="FM42" t="n">
-        <v>-135.42</v>
+        <v>-135.63</v>
       </c>
       <c r="FN42" t="inlineStr">
         <is>
@@ -22265,7 +22265,7 @@
         <v>0.3645833333333333</v>
       </c>
       <c r="FP42" t="n">
-        <v>-120.0699999999996</v>
+        <v>-121.7099999999998</v>
       </c>
       <c r="FQ42" t="b">
         <v>0</v>
@@ -22771,7 +22771,7 @@
         <v>0.01</v>
       </c>
       <c r="FM43" t="n">
-        <v>-148.15</v>
+        <v>-148.38</v>
       </c>
       <c r="FN43" t="inlineStr">
         <is>
@@ -22782,7 +22782,7 @@
         <v>2.302083333333333</v>
       </c>
       <c r="FP43" t="n">
-        <v>-268.2199999999996</v>
+        <v>-270.0899999999997</v>
       </c>
       <c r="FQ43" t="b">
         <v>0</v>
@@ -23286,7 +23286,7 @@
         <v>0.01</v>
       </c>
       <c r="FM44" t="n">
-        <v>862.22</v>
+        <v>863.47</v>
       </c>
       <c r="FN44" t="inlineStr">
         <is>
@@ -23297,7 +23297,7 @@
         <v>1.125</v>
       </c>
       <c r="FP44" t="n">
-        <v>594.0000000000005</v>
+        <v>593.3800000000003</v>
       </c>
       <c r="FQ44" t="b">
         <v>1</v>
@@ -23803,7 +23803,7 @@
         <v>0.01</v>
       </c>
       <c r="FM45" t="n">
-        <v>-500.67</v>
+        <v>-501.44</v>
       </c>
       <c r="FN45" t="inlineStr">
         <is>
@@ -23814,7 +23814,7 @@
         <v>0.02083333333333333</v>
       </c>
       <c r="FP45" t="n">
-        <v>93.33000000000044</v>
+        <v>91.94000000000034</v>
       </c>
       <c r="FQ45" t="b">
         <v>0</v>
@@ -24320,7 +24320,7 @@
         <v>0.01</v>
       </c>
       <c r="FM46" t="n">
-        <v>-208.44</v>
+        <v>-208.76</v>
       </c>
       <c r="FN46" t="inlineStr">
         <is>
@@ -24331,7 +24331,7 @@
         <v>0.5</v>
       </c>
       <c r="FP46" t="n">
-        <v>-115.1099999999996</v>
+        <v>-116.8199999999997</v>
       </c>
       <c r="FQ46" t="b">
         <v>0</v>
@@ -24839,7 +24839,7 @@
         <v>0.01</v>
       </c>
       <c r="FM47" t="n">
-        <v>82.55</v>
+        <v>82.67</v>
       </c>
       <c r="FN47" t="inlineStr">
         <is>
@@ -24850,7 +24850,7 @@
         <v>0.3854166666666667</v>
       </c>
       <c r="FP47" t="n">
-        <v>-32.55999999999956</v>
+        <v>-34.14999999999965</v>
       </c>
       <c r="FQ47" t="b">
         <v>1</v>
@@ -25358,7 +25358,7 @@
         <v>0.01</v>
       </c>
       <c r="FM48" t="n">
-        <v>-110.67</v>
+        <v>-110.84</v>
       </c>
       <c r="FN48" t="inlineStr">
         <is>
@@ -25369,7 +25369,7 @@
         <v>0.2083333333333333</v>
       </c>
       <c r="FP48" t="n">
-        <v>-143.2299999999996</v>
+        <v>-144.9899999999997</v>
       </c>
       <c r="FQ48" t="b">
         <v>0</v>
@@ -25875,7 +25875,7 @@
         <v>0.01</v>
       </c>
       <c r="FM49" t="n">
-        <v>-198.54</v>
+        <v>-198.84</v>
       </c>
       <c r="FN49" t="inlineStr">
         <is>
@@ -25886,7 +25886,7 @@
         <v>0.1979166666666667</v>
       </c>
       <c r="FP49" t="n">
-        <v>-341.7699999999995</v>
+        <v>-343.8299999999997</v>
       </c>
       <c r="FQ49" t="b">
         <v>0</v>
@@ -26392,7 +26392,7 @@
         <v>0.01</v>
       </c>
       <c r="FM50" t="n">
-        <v>-18.39</v>
+        <v>-18.41</v>
       </c>
       <c r="FN50" t="inlineStr">
         <is>
@@ -26403,7 +26403,7 @@
         <v>0.2291666666666667</v>
       </c>
       <c r="FP50" t="n">
-        <v>-360.1599999999995</v>
+        <v>-362.2399999999997</v>
       </c>
       <c r="FQ50" t="b">
         <v>0</v>
@@ -26909,7 +26909,7 @@
         <v>0.01</v>
       </c>
       <c r="FM51" t="n">
-        <v>31.46</v>
+        <v>31.51</v>
       </c>
       <c r="FN51" t="inlineStr">
         <is>
@@ -26920,7 +26920,7 @@
         <v>0.2291666666666667</v>
       </c>
       <c r="FP51" t="n">
-        <v>-328.6999999999995</v>
+        <v>-330.7299999999997</v>
       </c>
       <c r="FQ51" t="b">
         <v>1</v>
@@ -27439,7 +27439,7 @@
         <v>0.3020833333333333</v>
       </c>
       <c r="FP52" t="n">
-        <v>-333.8299999999995</v>
+        <v>-335.8599999999997</v>
       </c>
       <c r="FQ52" t="b">
         <v>0</v>
@@ -27943,7 +27943,7 @@
         <v>0.01</v>
       </c>
       <c r="FM53" t="n">
-        <v>-226.29</v>
+        <v>-226.63</v>
       </c>
       <c r="FN53" t="inlineStr">
         <is>
@@ -27954,7 +27954,7 @@
         <v>0.01041666666666667</v>
       </c>
       <c r="FP53" t="n">
-        <v>-560.1199999999995</v>
+        <v>-562.4899999999998</v>
       </c>
       <c r="FQ53" t="b">
         <v>0</v>
@@ -28460,7 +28460,7 @@
         <v>0.01</v>
       </c>
       <c r="FM54" t="n">
-        <v>-247.51</v>
+        <v>-247.88</v>
       </c>
       <c r="FN54" t="inlineStr">
         <is>
@@ -28471,7 +28471,7 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="FP54" t="n">
-        <v>-807.6299999999995</v>
+        <v>-810.3699999999998</v>
       </c>
       <c r="FQ54" t="b">
         <v>0</v>
@@ -28975,7 +28975,7 @@
         <v>0.01</v>
       </c>
       <c r="FM55" t="n">
-        <v>5.48</v>
+        <v>5.49</v>
       </c>
       <c r="FN55" t="inlineStr">
         <is>
@@ -28986,7 +28986,7 @@
         <v>0.2916666666666667</v>
       </c>
       <c r="FP55" t="n">
-        <v>-802.1499999999995</v>
+        <v>-804.8799999999998</v>
       </c>
       <c r="FQ55" t="b">
         <v>1</v>
@@ -29496,7 +29496,7 @@
         <v>0.01</v>
       </c>
       <c r="FM56" t="n">
-        <v>-351.64</v>
+        <v>-352.16</v>
       </c>
       <c r="FN56" t="inlineStr">
         <is>
@@ -29507,7 +29507,7 @@
         <v>0.02083333333333333</v>
       </c>
       <c r="FP56" t="n">
-        <v>-1153.79</v>
+        <v>-1157.04</v>
       </c>
       <c r="FQ56" t="b">
         <v>0</v>
@@ -30015,7 +30015,7 @@
         <v>0.01</v>
       </c>
       <c r="FM57" t="n">
-        <v>-210.38</v>
+        <v>-210.69</v>
       </c>
       <c r="FN57" t="inlineStr">
         <is>
@@ -30026,7 +30026,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="FP57" t="n">
-        <v>-1364.17</v>
+        <v>-1367.73</v>
       </c>
       <c r="FQ57" t="b">
         <v>0</v>
@@ -30534,7 +30534,7 @@
         <v>0.01</v>
       </c>
       <c r="FM58" t="n">
-        <v>-88.93000000000001</v>
+        <v>-89.06</v>
       </c>
       <c r="FN58" t="inlineStr">
         <is>
@@ -30545,7 +30545,7 @@
         <v>0.09375</v>
       </c>
       <c r="FP58" t="n">
-        <v>-1453.1</v>
+        <v>-1456.79</v>
       </c>
       <c r="FQ58" t="b">
         <v>0</v>
@@ -31053,7 +31053,7 @@
         <v>0.01</v>
       </c>
       <c r="FM59" t="n">
-        <v>129.21</v>
+        <v>129.39</v>
       </c>
       <c r="FN59" t="inlineStr">
         <is>
@@ -31064,7 +31064,7 @@
         <v>0.4583333333333333</v>
       </c>
       <c r="FP59" t="n">
-        <v>-1323.89</v>
+        <v>-1327.4</v>
       </c>
       <c r="FQ59" t="b">
         <v>1</v>
@@ -31572,7 +31572,7 @@
         <v>0.01</v>
       </c>
       <c r="FM60" t="n">
-        <v>38.89</v>
+        <v>38.94</v>
       </c>
       <c r="FN60" t="inlineStr">
         <is>
@@ -31583,7 +31583,7 @@
         <v>0.2604166666666667</v>
       </c>
       <c r="FP60" t="n">
-        <v>-1285</v>
+        <v>-1288.46</v>
       </c>
       <c r="FQ60" t="b">
         <v>1</v>
@@ -32089,7 +32089,7 @@
         <v>0.01</v>
       </c>
       <c r="FM61" t="n">
-        <v>-78.67</v>
+        <v>-78.79000000000001</v>
       </c>
       <c r="FN61" t="inlineStr">
         <is>
@@ -32100,7 +32100,7 @@
         <v>2.104166666666667</v>
       </c>
       <c r="FP61" t="n">
-        <v>-1363.67</v>
+        <v>-1367.25</v>
       </c>
       <c r="FQ61" t="b">
         <v>0</v>
@@ -32604,7 +32604,7 @@
         <v>0.01</v>
       </c>
       <c r="FM62" t="n">
-        <v>47.9</v>
+        <v>47.97</v>
       </c>
       <c r="FN62" t="inlineStr">
         <is>
@@ -32615,7 +32615,7 @@
         <v>0.3541666666666667</v>
       </c>
       <c r="FP62" t="n">
-        <v>-1315.77</v>
+        <v>-1319.28</v>
       </c>
       <c r="FQ62" t="b">
         <v>1</v>
@@ -33123,7 +33123,7 @@
         <v>0.01</v>
       </c>
       <c r="FM63" t="n">
-        <v>-23.87</v>
+        <v>-23.9</v>
       </c>
       <c r="FN63" t="inlineStr">
         <is>
@@ -33134,7 +33134,7 @@
         <v>0.2708333333333333</v>
       </c>
       <c r="FP63" t="n">
-        <v>-1339.639999999999</v>
+        <v>-1343.18</v>
       </c>
       <c r="FQ63" t="b">
         <v>0</v>
@@ -33640,7 +33640,7 @@
         <v>0.01</v>
       </c>
       <c r="FM64" t="n">
-        <v>-235.5</v>
+        <v>-235.84</v>
       </c>
       <c r="FN64" t="inlineStr">
         <is>
@@ -33651,7 +33651,7 @@
         <v>0.125</v>
       </c>
       <c r="FP64" t="n">
-        <v>-1575.139999999999</v>
+        <v>-1579.02</v>
       </c>
       <c r="FQ64" t="b">
         <v>0</v>
@@ -34157,7 +34157,7 @@
         <v>0.01</v>
       </c>
       <c r="FM65" t="n">
-        <v>-519.8</v>
+        <v>-520.55</v>
       </c>
       <c r="FN65" t="inlineStr">
         <is>
@@ -34168,7 +34168,7 @@
         <v>0.6498379629629629</v>
       </c>
       <c r="FP65" t="n">
-        <v>-2094.94</v>
+        <v>-2099.57</v>
       </c>
       <c r="FQ65" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
updated to fix potential error
</commit_message>
<xml_diff>
--- a/filtered_excel_df.xlsx
+++ b/filtered_excel_df.xlsx
@@ -1886,13 +1886,13 @@
         </is>
       </c>
       <c r="DW3" t="n">
-        <v>213.38</v>
+        <v>213.27</v>
       </c>
       <c r="DX3" s="4" t="n">
         <v>2.981701388888889</v>
       </c>
       <c r="DY3" t="n">
-        <v>913.38</v>
+        <v>913.27</v>
       </c>
       <c r="DZ3" t="b">
         <v>1</v>
@@ -2288,13 +2288,13 @@
         </is>
       </c>
       <c r="DW4" t="n">
-        <v>213.73</v>
+        <v>213.62</v>
       </c>
       <c r="DX4" s="4" t="n">
         <v>4.816400462962963</v>
       </c>
       <c r="DY4" t="n">
-        <v>1127.11</v>
+        <v>1126.89</v>
       </c>
       <c r="DZ4" t="b">
         <v>1</v>
@@ -2692,13 +2692,13 @@
         </is>
       </c>
       <c r="DW5" t="n">
-        <v>211.26</v>
+        <v>211.15</v>
       </c>
       <c r="DX5" s="4" t="n">
         <v>0.209537037037037</v>
       </c>
       <c r="DY5" t="n">
-        <v>1338.37</v>
+        <v>1338.04</v>
       </c>
       <c r="DZ5" t="b">
         <v>1</v>
@@ -3096,13 +3096,13 @@
         </is>
       </c>
       <c r="DW6" t="n">
-        <v>211.44</v>
+        <v>211.33</v>
       </c>
       <c r="DX6" s="4" t="n">
         <v>0.3541898148148148</v>
       </c>
       <c r="DY6" t="n">
-        <v>1549.81</v>
+        <v>1549.37</v>
       </c>
       <c r="DZ6" t="b">
         <v>1</v>
@@ -3498,13 +3498,13 @@
         </is>
       </c>
       <c r="DW7" t="n">
-        <v>213.03</v>
+        <v>212.91</v>
       </c>
       <c r="DX7" s="4" t="n">
         <v>2.146608796296296</v>
       </c>
       <c r="DY7" t="n">
-        <v>1762.84</v>
+        <v>1762.28</v>
       </c>
       <c r="DZ7" t="b">
         <v>1</v>
@@ -3900,13 +3900,13 @@
         </is>
       </c>
       <c r="DW8" t="n">
-        <v>213.2</v>
+        <v>213.09</v>
       </c>
       <c r="DX8" s="4" t="n">
         <v>0.3463078703703704</v>
       </c>
       <c r="DY8" t="n">
-        <v>1976.04</v>
+        <v>1975.37</v>
       </c>
       <c r="DZ8" t="b">
         <v>1</v>
@@ -4302,13 +4302,13 @@
         </is>
       </c>
       <c r="DW9" t="n">
-        <v>211.44</v>
+        <v>211.33</v>
       </c>
       <c r="DX9" s="4" t="n">
         <v>1.359097222222222</v>
       </c>
       <c r="DY9" t="n">
-        <v>2187.48</v>
+        <v>2186.7</v>
       </c>
       <c r="DZ9" t="b">
         <v>1</v>
@@ -4702,13 +4702,13 @@
         </is>
       </c>
       <c r="DW10" t="n">
-        <v>365.52</v>
+        <v>365.32</v>
       </c>
       <c r="DX10" s="4" t="n">
         <v>1.33962962962963</v>
       </c>
       <c r="DY10" t="n">
-        <v>2553</v>
+        <v>2552.02</v>
       </c>
       <c r="DZ10" t="b">
         <v>1</v>
@@ -5104,13 +5104,13 @@
         </is>
       </c>
       <c r="DW11" t="n">
-        <v>211.61</v>
+        <v>211.5</v>
       </c>
       <c r="DX11" s="4" t="n">
         <v>0.3543981481481481</v>
       </c>
       <c r="DY11" t="n">
-        <v>2764.61</v>
+        <v>2763.52</v>
       </c>
       <c r="DZ11" t="b">
         <v>1</v>
@@ -5500,13 +5500,13 @@
         </is>
       </c>
       <c r="DW12" t="n">
-        <v>-531.79</v>
+        <v>-531.51</v>
       </c>
       <c r="DX12" s="4" t="n">
         <v>1.439467592592593</v>
       </c>
       <c r="DY12" t="n">
-        <v>2232.82</v>
+        <v>2232.01</v>
       </c>
       <c r="DZ12" t="b">
         <v>0</v>
@@ -5896,13 +5896,13 @@
         </is>
       </c>
       <c r="DW13" t="n">
-        <v>-533.21</v>
+        <v>-532.92</v>
       </c>
       <c r="DX13" s="4" t="n">
         <v>7.884849537037037</v>
       </c>
       <c r="DY13" t="n">
-        <v>1699.61</v>
+        <v>1699.09</v>
       </c>
       <c r="DZ13" t="b">
         <v>0</v>
@@ -6296,13 +6296,13 @@
         </is>
       </c>
       <c r="DW14" t="n">
-        <v>216.91</v>
+        <v>216.79</v>
       </c>
       <c r="DX14" s="4" t="n">
         <v>0.7638888888888888</v>
       </c>
       <c r="DY14" t="n">
-        <v>1916.52</v>
+        <v>1915.88</v>
       </c>
       <c r="DZ14" t="b">
         <v>1</v>
@@ -6692,13 +6692,13 @@
         </is>
       </c>
       <c r="DW15" t="n">
-        <v>-528.4299999999999</v>
+        <v>-528.15</v>
       </c>
       <c r="DX15" s="4" t="n">
         <v>3.650717592592593</v>
       </c>
       <c r="DY15" t="n">
-        <v>1388.09</v>
+        <v>1387.73</v>
       </c>
       <c r="DZ15" t="b">
         <v>0</v>
@@ -7092,13 +7092,13 @@
         </is>
       </c>
       <c r="DW16" t="n">
-        <v>779.5700000000001</v>
+        <v>779.15</v>
       </c>
       <c r="DX16" s="4" t="n">
         <v>3.164212962962963</v>
       </c>
       <c r="DY16" t="n">
-        <v>2167.66</v>
+        <v>2166.88</v>
       </c>
       <c r="DZ16" t="b">
         <v>1</v>
@@ -7492,13 +7492,13 @@
         </is>
       </c>
       <c r="DW17" t="n">
-        <v>777.1</v>
+        <v>776.6900000000001</v>
       </c>
       <c r="DX17" s="4" t="n">
         <v>3.080706018518518</v>
       </c>
       <c r="DY17" t="n">
-        <v>2944.76</v>
+        <v>2943.57</v>
       </c>
       <c r="DZ17" t="b">
         <v>1</v>
@@ -7894,13 +7894,13 @@
         </is>
       </c>
       <c r="DW18" t="n">
-        <v>217.44</v>
+        <v>217.32</v>
       </c>
       <c r="DX18" s="4" t="n">
         <v>1.537280092592593</v>
       </c>
       <c r="DY18" t="n">
-        <v>3162.2</v>
+        <v>3160.89</v>
       </c>
       <c r="DZ18" t="b">
         <v>1</v>
@@ -8298,13 +8298,13 @@
         </is>
       </c>
       <c r="DW19" t="n">
-        <v>353.69</v>
+        <v>353.5</v>
       </c>
       <c r="DX19" s="4" t="n">
         <v>2.023298611111111</v>
       </c>
       <c r="DY19" t="n">
-        <v>3515.89</v>
+        <v>3514.39</v>
       </c>
       <c r="DZ19" t="b">
         <v>1</v>
@@ -8694,13 +8694,13 @@
         </is>
       </c>
       <c r="DW20" t="n">
-        <v>-527.9</v>
+        <v>-527.62</v>
       </c>
       <c r="DX20" s="4" t="n">
         <v>0.8544560185185185</v>
       </c>
       <c r="DY20" t="n">
-        <v>2987.99</v>
+        <v>2986.77</v>
       </c>
       <c r="DZ20" t="b">
         <v>0</v>
@@ -9094,13 +9094,13 @@
         </is>
       </c>
       <c r="DW21" t="n">
-        <v>918.64</v>
+        <v>918.16</v>
       </c>
       <c r="DX21" s="4" t="n">
         <v>3.609849537037037</v>
       </c>
       <c r="DY21" t="n">
-        <v>3906.63</v>
+        <v>3904.93</v>
       </c>
       <c r="DZ21" t="b">
         <v>1</v>
@@ -9494,13 +9494,13 @@
         </is>
       </c>
       <c r="DW22" t="n">
-        <v>213.56</v>
+        <v>213.44</v>
       </c>
       <c r="DX22" s="4" t="n">
         <v>3.07744212962963</v>
       </c>
       <c r="DY22" t="n">
-        <v>4120.190000000001</v>
+        <v>4118.37</v>
       </c>
       <c r="DZ22" t="b">
         <v>1</v>
@@ -9894,13 +9894,13 @@
         </is>
       </c>
       <c r="DW23" t="n">
-        <v>354.75</v>
+        <v>354.56</v>
       </c>
       <c r="DX23" s="4" t="n">
         <v>2.620844907407407</v>
       </c>
       <c r="DY23" t="n">
-        <v>4474.940000000001</v>
+        <v>4472.93</v>
       </c>
       <c r="DZ23" t="b">
         <v>1</v>
@@ -10296,13 +10296,13 @@
         </is>
       </c>
       <c r="DW24" t="n">
-        <v>-526.66</v>
+        <v>-526.39</v>
       </c>
       <c r="DX24" s="4" t="n">
         <v>4.780578703703704</v>
       </c>
       <c r="DY24" t="n">
-        <v>3948.280000000001</v>
+        <v>3946.54</v>
       </c>
       <c r="DZ24" t="b">
         <v>0</v>
@@ -10698,13 +10698,13 @@
         </is>
       </c>
       <c r="DW25" t="n">
-        <v>214.26</v>
+        <v>214.15</v>
       </c>
       <c r="DX25" s="4" t="n">
         <v>3.821481481481482</v>
       </c>
       <c r="DY25" t="n">
-        <v>4162.540000000001</v>
+        <v>4160.690000000001</v>
       </c>
       <c r="DZ25" t="b">
         <v>1</v>
@@ -11100,13 +11100,13 @@
         </is>
       </c>
       <c r="DW26" t="n">
-        <v>212.85</v>
+        <v>212.74</v>
       </c>
       <c r="DX26" s="4" t="n">
         <v>3.104861111111111</v>
       </c>
       <c r="DY26" t="n">
-        <v>4375.390000000001</v>
+        <v>4373.43</v>
       </c>
       <c r="DZ26" t="b">
         <v>1</v>
@@ -11502,13 +11502,13 @@
         </is>
       </c>
       <c r="DW27" t="n">
-        <v>214.79</v>
+        <v>214.68</v>
       </c>
       <c r="DX27" s="4" t="n">
         <v>1.045034722222222</v>
       </c>
       <c r="DY27" t="n">
-        <v>4590.180000000001</v>
+        <v>4588.110000000001</v>
       </c>
       <c r="DZ27" t="b">
         <v>1</v>
@@ -11904,13 +11904,13 @@
         </is>
       </c>
       <c r="DW28" t="n">
-        <v>497.36</v>
+        <v>497.09</v>
       </c>
       <c r="DX28" s="4" t="n">
         <v>1.781018518518519</v>
       </c>
       <c r="DY28" t="n">
-        <v>5087.540000000001</v>
+        <v>5085.200000000001</v>
       </c>
       <c r="DZ28" t="b">
         <v>1</v>
@@ -12300,7 +12300,7 @@
       </c>
       <c r="DX29" t="inlineStr"/>
       <c r="DY29" t="n">
-        <v>5087.540000000001</v>
+        <v>5085.200000000001</v>
       </c>
       <c r="DZ29" t="b">
         <v>0</v>
@@ -12694,13 +12694,13 @@
         </is>
       </c>
       <c r="DW30" t="n">
-        <v>214.79</v>
+        <v>214.68</v>
       </c>
       <c r="DX30" s="4" t="n">
         <v>2.126793981481482</v>
       </c>
       <c r="DY30" t="n">
-        <v>5302.330000000001</v>
+        <v>5299.880000000001</v>
       </c>
       <c r="DZ30" t="b">
         <v>1</v>
@@ -13094,13 +13094,13 @@
         </is>
       </c>
       <c r="DW31" t="n">
-        <v>211.79</v>
+        <v>211.68</v>
       </c>
       <c r="DX31" s="4" t="n">
         <v>3.169363425925926</v>
       </c>
       <c r="DY31" t="n">
-        <v>5514.120000000001</v>
+        <v>5511.560000000001</v>
       </c>
       <c r="DZ31" t="b">
         <v>1</v>
@@ -13496,13 +13496,13 @@
         </is>
       </c>
       <c r="DW32" t="n">
-        <v>212.85</v>
+        <v>212.74</v>
       </c>
       <c r="DX32" s="4" t="n">
         <v>2.063067129629629</v>
       </c>
       <c r="DY32" t="n">
-        <v>5726.970000000001</v>
+        <v>5724.300000000001</v>
       </c>
       <c r="DZ32" t="b">
         <v>1</v>
@@ -13896,13 +13896,13 @@
         </is>
       </c>
       <c r="DW33" t="n">
-        <v>500.53</v>
+        <v>500.27</v>
       </c>
       <c r="DX33" s="4" t="n">
         <v>1.892222222222222</v>
       </c>
       <c r="DY33" t="n">
-        <v>6227.500000000001</v>
+        <v>6224.570000000002</v>
       </c>
       <c r="DZ33" t="b">
         <v>1</v>
@@ -14292,13 +14292,13 @@
         </is>
       </c>
       <c r="DW34" t="n">
-        <v>-524.1900000000001</v>
+        <v>-523.91</v>
       </c>
       <c r="DX34" s="4" t="n">
         <v>5.905219907407408</v>
       </c>
       <c r="DY34" t="n">
-        <v>5703.310000000001</v>
+        <v>5700.660000000002</v>
       </c>
       <c r="DZ34" t="b">
         <v>0</v>
@@ -14694,13 +14694,13 @@
         </is>
       </c>
       <c r="DW35" t="n">
-        <v>494</v>
+        <v>493.74</v>
       </c>
       <c r="DX35" s="4" t="n">
         <v>3.846331018518518</v>
       </c>
       <c r="DY35" t="n">
-        <v>6197.310000000001</v>
+        <v>6194.400000000001</v>
       </c>
       <c r="DZ35" t="b">
         <v>1</v>
@@ -15096,13 +15096,13 @@
         </is>
       </c>
       <c r="DW36" t="n">
-        <v>212.85</v>
+        <v>212.74</v>
       </c>
       <c r="DX36" s="4" t="n">
         <v>0.2920949074074074</v>
       </c>
       <c r="DY36" t="n">
-        <v>6410.160000000002</v>
+        <v>6407.140000000001</v>
       </c>
       <c r="DZ36" t="b">
         <v>1</v>
@@ -15498,13 +15498,13 @@
         </is>
       </c>
       <c r="DW37" t="n">
-        <v>361.1</v>
+        <v>360.91</v>
       </c>
       <c r="DX37" s="4" t="n">
         <v>3.138564814814815</v>
       </c>
       <c r="DY37" t="n">
-        <v>6771.260000000002</v>
+        <v>6768.050000000001</v>
       </c>
       <c r="DZ37" t="b">
         <v>1</v>
@@ -15894,13 +15894,13 @@
         </is>
       </c>
       <c r="DW38" t="n">
-        <v>-527.55</v>
+        <v>-527.27</v>
       </c>
       <c r="DX38" s="4" t="n">
         <v>1.22099537037037</v>
       </c>
       <c r="DY38" t="n">
-        <v>6243.710000000002</v>
+        <v>6240.780000000001</v>
       </c>
       <c r="DZ38" t="b">
         <v>0</v>
@@ -16296,13 +16296,13 @@
         </is>
       </c>
       <c r="DW39" t="n">
-        <v>492.94</v>
+        <v>492.68</v>
       </c>
       <c r="DX39" s="4" t="n">
         <v>1.995300925925926</v>
       </c>
       <c r="DY39" t="n">
-        <v>6736.650000000001</v>
+        <v>6733.460000000001</v>
       </c>
       <c r="DZ39" t="b">
         <v>1</v>
@@ -16698,13 +16698,13 @@
         </is>
       </c>
       <c r="DW40" t="n">
-        <v>-530.55</v>
+        <v>-530.27</v>
       </c>
       <c r="DX40" s="4" t="n">
         <v>0.1813773148148148</v>
       </c>
       <c r="DY40" t="n">
-        <v>6206.100000000001</v>
+        <v>6203.190000000001</v>
       </c>
       <c r="DZ40" t="b">
         <v>0</v>
@@ -17094,13 +17094,13 @@
         </is>
       </c>
       <c r="DW41" t="n">
-        <v>-531.62</v>
+        <v>-531.34</v>
       </c>
       <c r="DX41" s="4" t="n">
         <v>4.38431712962963</v>
       </c>
       <c r="DY41" t="n">
-        <v>5674.480000000001</v>
+        <v>5671.85</v>
       </c>
       <c r="DZ41" t="b">
         <v>0</v>
@@ -17496,13 +17496,13 @@
         </is>
       </c>
       <c r="DW42" t="n">
-        <v>235.09</v>
+        <v>234.96</v>
       </c>
       <c r="DX42" s="4" t="n">
         <v>0.8333449074074074</v>
       </c>
       <c r="DY42" t="n">
-        <v>5909.570000000002</v>
+        <v>5906.81</v>
       </c>
       <c r="DZ42" t="b">
         <v>1</v>
@@ -17896,13 +17896,13 @@
         </is>
       </c>
       <c r="DW43" t="n">
-        <v>211.26</v>
+        <v>211.15</v>
       </c>
       <c r="DX43" s="4" t="n">
         <v>0.4417476851851852</v>
       </c>
       <c r="DY43" t="n">
-        <v>6120.830000000002</v>
+        <v>6117.96</v>
       </c>
       <c r="DZ43" t="b">
         <v>1</v>
@@ -18292,13 +18292,13 @@
         </is>
       </c>
       <c r="DW44" t="n">
-        <v>-530.55</v>
+        <v>-530.27</v>
       </c>
       <c r="DX44" s="4" t="n">
         <v>0.9300462962962963</v>
       </c>
       <c r="DY44" t="n">
-        <v>5590.280000000002</v>
+        <v>5587.690000000001</v>
       </c>
       <c r="DZ44" t="b">
         <v>0</v>
@@ -18692,13 +18692,13 @@
         </is>
       </c>
       <c r="DW45" t="n">
-        <v>495.59</v>
+        <v>495.33</v>
       </c>
       <c r="DX45" s="4" t="n">
         <v>1.016921296296296</v>
       </c>
       <c r="DY45" t="n">
-        <v>6085.870000000002</v>
+        <v>6083.02</v>
       </c>
       <c r="DZ45" t="b">
         <v>1</v>
@@ -19094,13 +19094,13 @@
         </is>
       </c>
       <c r="DW46" t="n">
-        <v>-529.14</v>
+        <v>-528.86</v>
       </c>
       <c r="DX46" s="4" t="n">
         <v>0.9243287037037037</v>
       </c>
       <c r="DY46" t="n">
-        <v>5556.730000000001</v>
+        <v>5554.160000000001</v>
       </c>
       <c r="DZ46" t="b">
         <v>0</v>
@@ -19494,13 +19494,13 @@
         </is>
       </c>
       <c r="DW47" t="n">
-        <v>200.67</v>
+        <v>200.57</v>
       </c>
       <c r="DX47" s="4" t="n">
         <v>0.878900462962963</v>
       </c>
       <c r="DY47" t="n">
-        <v>5757.400000000001</v>
+        <v>5754.73</v>
       </c>
       <c r="DZ47" t="b">
         <v>1</v>
@@ -19896,13 +19896,13 @@
         </is>
       </c>
       <c r="DW48" t="n">
-        <v>212.14</v>
+        <v>212.03</v>
       </c>
       <c r="DX48" s="4" t="n">
         <v>1.560590277777778</v>
       </c>
       <c r="DY48" t="n">
-        <v>5969.540000000002</v>
+        <v>5966.76</v>
       </c>
       <c r="DZ48" t="b">
         <v>1</v>
@@ -20298,13 +20298,13 @@
         </is>
       </c>
       <c r="DW49" t="n">
-        <v>212.67</v>
+        <v>212.56</v>
       </c>
       <c r="DX49" s="4" t="n">
         <v>3.739513888888889</v>
       </c>
       <c r="DY49" t="n">
-        <v>6182.210000000002</v>
+        <v>6179.320000000001</v>
       </c>
       <c r="DZ49" t="b">
         <v>1</v>
@@ -20700,13 +20700,13 @@
         </is>
       </c>
       <c r="DW50" t="n">
-        <v>213.91</v>
+        <v>213.8</v>
       </c>
       <c r="DX50" s="4" t="n">
         <v>3.787314814814815</v>
       </c>
       <c r="DY50" t="n">
-        <v>6396.120000000002</v>
+        <v>6393.120000000001</v>
       </c>
       <c r="DZ50" t="b">
         <v>1</v>
@@ -21096,13 +21096,13 @@
         </is>
       </c>
       <c r="DW51" t="n">
-        <v>-545.05</v>
+        <v>-544.76</v>
       </c>
       <c r="DX51" s="4" t="n">
         <v>2.781840277777778</v>
       </c>
       <c r="DY51" t="n">
-        <v>5851.070000000002</v>
+        <v>5848.360000000001</v>
       </c>
       <c r="DZ51" t="b">
         <v>0</v>
@@ -21492,13 +21492,13 @@
         </is>
       </c>
       <c r="DW52" t="n">
-        <v>-497.32</v>
+        <v>-497.06</v>
       </c>
       <c r="DX52" s="4" t="n">
         <v>1.964756944444444</v>
       </c>
       <c r="DY52" t="n">
-        <v>5353.750000000002</v>
+        <v>5351.3</v>
       </c>
       <c r="DZ52" t="b">
         <v>0</v>
@@ -21892,13 +21892,13 @@
         </is>
       </c>
       <c r="DW53" t="n">
-        <v>1064.07</v>
+        <v>1063.51</v>
       </c>
       <c r="DX53" s="4" t="n">
         <v>5.944155092592593</v>
       </c>
       <c r="DY53" t="n">
-        <v>6417.820000000002</v>
+        <v>6414.81</v>
       </c>
       <c r="DZ53" t="b">
         <v>1</v>
@@ -22294,13 +22294,13 @@
         </is>
       </c>
       <c r="DW54" t="n">
-        <v>498.77</v>
+        <v>498.5</v>
       </c>
       <c r="DX54" s="4" t="n">
         <v>3.357546296296296</v>
       </c>
       <c r="DY54" t="n">
-        <v>6916.590000000002</v>
+        <v>6913.31</v>
       </c>
       <c r="DZ54" t="b">
         <v>1</v>
@@ -22696,13 +22696,13 @@
         </is>
       </c>
       <c r="DW55" t="n">
-        <v>-528.4299999999999</v>
+        <v>-528.15</v>
       </c>
       <c r="DX55" s="4" t="n">
         <v>1.325497685185185</v>
       </c>
       <c r="DY55" t="n">
-        <v>6388.160000000002</v>
+        <v>6385.160000000001</v>
       </c>
       <c r="DZ55" t="b">
         <v>0</v>
@@ -23096,13 +23096,13 @@
         </is>
       </c>
       <c r="DW56" t="n">
-        <v>493.83</v>
+        <v>493.57</v>
       </c>
       <c r="DX56" s="4" t="n">
         <v>7.447986111111111</v>
       </c>
       <c r="DY56" t="n">
-        <v>6881.990000000002</v>
+        <v>6878.73</v>
       </c>
       <c r="DZ56" t="b">
         <v>1</v>
@@ -23498,13 +23498,13 @@
         </is>
       </c>
       <c r="DW57" t="n">
-        <v>212.67</v>
+        <v>212.56</v>
       </c>
       <c r="DX57" s="4" t="n">
         <v>6.860833333333333</v>
       </c>
       <c r="DY57" t="n">
-        <v>7094.660000000002</v>
+        <v>7091.290000000001</v>
       </c>
       <c r="DZ57" t="b">
         <v>1</v>
@@ -23894,13 +23894,13 @@
         </is>
       </c>
       <c r="DW58" t="n">
-        <v>-529.3200000000001</v>
+        <v>-529.04</v>
       </c>
       <c r="DX58" s="4" t="n">
         <v>0.9877893518518519</v>
       </c>
       <c r="DY58" t="n">
-        <v>6565.340000000002</v>
+        <v>6562.250000000001</v>
       </c>
       <c r="DZ58" t="b">
         <v>0</v>
@@ -24296,13 +24296,13 @@
         </is>
       </c>
       <c r="DW59" t="n">
-        <v>211.79</v>
+        <v>211.68</v>
       </c>
       <c r="DX59" s="4" t="n">
         <v>0.653912037037037</v>
       </c>
       <c r="DY59" t="n">
-        <v>6777.130000000002</v>
+        <v>6773.930000000001</v>
       </c>
       <c r="DZ59" t="b">
         <v>1</v>

</xml_diff>